<commit_message>
Updated Smart Deadbolt Gen1 tab
Closed some low priority issues, updated the status of the production
tester
</commit_message>
<xml_diff>
--- a/Project Tracking/SecuRemote Project Issues.xlsx
+++ b/Project Tracking/SecuRemote Project Issues.xlsx
@@ -4,16 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24105" windowHeight="9870"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24105" windowHeight="9870" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Smart Deadbolt" sheetId="2" r:id="rId1"/>
+    <sheet name="Smart Deadbolt Gen1" sheetId="2" r:id="rId1"/>
     <sheet name="Smart Deadbolt Gen2" sheetId="3" r:id="rId2"/>
     <sheet name="Keeler Lock" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'Keeler Lock'!$1:$3</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Smart Deadbolt'!$1:$3</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Smart Deadbolt Gen1'!$1:$3</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Smart Deadbolt Gen2'!$1:$3</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -230,9 +230,6 @@
     <t>Production test fixture</t>
   </si>
   <si>
-    <t>Probuck has one, it might have issues. India team to review tester before 1st production build. It was reviewed and deemed sufficient for small production quantities. Will be monitored for first build.</t>
-  </si>
-  <si>
     <t>Need Internal Plate Assy drawing</t>
   </si>
   <si>
@@ -282,9 +279,6 @@
   </si>
   <si>
     <t>PCBs have been updated, samples are out of date.</t>
-  </si>
-  <si>
-    <t>Has testing been done on new Rev? Probuck has not seen new circuit boards, only drawings. Delphian to order latest PCBAs and send them to Probuck when assembled.</t>
   </si>
   <si>
     <t>Motor gears bind up when using knob</t>
@@ -339,9 +333,6 @@
     <t>It only works on Android V4.3 or higher. This is correct in the User manual, but App Install says "V2.1 &amp; higher" in "Supported Platforms". Discuss with Ashok. Sent email to Bhikhu.</t>
   </si>
   <si>
-    <t>Invite User a little flaky on Android 4.4.2</t>
-  </si>
-  <si>
     <t>First time try I got an error message about "known issue with Android system". Second time it worked. Discuss with Ashok, add to bug report.</t>
   </si>
   <si>
@@ -354,9 +345,6 @@
     <t>Error message "Cannot connect to Smart Deadbolt".</t>
   </si>
   <si>
-    <t>This occurs on occasion. Discussed with Ashok, we may have to warn the customer of a work around (trun BT off then back on again).</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
@@ -388,6 +376,18 @@
   </si>
   <si>
     <t>Smart Deadbolt, Gen 2</t>
+  </si>
+  <si>
+    <t>New fixture being shipped to Probuck. Need George/Navy to confim.</t>
+  </si>
+  <si>
+    <t>EXT Board has design issue, jumper required.</t>
+  </si>
+  <si>
+    <t>Invite User a little flaky on Android 4.4.2 (LG phone)</t>
+  </si>
+  <si>
+    <t>This occurs on occasion. Discussed with Ashok, we may have to warn the customer of a work around (turn BT off then back on again). Check with new chip</t>
   </si>
 </sst>
 </file>
@@ -1157,8 +1157,8 @@
   </sheetPr>
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1199,7 +1199,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="56">
         <f ca="1">TODAY()</f>
-        <v>42192</v>
+        <v>42195</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -1342,7 +1342,7 @@
       <c r="H8" s="65"/>
       <c r="I8" s="63"/>
     </row>
-    <row r="9" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
         <v>58</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>64</v>
       </c>
       <c r="D9" s="61" t="s">
-        <v>65</v>
+        <v>114</v>
       </c>
       <c r="E9" s="62" t="s">
         <v>54</v>
@@ -1361,11 +1361,9 @@
       <c r="F9" s="63">
         <v>42062</v>
       </c>
-      <c r="G9" s="66">
-        <v>42100</v>
-      </c>
+      <c r="G9" s="66"/>
       <c r="H9" s="65">
-        <v>42121</v>
+        <v>42195</v>
       </c>
       <c r="I9" s="63"/>
     </row>
@@ -1410,7 +1408,7 @@
       </c>
       <c r="B13" s="67"/>
       <c r="C13" s="68" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D13" s="68"/>
       <c r="E13" s="67" t="s">
@@ -1433,10 +1431,10 @@
         <v>2</v>
       </c>
       <c r="C14" s="68" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="68" t="s">
         <v>67</v>
-      </c>
-      <c r="D14" s="68" t="s">
-        <v>68</v>
       </c>
       <c r="E14" s="67" t="s">
         <v>54</v>
@@ -1460,13 +1458,13 @@
         <v>1</v>
       </c>
       <c r="C15" s="68" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="68" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="68" t="s">
+      <c r="E15" s="67" t="s">
         <v>70</v>
-      </c>
-      <c r="E15" s="67" t="s">
-        <v>71</v>
       </c>
       <c r="F15" s="69">
         <v>41989</v>
@@ -1513,10 +1511,10 @@
         <v>2</v>
       </c>
       <c r="C18" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="34" t="s">
         <v>72</v>
-      </c>
-      <c r="D18" s="34" t="s">
-        <v>73</v>
       </c>
       <c r="E18" s="33" t="s">
         <v>54</v>
@@ -1538,10 +1536,10 @@
         <v>3</v>
       </c>
       <c r="C19" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="34" t="s">
         <v>74</v>
-      </c>
-      <c r="D19" s="34" t="s">
-        <v>75</v>
       </c>
       <c r="E19" s="33" t="s">
         <v>54</v>
@@ -1561,13 +1559,13 @@
         <v>4</v>
       </c>
       <c r="C20" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="D20" s="34" t="s">
+      <c r="E20" s="33" t="s">
         <v>77</v>
-      </c>
-      <c r="E20" s="33" t="s">
-        <v>78</v>
       </c>
       <c r="F20" s="35">
         <v>42102</v>
@@ -1584,13 +1582,13 @@
         <v>5</v>
       </c>
       <c r="C21" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="D21" s="34" t="s">
+      <c r="E21" s="33" t="s">
         <v>80</v>
-      </c>
-      <c r="E21" s="33" t="s">
-        <v>81</v>
       </c>
       <c r="F21" s="35">
         <v>42024</v>
@@ -1599,7 +1597,7 @@
       <c r="H21" s="22"/>
       <c r="I21" s="36"/>
     </row>
-    <row r="22" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A22" s="32" t="s">
         <v>58</v>
       </c>
@@ -1607,20 +1605,20 @@
         <v>9</v>
       </c>
       <c r="C22" s="34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D22" s="34" t="s">
-        <v>83</v>
+        <v>115</v>
       </c>
       <c r="E22" s="33" t="s">
-        <v>57</v>
+        <v>15</v>
       </c>
       <c r="F22" s="35">
         <v>41992</v>
       </c>
       <c r="G22" s="23"/>
       <c r="H22" s="22">
-        <v>42121</v>
+        <v>42195</v>
       </c>
       <c r="I22" s="36"/>
     </row>
@@ -1632,13 +1630,13 @@
         <v>10</v>
       </c>
       <c r="C23" s="34" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D23" s="34" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E23" s="33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F23" s="35">
         <v>42050</v>
@@ -1657,10 +1655,10 @@
         <v>5</v>
       </c>
       <c r="C24" s="68" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D24" s="68" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E24" s="67" t="s">
         <v>54</v>
@@ -1684,13 +1682,13 @@
         <v>3</v>
       </c>
       <c r="C25" s="68" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D25" s="68" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E25" s="67" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F25" s="69">
         <v>42061</v>
@@ -1711,13 +1709,13 @@
         <v>1</v>
       </c>
       <c r="C26" s="68" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D26" s="68" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E26" s="67" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F26" s="69">
         <v>41995</v>
@@ -1738,13 +1736,13 @@
         <v>6</v>
       </c>
       <c r="C27" s="68" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D27" s="68" t="s">
+        <v>69</v>
+      </c>
+      <c r="E27" s="67" t="s">
         <v>70</v>
-      </c>
-      <c r="E27" s="67" t="s">
-        <v>71</v>
       </c>
       <c r="F27" s="69">
         <v>41989</v>
@@ -1763,13 +1761,13 @@
         <v>7</v>
       </c>
       <c r="C28" s="68" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D28" s="68" t="s">
+        <v>69</v>
+      </c>
+      <c r="E28" s="67" t="s">
         <v>70</v>
-      </c>
-      <c r="E28" s="67" t="s">
-        <v>71</v>
       </c>
       <c r="F28" s="69">
         <v>41989</v>
@@ -1790,13 +1788,13 @@
         <v>8</v>
       </c>
       <c r="C29" s="68" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D29" s="68" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E29" s="67" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F29" s="69">
         <v>41989</v>
@@ -1815,13 +1813,13 @@
         <v>11</v>
       </c>
       <c r="C30" s="68" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D30" s="68" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E30" s="67" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F30" s="69">
         <v>42050</v>
@@ -1848,7 +1846,7 @@
       <c r="B32" s="14"/>
       <c r="C32" s="28"/>
       <c r="D32" s="28" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E32" s="29"/>
       <c r="F32" s="30"/>
@@ -1864,10 +1862,10 @@
         <v>1</v>
       </c>
       <c r="C33" s="34" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D33" s="34" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E33" s="33" t="s">
         <v>54</v>
@@ -1889,10 +1887,10 @@
         <v>2</v>
       </c>
       <c r="C34" s="34" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="D34" s="34" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E34" s="33" t="s">
         <v>54</v>
@@ -1914,10 +1912,10 @@
         <v>3</v>
       </c>
       <c r="C35" s="34" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D35" s="34" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E35" s="33" t="s">
         <v>54</v>
@@ -1941,10 +1939,10 @@
         <v>5</v>
       </c>
       <c r="C36" s="34" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D36" s="34" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="E36" s="33" t="s">
         <v>54</v>
@@ -1953,103 +1951,107 @@
         <v>42120</v>
       </c>
       <c r="G36" s="45"/>
-      <c r="H36" s="37"/>
+      <c r="H36" s="37">
+        <v>42195</v>
+      </c>
       <c r="I36" s="36"/>
     </row>
-    <row r="37" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" s="19" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="75" t="s">
+        <v>103</v>
+      </c>
+      <c r="B37" s="33">
+        <v>7</v>
+      </c>
+      <c r="C37" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="D37" s="34" t="s">
         <v>107</v>
-      </c>
-      <c r="B37" s="33">
-        <v>6</v>
-      </c>
-      <c r="C37" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="D37" s="34" t="s">
-        <v>109</v>
       </c>
       <c r="E37" s="33"/>
       <c r="F37" s="35">
+        <v>42040</v>
+      </c>
+      <c r="G37" s="35"/>
+      <c r="H37" s="37"/>
+      <c r="I37" s="36"/>
+    </row>
+    <row r="38" spans="1:9" s="19" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A38" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="B38" s="20">
+        <v>8</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="D38" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="E38" s="20"/>
+      <c r="F38" s="22">
+        <v>41989</v>
+      </c>
+      <c r="G38" s="22"/>
+      <c r="H38" s="24">
+        <v>42121</v>
+      </c>
+      <c r="I38" s="22"/>
+    </row>
+    <row r="39" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A39" s="74" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" s="67">
+        <v>4</v>
+      </c>
+      <c r="C39" s="68" t="s">
+        <v>110</v>
+      </c>
+      <c r="D39" s="68" t="s">
+        <v>111</v>
+      </c>
+      <c r="E39" s="67" t="s">
+        <v>54</v>
+      </c>
+      <c r="F39" s="69">
         <v>42024</v>
       </c>
-      <c r="G37" s="35"/>
-      <c r="H37" s="37">
+      <c r="G39" s="70">
+        <v>42097</v>
+      </c>
+      <c r="H39" s="71">
+        <v>42098</v>
+      </c>
+      <c r="I39" s="73">
         <v>42121</v>
       </c>
-      <c r="I37" s="36"/>
-    </row>
-    <row r="38" spans="1:9" s="19" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="75" t="s">
-        <v>107</v>
-      </c>
-      <c r="B38" s="33">
-        <v>7</v>
-      </c>
-      <c r="C38" s="34" t="s">
-        <v>110</v>
-      </c>
-      <c r="D38" s="34" t="s">
-        <v>111</v>
-      </c>
-      <c r="E38" s="33"/>
-      <c r="F38" s="35">
-        <v>42040</v>
-      </c>
-      <c r="G38" s="35"/>
-      <c r="H38" s="37"/>
-      <c r="I38" s="36"/>
-    </row>
-    <row r="39" spans="1:9" s="19" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A39" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="B39" s="20">
-        <v>8</v>
-      </c>
-      <c r="C39" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="D39" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="E39" s="20"/>
-      <c r="F39" s="22">
-        <v>41989</v>
-      </c>
-      <c r="G39" s="22"/>
-      <c r="H39" s="24">
-        <v>42121</v>
-      </c>
-      <c r="I39" s="22"/>
-    </row>
-    <row r="40" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A40" s="74" t="s">
-        <v>12</v>
+    </row>
+    <row r="40" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A40" s="72" t="s">
+        <v>103</v>
       </c>
       <c r="B40" s="67">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C40" s="68" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="D40" s="68" t="s">
-        <v>115</v>
-      </c>
-      <c r="E40" s="67" t="s">
-        <v>54</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="E40" s="67"/>
       <c r="F40" s="69">
         <v>42024</v>
       </c>
-      <c r="G40" s="70">
-        <v>42097</v>
-      </c>
+      <c r="G40" s="69"/>
       <c r="H40" s="71">
-        <v>42098</v>
+        <v>42121</v>
       </c>
       <c r="I40" s="73">
-        <v>42121</v>
+        <v>42195</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2113,7 +2115,7 @@
     </row>
     <row r="2" spans="1:9" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B2"/>
       <c r="C2" s="7"/>
@@ -2123,7 +2125,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="56">
         <f ca="1">TODAY()</f>
-        <v>42192</v>
+        <v>42195</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -2256,7 +2258,7 @@
       <c r="B12" s="14"/>
       <c r="C12" s="28"/>
       <c r="D12" s="28" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E12" s="29"/>
       <c r="F12" s="30"/>
@@ -2300,8 +2302,8 @@
   </sheetPr>
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2332,7 +2334,7 @@
     </row>
     <row r="2" spans="1:9" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B2"/>
       <c r="C2" s="7"/>
@@ -2342,7 +2344,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="54">
         <f ca="1">TODAY()</f>
-        <v>42192</v>
+        <v>42195</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added UDI & PDI issues
Major and blocking issues have been added
</commit_message>
<xml_diff>
--- a/Project Tracking/SecuRemote Project Issues.xlsx
+++ b/Project Tracking/SecuRemote Project Issues.xlsx
@@ -1,27 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SCiTeR\Github\SecuRemote\Project Tracking\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24105" windowHeight="9870" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24105" windowHeight="9870" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Smart Deadbolt Gen1" sheetId="2" r:id="rId1"/>
     <sheet name="Smart Deadbolt Gen2" sheetId="3" r:id="rId2"/>
     <sheet name="Keeler Lock" sheetId="1" r:id="rId3"/>
+    <sheet name="UDI" sheetId="4" r:id="rId4"/>
+    <sheet name="PDI" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'Keeler Lock'!$1:$3</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Smart Deadbolt Gen1'!$1:$3</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Smart Deadbolt Gen2'!$1:$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="143">
   <si>
     <t>Open Issues List</t>
   </si>
@@ -388,6 +395,81 @@
   </si>
   <si>
     <t>This occurs on occasion. Discussed with Ashok, we may have to warn the customer of a work around (turn BT off then back on again). Check with new chip/new app. 7/17- App has been updated for Android users. Doug to verify.</t>
+  </si>
+  <si>
+    <t>SecuRemote Portal w/ SecuRemote 2.0</t>
+  </si>
+  <si>
+    <t>Mantis Bug Id- 1953: After factory Reset, when device is pulled to other account, admin gets user unauthorized error.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mantis Bug Id- 1988: User Management and SR Device update functionality is not working properly </t>
+  </si>
+  <si>
+    <t>Mantis Bug Id- 1987: Sometime SR Device update functionality is not working</t>
+  </si>
+  <si>
+    <t>Mantis Bug Id- 1340: In RAS device more than 10 users should not allow to add in application</t>
+  </si>
+  <si>
+    <t>Mantis Bug Id- 1962: After Activated Rule for any user, Admin can't delete that user from SRP or SR Smart app</t>
+  </si>
+  <si>
+    <t>Mantis Bug Id- 1968: When Admin creates new rule with any "Time Zone" then rule will be created with "UTC" time always</t>
+  </si>
+  <si>
+    <t>Mantis Bug Id- 1970: When user tries to create rule with invalid date then message is not displayed</t>
+  </si>
+  <si>
+    <t>Mantis Bug Id- 1954: User can operate SR devices in "Remote Mode" when Bridge "Status" is disabled</t>
+  </si>
+  <si>
+    <t>Mantis Bug Id- 1930: Server is not giving any time out for request of OperationStatus API.</t>
+  </si>
+  <si>
+    <t>Mantis Bug Id- 1927: In "Dashboard" page there should be display "SR Device" Name instead of "User Device" Name</t>
+  </si>
+  <si>
+    <t>Mantis Bug Id- 1837: After got success message in Remote mode, again give same operation then app display "Remote Operation Fail"</t>
+  </si>
+  <si>
+    <t>Mantis Bug Id- 1353: Admin can operate device as an user but not having admin rights when we "Disable" device from SecuRemote portal and enable again</t>
+  </si>
+  <si>
+    <t>Mantis Bug Id- 1578: When "GeneralRequestFailure" message display then not allow to add device</t>
+  </si>
+  <si>
+    <t>Mantis Bug Id- 1894: DeregisterSRDevice API will not actually removed/deleted particular SR device from user's account.</t>
+  </si>
+  <si>
+    <t>Mantis Bug Id- 1665: "portal.securemote.com" doesn't give response when user enter wrong password first &amp; then enter correct password for login</t>
+  </si>
+  <si>
+    <t>Mantis Bug Id- 1348: In portal.securemote.com, "Manage" option is not displayed for "GDO" and "SR Bridge" - new portal</t>
+  </si>
+  <si>
+    <t>Mantis Bug Id- 1473: At "SecuRemote Portal" in "Audit Logs" section, 'Operation' field display wrong operations type for Keeler &amp; RAS device</t>
+  </si>
+  <si>
+    <t>Mantis Bug Id- 1574: When user switch bridge to another account then also its display old device which was added under bridge on old account</t>
+  </si>
+  <si>
+    <t>Mantis Bug Id- 1539: Sometimes in portal SR Device details not update properly</t>
+  </si>
+  <si>
+    <t>Mantis Bug Id- 1929: After pull SR Device in another account if user enter old account's invite code then it displays "UserDeviceAlreadyAssociated"</t>
+  </si>
+  <si>
+    <t>Mantis Bug Id- 1984: TCP link was breaking constantly between 4 &amp; 5 AM USA Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mantis Bug Id- 1440: In Remote Mode, We operate same device by three phone then it will response to one device &amp; other requests are not being served </t>
+  </si>
+  <si>
+    <t>Mantis Bug Id- 1681: If GDO gives two async event at same time then in that case server disconnect TCP link for connected SR Bridge and GDO</t>
+  </si>
+  <si>
+    <t>SecuRemote PDI w/ SecuRemote 2.0</t>
   </si>
 </sst>
 </file>
@@ -923,7 +1005,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -958,7 +1040,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1214,7 +1296,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="56">
         <f ca="1">TODAY()</f>
-        <v>42202</v>
+        <v>42213</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -2144,7 +2226,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="56">
         <f ca="1">TODAY()</f>
-        <v>42202</v>
+        <v>42213</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -2321,8 +2403,8 @@
   </sheetPr>
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection sqref="A1:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2363,7 +2445,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="54">
         <f ca="1">TODAY()</f>
-        <v>42202</v>
+        <v>42213</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -2890,4 +2972,633 @@
   <pageSetup scale="70" orientation="landscape" verticalDpi="360" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.42578125" customWidth="1"/>
+    <col min="3" max="3" width="42.42578125" customWidth="1"/>
+    <col min="4" max="4" width="54.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" customWidth="1"/>
+    <col min="7" max="8" width="10.140625" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="53"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="5"/>
+    </row>
+    <row r="2" spans="1:9" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="54">
+        <f ca="1">TODAY()</f>
+        <v>42213</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="13"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="16"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="18"/>
+    </row>
+    <row r="5" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="52"/>
+      <c r="B5" s="20">
+        <v>1</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" s="21"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="22"/>
+    </row>
+    <row r="6" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A6" s="52"/>
+      <c r="B6" s="20">
+        <v>2</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6" s="21"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="22"/>
+    </row>
+    <row r="7" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="52"/>
+      <c r="B7" s="20">
+        <v>3</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="D7" s="21"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="22"/>
+    </row>
+    <row r="8" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="52"/>
+      <c r="B8" s="20">
+        <v>4</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="D8" s="21"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="22"/>
+    </row>
+    <row r="9" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="52"/>
+      <c r="B9" s="20">
+        <v>5</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="D9" s="21"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="22"/>
+    </row>
+    <row r="10" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A10" s="52"/>
+      <c r="B10" s="20">
+        <v>6</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="D10" s="21"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="22"/>
+    </row>
+    <row r="11" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A11" s="52"/>
+      <c r="B11" s="20">
+        <v>7</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="D11" s="21"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="22"/>
+    </row>
+    <row r="12" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="52"/>
+      <c r="B12" s="20">
+        <v>8</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="D12" s="21"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="22"/>
+    </row>
+    <row r="13" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A13" s="52"/>
+      <c r="B13" s="20">
+        <v>9</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="D13" s="21"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="22"/>
+    </row>
+    <row r="14" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="52"/>
+      <c r="B14" s="20">
+        <v>10</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="D14" s="21"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="22"/>
+    </row>
+    <row r="15" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A15" s="52"/>
+      <c r="B15" s="20">
+        <v>11</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="D15" s="21"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="22"/>
+    </row>
+    <row r="16" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A16" s="52"/>
+      <c r="B16" s="20">
+        <v>12</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="D16" s="21"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="22"/>
+    </row>
+    <row r="17" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A17" s="52"/>
+      <c r="B17" s="20">
+        <v>13</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="D17" s="21"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="22"/>
+    </row>
+    <row r="18" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A18" s="52"/>
+      <c r="B18" s="20">
+        <v>14</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="D18" s="21"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="22"/>
+    </row>
+    <row r="19" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A19" s="52"/>
+      <c r="B19" s="20">
+        <v>15</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="D19" s="21"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="22"/>
+    </row>
+    <row r="20" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A20" s="52"/>
+      <c r="B20" s="20">
+        <v>16</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="D20" s="21"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="22"/>
+    </row>
+    <row r="21" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A21" s="52"/>
+      <c r="B21" s="20">
+        <v>17</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="D21" s="21"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="22"/>
+    </row>
+    <row r="22" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A22" s="52"/>
+      <c r="B22" s="20">
+        <v>18</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="D22" s="21"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="22"/>
+    </row>
+    <row r="23" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A23" s="52"/>
+      <c r="B23" s="20">
+        <v>19</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="D23" s="21"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="22"/>
+    </row>
+    <row r="24" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A24" s="52"/>
+      <c r="B24" s="20">
+        <v>20</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="D24" s="21"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="22"/>
+    </row>
+    <row r="25" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="52"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="22"/>
+    </row>
+    <row r="26" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="52"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="22"/>
+    </row>
+    <row r="27" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="52"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="22"/>
+    </row>
+    <row r="28" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="52"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="22"/>
+    </row>
+    <row r="29" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="52"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="22"/>
+    </row>
+    <row r="30" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="52"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="22"/>
+    </row>
+    <row r="31" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="52"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="22"/>
+    </row>
+    <row r="32" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="52"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="22"/>
+    </row>
+    <row r="33" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="52"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="22"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.42578125" customWidth="1"/>
+    <col min="3" max="3" width="42.42578125" customWidth="1"/>
+    <col min="4" max="4" width="54.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" customWidth="1"/>
+    <col min="7" max="8" width="10.140625" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="53"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="5"/>
+    </row>
+    <row r="2" spans="1:9" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="54">
+        <f ca="1">TODAY()</f>
+        <v>42213</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="13"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="16"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="18"/>
+    </row>
+    <row r="5" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="52"/>
+      <c r="B5" s="20">
+        <v>1</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="D5" s="21"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="22"/>
+    </row>
+    <row r="6" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" s="52"/>
+      <c r="B6" s="20">
+        <v>2</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="D6" s="21"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="22"/>
+    </row>
+    <row r="7" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="52"/>
+      <c r="B7" s="20">
+        <v>3</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="D7" s="21"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="22"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated progress and issues
The project is moving along on or ahead of schedule.
</commit_message>
<xml_diff>
--- a/Project Tracking/SecuRemote Project Issues.xlsx
+++ b/Project Tracking/SecuRemote Project Issues.xlsx
@@ -502,13 +502,13 @@
     <t>Garage Door Opener</t>
   </si>
   <si>
-    <t>GDO wires are too short. Need to be about 16 feet long.</t>
-  </si>
-  <si>
     <t>Sensor wires are fine, maybe too long.</t>
   </si>
   <si>
     <t>Installation portion of the Users Manual is hard to follow, text boxes are missing information.</t>
+  </si>
+  <si>
+    <t>GDO control wires are too short. Need to be about 16 feet long.</t>
   </si>
 </sst>
 </file>
@@ -1356,7 +1356,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="56">
         <f ca="1">TODAY()</f>
-        <v>42240</v>
+        <v>42243</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -2286,7 +2286,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="56">
         <f ca="1">TODAY()</f>
-        <v>42240</v>
+        <v>42243</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -2464,7 +2464,7 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2505,7 +2505,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="54">
         <f ca="1">TODAY()</f>
-        <v>42240</v>
+        <v>42243</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -3180,7 +3180,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -3221,7 +3221,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="56">
         <f ca="1">TODAY()</f>
-        <v>42240</v>
+        <v>42243</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -3322,7 +3322,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="20"/>
@@ -3365,10 +3365,10 @@
         <v>1</v>
       </c>
       <c r="C12" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="D12" s="34" t="s">
         <v>154</v>
-      </c>
-      <c r="D12" s="34" t="s">
-        <v>155</v>
       </c>
       <c r="E12" s="33"/>
       <c r="F12" s="35">
@@ -3473,7 +3473,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="54">
         <f ca="1">TODAY()</f>
-        <v>42240</v>
+        <v>42243</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -3964,7 +3964,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="54">
         <f ca="1">TODAY()</f>
-        <v>42240</v>
+        <v>42243</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updates to timing and issues list
Just minor updates for Friday's meeting.
</commit_message>
<xml_diff>
--- a/Project Tracking/SecuRemote Project Issues.xlsx
+++ b/Project Tracking/SecuRemote Project Issues.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="159">
   <si>
     <t>Open Issues List</t>
   </si>
@@ -133,9 +133,6 @@
     <t>Push Notifications</t>
   </si>
   <si>
-    <t>Rules for notifications needs to be defined</t>
-  </si>
-  <si>
     <t>Page layout / appearance</t>
   </si>
   <si>
@@ -456,9 +453,6 @@
   </si>
   <si>
     <t>Access Control Rules in development. 7/17- Web portal functions, but there's a bug in the AM/PM time settings. 8/3 - retested, appears to be working fine now.</t>
-  </si>
-  <si>
-    <t>Threads were wrong for collar, date code not stamped in.  Waiting for resubmission from supplier. 8/6 - still waiting.</t>
   </si>
   <si>
     <t>Creating part numbers and entering into JDE. 8/6 - will add more information, once parts are available.</t>
@@ -481,15 +475,9 @@
     </r>
   </si>
   <si>
-    <t>Still working through some issues. Should be ready for testing mid July. 3 GDO units sent on 7/16. 7/29 - Doug to install one unit and test.</t>
-  </si>
-  <si>
     <t>Mike to take a look. Possibly change main harness length and add sleeving, so harness can be routed behind battery housing. ECO-1139. Verify parts when available. 7/27 - order parts 8/13 - Parts on order (PO 122419), 100pcs</t>
   </si>
   <si>
-    <t>Verify in displays. Order several samples. 8/13- samples received. When batteries installed, housing is too thick. Found a better solution on Alibaba. Ashley to order samples.</t>
-  </si>
-  <si>
     <t>Order boards, build samples. 8/14 - PO 122419</t>
   </si>
   <si>
@@ -509,6 +497,24 @@
   </si>
   <si>
     <t>GDO control wires are too short. Need to be about 16 feet long.</t>
+  </si>
+  <si>
+    <t>Still working through some issues. Should be ready for testing mid July. 3 GDO units sent on 7/16. 7/29 - Doug to install one unit and test. 9/2 - Tested local and remote functionality. Now need to add more devices to operate through.</t>
+  </si>
+  <si>
+    <t>Verify in displays. Order several samples. 8/13- samples received. When batteries installed, housing is too thick. Found a better solution on Alibaba. Ashley to order samples. Parts from Stride don't work. More coming from Tysonic.</t>
+  </si>
+  <si>
+    <t>Threads were wrong for collar, date code not stamped in.  Waiting for resubmission from supplier. 8/6 - still waiting. 9/2 - threads still wrong for our rose nut sample.</t>
+  </si>
+  <si>
+    <t>Rules for notifications needs to be defined. 9/2 - Preliminary code in place.</t>
+  </si>
+  <si>
+    <t>App doesn't ask if user wants to operate the device remotely when out of Bluetooth range and BT is ON.</t>
+  </si>
+  <si>
+    <t>The app should first ask if user wants to operate remotely. User has to manually turn BT off before being asked to operate remotely.</t>
   </si>
 </sst>
 </file>
@@ -1346,7 +1352,7 @@
     </row>
     <row r="2" spans="1:9" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2"/>
       <c r="C2" s="7"/>
@@ -1356,7 +1362,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="56">
         <f ca="1">TODAY()</f>
-        <v>42243</v>
+        <v>42249</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -1393,7 +1399,7 @@
       <c r="B4" s="14"/>
       <c r="C4" s="15"/>
       <c r="D4" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4" s="16"/>
       <c r="F4" s="17"/>
@@ -1409,13 +1415,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="E5" s="20" t="s">
         <v>41</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>42</v>
       </c>
       <c r="F5" s="22">
         <v>42048</v>
@@ -1434,13 +1440,13 @@
         <v>2</v>
       </c>
       <c r="C6" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="E6" s="20" t="s">
         <v>44</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>45</v>
       </c>
       <c r="F6" s="22">
         <v>42047</v>
@@ -1453,19 +1459,19 @@
     </row>
     <row r="7" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" s="20">
         <v>3</v>
       </c>
       <c r="C7" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="21" t="s">
-        <v>48</v>
-      </c>
       <c r="E7" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F7" s="22">
         <v>42048</v>
@@ -1478,19 +1484,19 @@
     </row>
     <row r="8" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" s="20">
         <v>4</v>
       </c>
       <c r="C8" s="61" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="61" t="s">
+      <c r="E8" s="62" t="s">
         <v>50</v>
-      </c>
-      <c r="E8" s="62" t="s">
-        <v>51</v>
       </c>
       <c r="F8" s="63">
         <v>42048</v>
@@ -1501,19 +1507,19 @@
     </row>
     <row r="9" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="71" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="66">
         <v>5</v>
       </c>
       <c r="C9" s="80" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D9" s="80" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E9" s="81" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F9" s="72">
         <v>42062</v>
@@ -1563,15 +1569,15 @@
     </row>
     <row r="13" spans="1:9" s="19" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="66" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" s="66"/>
       <c r="C13" s="67" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D13" s="67"/>
       <c r="E13" s="66" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F13" s="68">
         <v>41992</v>
@@ -1584,19 +1590,19 @@
     </row>
     <row r="14" spans="1:9" s="19" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="66" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" s="66">
         <v>2</v>
       </c>
       <c r="C14" s="67" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="67" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="67" t="s">
-        <v>55</v>
-      </c>
       <c r="E14" s="66" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F14" s="68">
         <v>41992</v>
@@ -1611,19 +1617,19 @@
     </row>
     <row r="15" spans="1:9" s="19" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="66" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B15" s="66">
         <v>1</v>
       </c>
       <c r="C15" s="67" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="67" t="s">
+      <c r="E15" s="66" t="s">
         <v>57</v>
-      </c>
-      <c r="E15" s="66" t="s">
-        <v>58</v>
       </c>
       <c r="F15" s="68">
         <v>41989</v>
@@ -1670,13 +1676,13 @@
         <v>2</v>
       </c>
       <c r="C18" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="34" t="s">
-        <v>60</v>
-      </c>
       <c r="E18" s="33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F18" s="35">
         <v>42093</v>
@@ -1695,13 +1701,13 @@
         <v>3</v>
       </c>
       <c r="C19" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="D19" s="34" t="s">
-        <v>62</v>
-      </c>
       <c r="E19" s="33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F19" s="35">
         <v>42102</v>
@@ -1718,13 +1724,13 @@
         <v>4</v>
       </c>
       <c r="C20" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="D20" s="34" t="s">
+      <c r="E20" s="33" t="s">
         <v>64</v>
-      </c>
-      <c r="E20" s="33" t="s">
-        <v>65</v>
       </c>
       <c r="F20" s="35">
         <v>42102</v>
@@ -1735,19 +1741,19 @@
     </row>
     <row r="21" spans="1:9" s="19" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B21" s="33">
         <v>5</v>
       </c>
       <c r="C21" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="D21" s="34" t="s">
+      <c r="E21" s="33" t="s">
         <v>67</v>
-      </c>
-      <c r="E21" s="33" t="s">
-        <v>68</v>
       </c>
       <c r="F21" s="35">
         <v>42024</v>
@@ -1758,16 +1764,16 @@
     </row>
     <row r="22" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A22" s="32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B22" s="33">
         <v>9</v>
       </c>
       <c r="C22" s="34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D22" s="34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E22" s="33" t="s">
         <v>15</v>
@@ -1783,19 +1789,19 @@
     </row>
     <row r="23" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A23" s="32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B23" s="33">
         <v>10</v>
       </c>
       <c r="C23" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="D23" s="34" t="s">
-        <v>71</v>
-      </c>
       <c r="E23" s="33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F23" s="35">
         <v>42050</v>
@@ -1808,19 +1814,19 @@
     </row>
     <row r="24" spans="1:9" s="19" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="71" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B24" s="66">
         <v>5</v>
       </c>
       <c r="C24" s="67" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="67" t="s">
         <v>72</v>
       </c>
-      <c r="D24" s="67" t="s">
-        <v>73</v>
-      </c>
       <c r="E24" s="66" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F24" s="68">
         <v>42000</v>
@@ -1835,19 +1841,19 @@
     </row>
     <row r="25" spans="1:9" s="19" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="71" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B25" s="66">
         <v>3</v>
       </c>
       <c r="C25" s="67" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="67" t="s">
         <v>74</v>
       </c>
-      <c r="D25" s="67" t="s">
-        <v>75</v>
-      </c>
       <c r="E25" s="66" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F25" s="68">
         <v>42061</v>
@@ -1868,13 +1874,13 @@
         <v>1</v>
       </c>
       <c r="C26" s="67" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" s="67" t="s">
         <v>76</v>
       </c>
-      <c r="D26" s="67" t="s">
-        <v>77</v>
-      </c>
       <c r="E26" s="66" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F26" s="68">
         <v>41995</v>
@@ -1889,19 +1895,19 @@
     </row>
     <row r="27" spans="1:9" s="19" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="71" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B27" s="66">
         <v>6</v>
       </c>
       <c r="C27" s="67" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D27" s="67" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" s="66" t="s">
         <v>57</v>
-      </c>
-      <c r="E27" s="66" t="s">
-        <v>58</v>
       </c>
       <c r="F27" s="68">
         <v>41989</v>
@@ -1914,19 +1920,19 @@
     </row>
     <row r="28" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A28" s="71" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B28" s="66">
         <v>7</v>
       </c>
       <c r="C28" s="67" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D28" s="67" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" s="66" t="s">
         <v>57</v>
-      </c>
-      <c r="E28" s="66" t="s">
-        <v>58</v>
       </c>
       <c r="F28" s="68">
         <v>41989</v>
@@ -1941,19 +1947,19 @@
     </row>
     <row r="29" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A29" s="71" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B29" s="66">
         <v>8</v>
       </c>
       <c r="C29" s="67" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29" s="67" t="s">
         <v>80</v>
       </c>
-      <c r="D29" s="67" t="s">
-        <v>81</v>
-      </c>
       <c r="E29" s="66" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F29" s="68">
         <v>41989</v>
@@ -1966,19 +1972,19 @@
     </row>
     <row r="30" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A30" s="71" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B30" s="66">
         <v>11</v>
       </c>
       <c r="C30" s="67" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="67" t="s">
         <v>82</v>
       </c>
-      <c r="D30" s="67" t="s">
-        <v>83</v>
-      </c>
       <c r="E30" s="66" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F30" s="68">
         <v>42050</v>
@@ -2005,7 +2011,7 @@
       <c r="B32" s="14"/>
       <c r="C32" s="28"/>
       <c r="D32" s="28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E32" s="29"/>
       <c r="F32" s="30"/>
@@ -2021,13 +2027,13 @@
         <v>1</v>
       </c>
       <c r="C33" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D33" s="34" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E33" s="33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F33" s="35">
         <v>41989</v>
@@ -2046,13 +2052,13 @@
         <v>2</v>
       </c>
       <c r="C34" s="34" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D34" s="34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E34" s="33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F34" s="35">
         <v>41991</v>
@@ -2071,13 +2077,13 @@
         <v>3</v>
       </c>
       <c r="C35" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="D35" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="D35" s="34" t="s">
-        <v>87</v>
-      </c>
       <c r="E35" s="33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F35" s="35">
         <v>41991</v>
@@ -2098,13 +2104,13 @@
         <v>5</v>
       </c>
       <c r="C36" s="34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D36" s="34" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E36" s="33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F36" s="35">
         <v>42120</v>
@@ -2119,16 +2125,16 @@
     </row>
     <row r="37" spans="1:9" s="19" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="74" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B37" s="33">
         <v>7</v>
       </c>
       <c r="C37" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="D37" s="34" t="s">
         <v>92</v>
-      </c>
-      <c r="D37" s="34" t="s">
-        <v>93</v>
       </c>
       <c r="E37" s="33"/>
       <c r="F37" s="35">
@@ -2140,16 +2146,16 @@
     </row>
     <row r="38" spans="1:9" s="19" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B38" s="20">
         <v>8</v>
       </c>
       <c r="C38" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" s="21" t="s">
         <v>94</v>
-      </c>
-      <c r="D38" s="21" t="s">
-        <v>95</v>
       </c>
       <c r="E38" s="20"/>
       <c r="F38" s="22">
@@ -2169,13 +2175,13 @@
         <v>4</v>
       </c>
       <c r="C39" s="67" t="s">
+        <v>95</v>
+      </c>
+      <c r="D39" s="67" t="s">
         <v>96</v>
       </c>
-      <c r="D39" s="67" t="s">
-        <v>97</v>
-      </c>
       <c r="E39" s="66" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F39" s="68">
         <v>42024</v>
@@ -2192,16 +2198,16 @@
     </row>
     <row r="40" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A40" s="71" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B40" s="66">
         <v>6</v>
       </c>
       <c r="C40" s="67" t="s">
+        <v>89</v>
+      </c>
+      <c r="D40" s="67" t="s">
         <v>90</v>
-      </c>
-      <c r="D40" s="67" t="s">
-        <v>91</v>
       </c>
       <c r="E40" s="66"/>
       <c r="F40" s="68">
@@ -2276,7 +2282,7 @@
     </row>
     <row r="2" spans="1:9" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B2"/>
       <c r="C2" s="7"/>
@@ -2286,7 +2292,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="56">
         <f ca="1">TODAY()</f>
-        <v>42243</v>
+        <v>42249</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -2323,7 +2329,7 @@
       <c r="B4" s="14"/>
       <c r="C4" s="15"/>
       <c r="D4" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4" s="16"/>
       <c r="F4" s="17"/>
@@ -2419,7 +2425,7 @@
       <c r="B12" s="14"/>
       <c r="C12" s="28"/>
       <c r="D12" s="28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E12" s="29"/>
       <c r="F12" s="30"/>
@@ -2461,10 +2467,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2495,7 +2501,7 @@
     </row>
     <row r="2" spans="1:9" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B2"/>
       <c r="C2" s="7"/>
@@ -2505,7 +2511,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="54">
         <f ca="1">TODAY()</f>
-        <v>42243</v>
+        <v>42249</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -2561,7 +2567,7 @@
         <v>26</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E5" s="20" t="s">
         <v>15</v>
@@ -2583,13 +2589,13 @@
         <v>2</v>
       </c>
       <c r="C6" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="D6" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="D6" s="21" t="s">
-        <v>136</v>
-      </c>
       <c r="E6" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F6" s="22">
         <v>42212</v>
@@ -2632,13 +2638,13 @@
         <v>9</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D9" s="34" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E9" s="33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F9" s="35">
         <v>42216</v>
@@ -2657,13 +2663,13 @@
         <v>10</v>
       </c>
       <c r="C10" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="D10" s="34" t="s">
         <v>140</v>
       </c>
-      <c r="D10" s="34" t="s">
-        <v>141</v>
-      </c>
       <c r="E10" s="33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F10" s="35">
         <v>42219</v>
@@ -2672,9 +2678,9 @@
       <c r="H10" s="22"/>
       <c r="I10" s="36"/>
     </row>
-    <row r="11" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" s="33">
         <v>4</v>
@@ -2683,23 +2689,23 @@
         <v>29</v>
       </c>
       <c r="D11" s="34" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="E11" s="33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F11" s="35">
         <v>42182</v>
       </c>
       <c r="G11" s="23"/>
       <c r="H11" s="22">
-        <v>42214</v>
+        <v>42249</v>
       </c>
       <c r="I11" s="36"/>
     </row>
     <row r="12" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" s="33">
         <v>5</v>
@@ -2708,10 +2714,10 @@
         <v>30</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E12" s="33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F12" s="35">
         <v>42182</v>
@@ -2722,43 +2728,43 @@
       </c>
       <c r="I12" s="36"/>
     </row>
-    <row r="13" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" s="33">
         <v>7</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="E13" s="33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F13" s="35">
         <v>42212</v>
       </c>
       <c r="G13" s="23"/>
       <c r="H13" s="22">
-        <v>42230</v>
+        <v>42249</v>
       </c>
       <c r="I13" s="36"/>
     </row>
     <row r="14" spans="1:9" s="19" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" s="33">
         <v>8</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E14" s="33" t="s">
         <v>15</v>
@@ -2772,7 +2778,7 @@
       </c>
       <c r="I14" s="36"/>
     </row>
-    <row r="15" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A15" s="46"/>
       <c r="B15" s="33">
         <v>1</v>
@@ -2781,7 +2787,7 @@
         <v>22</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="E15" s="33" t="s">
         <v>23</v>
@@ -2791,7 +2797,7 @@
       </c>
       <c r="G15" s="23"/>
       <c r="H15" s="22">
-        <v>42222</v>
+        <v>42249</v>
       </c>
       <c r="I15" s="36"/>
     </row>
@@ -2804,7 +2810,7 @@
         <v>24</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E16" s="33" t="s">
         <v>23</v>
@@ -2829,7 +2835,7 @@
         <v>25</v>
       </c>
       <c r="D17" s="34" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E17" s="33" t="s">
         <v>23</v>
@@ -2852,7 +2858,7 @@
         <v>32</v>
       </c>
       <c r="D18" s="67" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E18" s="66" t="s">
         <v>31</v>
@@ -2901,7 +2907,7 @@
         <v>14</v>
       </c>
       <c r="D21" s="34" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E21" s="33" t="s">
         <v>15</v>
@@ -2915,124 +2921,124 @@
       </c>
       <c r="I21" s="35"/>
     </row>
-    <row r="22" spans="1:9" s="19" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="73" t="s">
+    <row r="22" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A22" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="66">
+      <c r="B22" s="33">
+        <v>3</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="D22" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="E22" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="35">
+        <v>42249</v>
+      </c>
+      <c r="G22" s="45"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="35"/>
+    </row>
+    <row r="23" spans="1:9" s="19" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="73" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="66">
         <v>2</v>
       </c>
-      <c r="C22" s="67" t="s">
+      <c r="C23" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="67" t="s">
-        <v>145</v>
-      </c>
-      <c r="E22" s="66" t="s">
-        <v>42</v>
-      </c>
-      <c r="F22" s="68">
+      <c r="D23" s="67" t="s">
+        <v>143</v>
+      </c>
+      <c r="E23" s="66" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" s="68">
         <v>42160</v>
       </c>
-      <c r="G22" s="69"/>
-      <c r="H22" s="70">
+      <c r="G23" s="69"/>
+      <c r="H23" s="70">
         <v>42226</v>
       </c>
-      <c r="I22" s="72">
+      <c r="I23" s="72">
         <v>42228</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="44"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="36"/>
-    </row>
-    <row r="24" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="27"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28" t="s">
+    <row r="24" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="44"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="36"/>
+    </row>
+    <row r="25" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="27"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="29"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="31"/>
-    </row>
-    <row r="25" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="47"/>
-      <c r="B25" s="33">
+      <c r="E25" s="29"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="31"/>
+    </row>
+    <row r="26" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="47"/>
+      <c r="B26" s="33">
         <v>1</v>
       </c>
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="45"/>
-      <c r="H25" s="37"/>
-      <c r="I25" s="35"/>
-    </row>
-    <row r="26" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="44"/>
-      <c r="B26" s="33"/>
       <c r="C26" s="34"/>
       <c r="D26" s="34"/>
       <c r="E26" s="33"/>
       <c r="F26" s="35"/>
-      <c r="G26" s="35"/>
+      <c r="G26" s="45"/>
       <c r="H26" s="37"/>
-      <c r="I26" s="36"/>
-    </row>
-    <row r="27" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="27"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28" t="s">
+      <c r="I26" s="35"/>
+    </row>
+    <row r="27" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="44"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="35"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="36"/>
+    </row>
+    <row r="28" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="27"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="E27" s="29"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="31"/>
-    </row>
-    <row r="28" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="44"/>
-      <c r="B28" s="33">
-        <v>3</v>
-      </c>
-      <c r="C28" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="E28" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="F28" s="35">
-        <v>42179</v>
-      </c>
-      <c r="G28" s="35"/>
-      <c r="H28" s="37">
-        <v>42182</v>
-      </c>
-      <c r="I28" s="36"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="31"/>
     </row>
     <row r="29" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="44"/>
       <c r="B29" s="33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C29" s="34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D29" s="34" t="s">
         <v>33</v>
@@ -3052,114 +3058,139 @@
     <row r="30" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="44"/>
       <c r="B30" s="33">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C30" s="34" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D30" s="34" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E30" s="33" t="s">
         <v>20</v>
       </c>
       <c r="F30" s="35">
+        <v>42179</v>
+      </c>
+      <c r="G30" s="35"/>
+      <c r="H30" s="37">
         <v>42182</v>
       </c>
-      <c r="G30" s="35"/>
-      <c r="H30" s="37"/>
       <c r="I30" s="36"/>
     </row>
     <row r="31" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A31" s="44"/>
       <c r="B31" s="33">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C31" s="34" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D31" s="34" t="s">
-        <v>104</v>
+        <v>156</v>
       </c>
       <c r="E31" s="33" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="F31" s="35">
         <v>42182</v>
       </c>
-      <c r="G31" s="79">
+      <c r="G31" s="35"/>
+      <c r="H31" s="37">
+        <v>42249</v>
+      </c>
+      <c r="I31" s="36"/>
+    </row>
+    <row r="32" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A32" s="44"/>
+      <c r="B32" s="33">
+        <v>6</v>
+      </c>
+      <c r="C32" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="E32" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="F32" s="35">
+        <v>42182</v>
+      </c>
+      <c r="G32" s="79">
         <v>42223</v>
       </c>
-      <c r="H31" s="37"/>
-      <c r="I31" s="36"/>
-    </row>
-    <row r="32" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A32" s="78" t="s">
+      <c r="H32" s="37"/>
+      <c r="I32" s="36"/>
+    </row>
+    <row r="33" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A33" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="66">
+      <c r="B33" s="66">
         <v>1</v>
       </c>
-      <c r="C32" s="67" t="s">
+      <c r="C33" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="D32" s="67" t="s">
-        <v>103</v>
-      </c>
-      <c r="E32" s="66" t="s">
+      <c r="D33" s="67" t="s">
+        <v>102</v>
+      </c>
+      <c r="E33" s="66" t="s">
         <v>20</v>
-      </c>
-      <c r="F32" s="68">
-        <v>42160</v>
-      </c>
-      <c r="G32" s="69"/>
-      <c r="H32" s="70">
-        <v>42182</v>
-      </c>
-      <c r="I32" s="68">
-        <v>42202</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A33" s="84"/>
-      <c r="B33" s="66">
-        <v>2</v>
-      </c>
-      <c r="C33" s="67" t="s">
-        <v>21</v>
-      </c>
-      <c r="D33" s="67" t="s">
-        <v>142</v>
-      </c>
-      <c r="E33" s="66" t="s">
-        <v>42</v>
       </c>
       <c r="F33" s="68">
         <v>42160</v>
       </c>
-      <c r="G33" s="85">
-        <v>42216</v>
-      </c>
+      <c r="G33" s="69"/>
       <c r="H33" s="70">
         <v>42182</v>
       </c>
-      <c r="I33" s="72">
+      <c r="I33" s="68">
+        <v>42202</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A34" s="84"/>
+      <c r="B34" s="66">
+        <v>2</v>
+      </c>
+      <c r="C34" s="67" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="67" t="s">
+        <v>141</v>
+      </c>
+      <c r="E34" s="66" t="s">
+        <v>41</v>
+      </c>
+      <c r="F34" s="68">
+        <v>42160</v>
+      </c>
+      <c r="G34" s="85">
+        <v>42216</v>
+      </c>
+      <c r="H34" s="70">
+        <v>42182</v>
+      </c>
+      <c r="I34" s="72">
         <v>42223</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="44"/>
-      <c r="B34" s="33"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="35"/>
-      <c r="G34" s="35"/>
-      <c r="H34" s="37"/>
-      <c r="I34" s="36"/>
-    </row>
-    <row r="47" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D47" s="43"/>
+    <row r="35" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="44"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="37"/>
+      <c r="I35" s="36"/>
+    </row>
+    <row r="48" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D48" s="43"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
@@ -3211,7 +3242,7 @@
     </row>
     <row r="2" spans="1:9" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B2"/>
       <c r="C2" s="7"/>
@@ -3221,7 +3252,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="56">
         <f ca="1">TODAY()</f>
-        <v>42243</v>
+        <v>42249</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -3258,7 +3289,7 @@
       <c r="B4" s="14"/>
       <c r="C4" s="15"/>
       <c r="D4" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4" s="16"/>
       <c r="F4" s="17"/>
@@ -3322,7 +3353,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="20"/>
@@ -3365,10 +3396,10 @@
         <v>1</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E12" s="33"/>
       <c r="F12" s="35">
@@ -3394,7 +3425,7 @@
       <c r="B14" s="14"/>
       <c r="C14" s="28"/>
       <c r="D14" s="28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E14" s="29"/>
       <c r="F14" s="30"/>
@@ -3463,7 +3494,7 @@
     </row>
     <row r="2" spans="1:9" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2"/>
       <c r="C2" s="7"/>
@@ -3473,7 +3504,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="54">
         <f ca="1">TODAY()</f>
-        <v>42243</v>
+        <v>42249</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -3524,7 +3555,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D5" s="21"/>
       <c r="E5" s="20"/>
@@ -3539,7 +3570,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="20"/>
@@ -3554,7 +3585,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D7" s="21"/>
       <c r="E7" s="20"/>
@@ -3569,7 +3600,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="20"/>
@@ -3584,7 +3615,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D9" s="21"/>
       <c r="E9" s="20"/>
@@ -3599,7 +3630,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="20"/>
@@ -3614,7 +3645,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D11" s="21"/>
       <c r="E11" s="20"/>
@@ -3629,7 +3660,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="20"/>
@@ -3644,7 +3675,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="20"/>
@@ -3659,7 +3690,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="20"/>
@@ -3674,7 +3705,7 @@
         <v>11</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="20"/>
@@ -3689,7 +3720,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="20"/>
@@ -3704,7 +3735,7 @@
         <v>13</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D17" s="21"/>
       <c r="E17" s="20"/>
@@ -3719,7 +3750,7 @@
         <v>14</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D18" s="21"/>
       <c r="E18" s="20"/>
@@ -3734,7 +3765,7 @@
         <v>15</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D19" s="21"/>
       <c r="E19" s="20"/>
@@ -3749,7 +3780,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="20"/>
@@ -3764,7 +3795,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D21" s="21"/>
       <c r="E21" s="20"/>
@@ -3779,7 +3810,7 @@
         <v>18</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="20"/>
@@ -3794,7 +3825,7 @@
         <v>19</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D23" s="21"/>
       <c r="E23" s="20"/>
@@ -3809,7 +3840,7 @@
         <v>20</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D24" s="21"/>
       <c r="E24" s="20"/>
@@ -3954,7 +3985,7 @@
     </row>
     <row r="2" spans="1:9" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B2"/>
       <c r="C2" s="7"/>
@@ -3964,7 +3995,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="54">
         <f ca="1">TODAY()</f>
-        <v>42243</v>
+        <v>42249</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -4015,7 +4046,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D5" s="21"/>
       <c r="E5" s="20"/>
@@ -4030,7 +4061,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="20"/>
@@ -4045,7 +4076,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D7" s="21"/>
       <c r="E7" s="20"/>

</xml_diff>

<commit_message>
Updated timing and issues
The project is progressing well
</commit_message>
<xml_diff>
--- a/Project Tracking/SecuRemote Project Issues.xlsx
+++ b/Project Tracking/SecuRemote Project Issues.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="170">
   <si>
     <t>Open Issues List</t>
   </si>
@@ -461,9 +461,6 @@
     <t>GDO control wires are too short. Need to be about 16 feet long.</t>
   </si>
   <si>
-    <t>Threads were wrong for collar, date code not stamped in.  Waiting for resubmission from supplier. 8/6 - still waiting. 9/2 - threads still wrong for our rose nut sample.</t>
-  </si>
-  <si>
     <t>App doesn't ask if user wants to operate the device remotely when out of Bluetooth range and BT is ON.</t>
   </si>
   <si>
@@ -491,29 +488,12 @@
     <t>Doug       Dave</t>
   </si>
   <si>
-    <t>Do we send rev C CPUs or wait for Rev D? Need to get timing from Intertek. They can start 1st week of September. 8/17 - parts ordered. 9/3 - parts sent. 9/11 - Testing to start week of 9/14.</t>
-  </si>
-  <si>
     <t>Currently 32 LH and 11 RH assemblies in house. Need to order more of each and schedule assembly with Gene. 9/11 - Jim to check on status.</t>
   </si>
   <si>
     <t>Jim B</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Verify in displays. Order several samples. 8/13- samples received. When batteries installed, housing is too thick. Found a better solution on Alibaba. Ashley to order samples. Parts from Stride don't work. More coming from Tysonic. 9/10 - No useable sample from either vendors, yet. Need to revert back to previous battery pack and harnesses. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>9/11 - Jim to look for rubber band and other solutions.</t>
-    </r>
-  </si>
-  <si>
     <t>Non-GDO Bridge</t>
   </si>
   <si>
@@ -523,13 +503,7 @@
     <t>Locks for testing at Delphian</t>
   </si>
   <si>
-    <t>Ashok, Bhikhu need more lock assemblies, with new CPU and harnesses.</t>
-  </si>
-  <si>
     <t>Apps need to be tested and submitted to App Stores.</t>
-  </si>
-  <si>
-    <t>Apple takes at least 1 week, up to 2 weeks</t>
   </si>
   <si>
     <t>On the roadmap, not being developed yet.</t>
@@ -557,7 +531,22 @@
     </r>
   </si>
   <si>
-    <t>Approx. 15 Ethernet bridges were built. Are those up to date?</t>
+    <t>Rules for notifications needs to be defined. 9/2 - Preliminary code in place. 9/14 - I tested it on Android, looks good, just some minor issues.</t>
+  </si>
+  <si>
+    <t>Threads were wrong for collar, date code not stamped in.  Waiting for resubmission from supplier. 8/6 - still waiting. 9/2 - threads still wrong for our rose nut sample.9/22 - Found matching nut, Fas approved.</t>
+  </si>
+  <si>
+    <t>Approx. 15 Ethernet bridges were built. Approx. 23 CDMA units were built. JV wants 150 Ethernet units.</t>
+  </si>
+  <si>
+    <t>Ashok, Bhikhu need more lock assemblies, with new CPU and harnesses. 9/18 - Two locks ordered, more available from Intertek week of 9/28.</t>
+  </si>
+  <si>
+    <t>Verify in displays. Order several samples. 8/13- samples received. When batteries installed, housing is too thick. Found a better solution on Alibaba. Ashley to order samples. Parts from Stride don't work. More coming from Tysonic. 9/10 - No useable sample from either vendors, yet. Need to revert back to previous battery pack and harnesses. 9/11 - Jim to look for rubber band and other solutions. 9/22 - One large band works well for the current housing. Design team is working on a prototype cover.</t>
+  </si>
+  <si>
+    <t>Do we send rev C CPUs or wait for Rev D? Need to get timing from Intertek. They can start 1st week of September. 8/17 - parts ordered. 9/3 - parts sent. 9/11 - Testing to start week of 9/14. 9/22 - Testing complete. Failed Door Slam Test (battery issue?). Locks to be returned this week.</t>
   </si>
   <si>
     <r>
@@ -578,11 +567,14 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> length and add sleeving, so harness can be routed behind battery housing. ECO-1139. Verify parts when available. 7/27 - order parts 8/13 - Parts on order (PO 122419), 100pcs. 9/11 - parts received. Sleeving is a bit stiff and snags on Mortise lock while installing. Getting feedback from manufacturing. 9/14 - Jay doesn't like it.</t>
+      <t xml:space="preserve"> length and add sleeving, so harness can be routed behind battery housing. ECO-1139. Verify parts when available. 7/27 - order parts 8/13 - Parts on order (PO 122419), 100pcs. 9/11 - parts received. Sleeving is a bit stiff and snags on Mortise lock while installing. Getting feedback from manufacturing. 9/14 - Jay doesn't like it. Tubing is too thick. We will remove tubing and use up this batch, but a better solution needs to be found.</t>
     </r>
   </si>
   <si>
-    <t>Rules for notifications needs to be defined. 9/2 - Preliminary code in place. 9/14 - I tested it on Android, looks good, just some minor issues.</t>
+    <t>Apple takes at least 1 week, up to 2 weeks. 9/21 - Apps submitted. Android ready.</t>
+  </si>
+  <si>
+    <t>Closed Issues</t>
   </si>
 </sst>
 </file>
@@ -707,7 +699,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -747,6 +739,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -815,7 +813,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -956,9 +954,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1034,9 +1029,6 @@
     <xf numFmtId="0" fontId="16" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1087,6 +1079,18 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1398,7 +1402,7 @@
   <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1425,7 +1429,7 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="5"/>
-      <c r="I1" s="55"/>
+      <c r="I1" s="54"/>
     </row>
     <row r="2" spans="1:9" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -1437,37 +1441,37 @@
       <c r="E2" s="8"/>
       <c r="G2" s="10"/>
       <c r="H2" s="11"/>
-      <c r="I2" s="56">
+      <c r="I2" s="55">
         <f ca="1">TODAY()</f>
-        <v>42261</v>
+        <v>42269</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="57" t="s">
+      <c r="D3" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="57" t="s">
+      <c r="E3" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="58" t="s">
+      <c r="F3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="58" t="s">
+      <c r="G3" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="59" t="s">
+      <c r="H3" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="58" t="s">
+      <c r="I3" s="57" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1485,127 +1489,135 @@
       <c r="I4" s="18"/>
     </row>
     <row r="5" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="65">
         <v>1</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="22">
+      <c r="F5" s="67">
         <v>42048</v>
       </c>
-      <c r="G5" s="23"/>
-      <c r="H5" s="24">
+      <c r="G5" s="68"/>
+      <c r="H5" s="69">
         <v>42185</v>
       </c>
-      <c r="I5" s="22"/>
+      <c r="I5" s="67">
+        <v>42269</v>
+      </c>
     </row>
     <row r="6" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="20">
+      <c r="B6" s="65">
         <v>2</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="22">
+      <c r="F6" s="67">
         <v>42047</v>
       </c>
-      <c r="G6" s="23"/>
-      <c r="H6" s="24">
+      <c r="G6" s="68"/>
+      <c r="H6" s="69">
         <v>42185</v>
       </c>
-      <c r="I6" s="22"/>
+      <c r="I6" s="67">
+        <v>42269</v>
+      </c>
     </row>
     <row r="7" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="65" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="20">
+      <c r="B7" s="65">
         <v>3</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="67">
         <v>42048</v>
       </c>
-      <c r="G7" s="23"/>
-      <c r="H7" s="24">
+      <c r="G7" s="68"/>
+      <c r="H7" s="69">
         <v>42121</v>
       </c>
-      <c r="I7" s="22"/>
+      <c r="I7" s="67">
+        <v>42269</v>
+      </c>
     </row>
     <row r="8" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="20">
+      <c r="B8" s="65">
         <v>4</v>
       </c>
-      <c r="C8" s="61" t="s">
+      <c r="C8" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="61" t="s">
+      <c r="D8" s="78" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="62" t="s">
+      <c r="E8" s="79" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="63">
+      <c r="F8" s="71">
         <v>42048</v>
       </c>
-      <c r="G8" s="64"/>
-      <c r="H8" s="65"/>
-      <c r="I8" s="63"/>
+      <c r="G8" s="90"/>
+      <c r="H8" s="81"/>
+      <c r="I8" s="71">
+        <v>42269</v>
+      </c>
     </row>
     <row r="9" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="71" t="s">
+      <c r="A9" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="66">
+      <c r="B9" s="65">
         <v>5</v>
       </c>
-      <c r="C9" s="80" t="s">
+      <c r="C9" s="78" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="80" t="s">
+      <c r="D9" s="78" t="s">
         <v>103</v>
       </c>
-      <c r="E9" s="81" t="s">
+      <c r="E9" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="72">
+      <c r="F9" s="71">
         <v>42062</v>
       </c>
-      <c r="G9" s="82"/>
-      <c r="H9" s="83">
+      <c r="G9" s="80"/>
+      <c r="H9" s="81">
         <v>42195</v>
       </c>
-      <c r="I9" s="72">
+      <c r="I9" s="71">
         <v>42202</v>
       </c>
     </row>
@@ -1623,13 +1635,13 @@
     <row r="11" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="32"/>
       <c r="B11" s="20"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="64"/>
-      <c r="H11" s="65"/>
-      <c r="I11" s="63"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="64"/>
+      <c r="I11" s="62"/>
     </row>
     <row r="12" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13"/>
@@ -1645,79 +1657,79 @@
       <c r="I12" s="18"/>
     </row>
     <row r="13" spans="1:9" s="19" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="66" t="s">
+      <c r="A13" s="65" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="66"/>
-      <c r="C13" s="67" t="s">
+      <c r="B13" s="65"/>
+      <c r="C13" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="67"/>
-      <c r="E13" s="66" t="s">
+      <c r="D13" s="66"/>
+      <c r="E13" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="68">
+      <c r="F13" s="67">
         <v>41992</v>
       </c>
-      <c r="G13" s="69"/>
-      <c r="H13" s="70"/>
-      <c r="I13" s="68">
+      <c r="G13" s="68"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="67">
         <v>42045</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="19" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="66" t="s">
+      <c r="A14" s="65" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="66">
+      <c r="B14" s="65">
         <v>2</v>
       </c>
-      <c r="C14" s="67" t="s">
+      <c r="C14" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="67" t="s">
+      <c r="D14" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="E14" s="66" t="s">
+      <c r="E14" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="68">
+      <c r="F14" s="67">
         <v>41992</v>
       </c>
-      <c r="G14" s="68">
+      <c r="G14" s="67">
         <v>42068</v>
       </c>
-      <c r="H14" s="70"/>
-      <c r="I14" s="68">
+      <c r="H14" s="69"/>
+      <c r="I14" s="67">
         <v>42078</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="19" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="66" t="s">
+      <c r="A15" s="65" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="66">
+      <c r="B15" s="65">
         <v>1</v>
       </c>
-      <c r="C15" s="67" t="s">
+      <c r="C15" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="67" t="s">
+      <c r="D15" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="66" t="s">
+      <c r="E15" s="65" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="68">
+      <c r="F15" s="67">
         <v>41989</v>
       </c>
-      <c r="G15" s="69">
+      <c r="G15" s="68">
         <v>42076</v>
       </c>
-      <c r="H15" s="70">
+      <c r="H15" s="69">
         <v>42050</v>
       </c>
-      <c r="I15" s="68">
+      <c r="I15" s="67">
         <v>42122</v>
       </c>
     </row>
@@ -1746,329 +1758,341 @@
       <c r="I17" s="31"/>
     </row>
     <row r="18" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="33">
+      <c r="B18" s="65">
         <v>2</v>
       </c>
-      <c r="C18" s="34" t="s">
+      <c r="C18" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="34" t="s">
+      <c r="D18" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="33" t="s">
+      <c r="E18" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="35">
+      <c r="F18" s="67">
         <v>42093</v>
       </c>
-      <c r="G18" s="23"/>
-      <c r="H18" s="22">
+      <c r="G18" s="68"/>
+      <c r="H18" s="67">
         <v>42121</v>
       </c>
-      <c r="I18" s="36"/>
+      <c r="I18" s="71">
+        <v>42269</v>
+      </c>
     </row>
     <row r="19" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="46" t="s">
+      <c r="A19" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="33">
+      <c r="B19" s="65">
         <v>3</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="C19" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="D19" s="34" t="s">
+      <c r="D19" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="E19" s="33" t="s">
+      <c r="E19" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="F19" s="35">
+      <c r="F19" s="67">
         <v>42102</v>
       </c>
-      <c r="G19" s="23"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="36"/>
+      <c r="G19" s="68"/>
+      <c r="H19" s="67"/>
+      <c r="I19" s="71">
+        <v>42269</v>
+      </c>
     </row>
     <row r="20" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A20" s="46" t="s">
+      <c r="A20" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="33">
+      <c r="B20" s="65">
         <v>4</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="C20" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="34" t="s">
+      <c r="D20" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="E20" s="33" t="s">
+      <c r="E20" s="65" t="s">
         <v>63</v>
       </c>
-      <c r="F20" s="35">
+      <c r="F20" s="67">
         <v>42102</v>
       </c>
-      <c r="G20" s="23"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="36"/>
+      <c r="G20" s="68"/>
+      <c r="H20" s="67"/>
+      <c r="I20" s="71">
+        <v>42269</v>
+      </c>
     </row>
     <row r="21" spans="1:9" s="19" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="32" t="s">
+      <c r="A21" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="33">
+      <c r="B21" s="65">
         <v>5</v>
       </c>
-      <c r="C21" s="34" t="s">
+      <c r="C21" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="34" t="s">
+      <c r="D21" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="E21" s="33" t="s">
+      <c r="E21" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="F21" s="35">
+      <c r="F21" s="67">
         <v>42024</v>
       </c>
-      <c r="G21" s="23"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="36"/>
+      <c r="G21" s="68"/>
+      <c r="H21" s="67"/>
+      <c r="I21" s="71">
+        <v>42269</v>
+      </c>
     </row>
     <row r="22" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A22" s="32" t="s">
+      <c r="A22" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="33">
+      <c r="B22" s="65">
         <v>9</v>
       </c>
-      <c r="C22" s="34" t="s">
+      <c r="C22" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="D22" s="34" t="s">
+      <c r="D22" s="66" t="s">
         <v>98</v>
       </c>
-      <c r="E22" s="33" t="s">
+      <c r="E22" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="F22" s="35">
+      <c r="F22" s="67">
         <v>41992</v>
       </c>
-      <c r="G22" s="23"/>
-      <c r="H22" s="22">
+      <c r="G22" s="68"/>
+      <c r="H22" s="67">
         <v>42195</v>
       </c>
-      <c r="I22" s="36"/>
+      <c r="I22" s="71">
+        <v>42269</v>
+      </c>
     </row>
     <row r="23" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A23" s="32" t="s">
+      <c r="A23" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="33">
+      <c r="B23" s="65">
         <v>10</v>
       </c>
-      <c r="C23" s="34" t="s">
+      <c r="C23" s="66" t="s">
         <v>68</v>
       </c>
-      <c r="D23" s="34" t="s">
+      <c r="D23" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="E23" s="33" t="s">
+      <c r="E23" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="F23" s="35">
+      <c r="F23" s="67">
         <v>42050</v>
       </c>
-      <c r="G23" s="23"/>
-      <c r="H23" s="22">
+      <c r="G23" s="68"/>
+      <c r="H23" s="67">
         <v>42121</v>
       </c>
-      <c r="I23" s="36"/>
+      <c r="I23" s="71">
+        <v>42269</v>
+      </c>
     </row>
     <row r="24" spans="1:9" s="19" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="71" t="s">
+      <c r="A24" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="66">
+      <c r="B24" s="65">
         <v>5</v>
       </c>
-      <c r="C24" s="67" t="s">
+      <c r="C24" s="66" t="s">
         <v>70</v>
       </c>
-      <c r="D24" s="67" t="s">
+      <c r="D24" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="E24" s="66" t="s">
+      <c r="E24" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="68">
+      <c r="F24" s="67">
         <v>42000</v>
       </c>
-      <c r="G24" s="68"/>
-      <c r="H24" s="70">
+      <c r="G24" s="67"/>
+      <c r="H24" s="69">
         <v>42026</v>
       </c>
-      <c r="I24" s="72">
+      <c r="I24" s="71">
         <v>42089</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="19" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="71" t="s">
+      <c r="A25" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="66">
+      <c r="B25" s="65">
         <v>3</v>
       </c>
-      <c r="C25" s="67" t="s">
+      <c r="C25" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="D25" s="67" t="s">
+      <c r="D25" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="E25" s="66" t="s">
+      <c r="E25" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="F25" s="68">
+      <c r="F25" s="67">
         <v>42061</v>
       </c>
-      <c r="G25" s="69"/>
-      <c r="H25" s="68">
+      <c r="G25" s="68"/>
+      <c r="H25" s="67">
         <v>42072</v>
       </c>
-      <c r="I25" s="72">
+      <c r="I25" s="71">
         <v>42089</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A26" s="73" t="s">
+      <c r="A26" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="66">
+      <c r="B26" s="65">
         <v>1</v>
       </c>
-      <c r="C26" s="67" t="s">
+      <c r="C26" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="D26" s="67" t="s">
+      <c r="D26" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="E26" s="66" t="s">
+      <c r="E26" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="F26" s="68">
+      <c r="F26" s="67">
         <v>41995</v>
       </c>
-      <c r="G26" s="69"/>
-      <c r="H26" s="68">
+      <c r="G26" s="68"/>
+      <c r="H26" s="67">
         <v>42072</v>
       </c>
-      <c r="I26" s="72">
+      <c r="I26" s="71">
         <v>42097</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="19" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="71" t="s">
+      <c r="A27" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="66">
+      <c r="B27" s="65">
         <v>6</v>
       </c>
-      <c r="C27" s="67" t="s">
+      <c r="C27" s="66" t="s">
         <v>76</v>
       </c>
-      <c r="D27" s="67" t="s">
+      <c r="D27" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="E27" s="66" t="s">
+      <c r="E27" s="65" t="s">
         <v>56</v>
       </c>
-      <c r="F27" s="68">
+      <c r="F27" s="67">
         <v>41989</v>
       </c>
-      <c r="G27" s="69"/>
-      <c r="H27" s="68"/>
-      <c r="I27" s="72">
+      <c r="G27" s="68"/>
+      <c r="H27" s="67"/>
+      <c r="I27" s="71">
         <v>42121</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A28" s="71" t="s">
+      <c r="A28" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="66">
+      <c r="B28" s="65">
         <v>7</v>
       </c>
-      <c r="C28" s="67" t="s">
+      <c r="C28" s="66" t="s">
         <v>77</v>
       </c>
-      <c r="D28" s="67" t="s">
+      <c r="D28" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="E28" s="66" t="s">
+      <c r="E28" s="65" t="s">
         <v>56</v>
       </c>
-      <c r="F28" s="68">
+      <c r="F28" s="67">
         <v>41989</v>
       </c>
-      <c r="G28" s="69"/>
-      <c r="H28" s="68">
+      <c r="G28" s="68"/>
+      <c r="H28" s="67">
         <v>42050</v>
       </c>
-      <c r="I28" s="72">
+      <c r="I28" s="71">
         <v>42121</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A29" s="71" t="s">
+      <c r="A29" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="66">
+      <c r="B29" s="65">
         <v>8</v>
       </c>
-      <c r="C29" s="67" t="s">
+      <c r="C29" s="66" t="s">
         <v>78</v>
       </c>
-      <c r="D29" s="67" t="s">
+      <c r="D29" s="66" t="s">
         <v>79</v>
       </c>
-      <c r="E29" s="66" t="s">
+      <c r="E29" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="F29" s="68">
+      <c r="F29" s="67">
         <v>41989</v>
       </c>
-      <c r="G29" s="69"/>
-      <c r="H29" s="68"/>
-      <c r="I29" s="72">
+      <c r="G29" s="68"/>
+      <c r="H29" s="67"/>
+      <c r="I29" s="71">
         <v>42121</v>
       </c>
     </row>
     <row r="30" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A30" s="71" t="s">
+      <c r="A30" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="B30" s="66">
+      <c r="B30" s="65">
         <v>11</v>
       </c>
-      <c r="C30" s="67" t="s">
+      <c r="C30" s="66" t="s">
         <v>80</v>
       </c>
-      <c r="D30" s="67" t="s">
+      <c r="D30" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="E30" s="66" t="s">
+      <c r="E30" s="65" t="s">
         <v>56</v>
       </c>
-      <c r="F30" s="68">
+      <c r="F30" s="67">
         <v>42050</v>
       </c>
-      <c r="G30" s="69"/>
-      <c r="H30" s="68"/>
-      <c r="I30" s="72">
+      <c r="G30" s="68"/>
+      <c r="H30" s="67"/>
+      <c r="I30" s="71">
         <v>42121</v>
       </c>
     </row>
@@ -2096,205 +2120,217 @@
       <c r="H32" s="30"/>
       <c r="I32" s="31"/>
     </row>
-    <row r="33" spans="1:9" s="19" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A33" s="47" t="s">
+    <row r="33" spans="1:9" s="19" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="B33" s="33">
+      <c r="B33" s="65">
         <v>1</v>
       </c>
-      <c r="C33" s="34" t="s">
+      <c r="C33" s="66" t="s">
         <v>83</v>
       </c>
-      <c r="D33" s="34" t="s">
+      <c r="D33" s="66" t="s">
         <v>104</v>
       </c>
-      <c r="E33" s="33" t="s">
+      <c r="E33" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="F33" s="35">
+      <c r="F33" s="67">
         <v>41989</v>
       </c>
-      <c r="G33" s="79">
+      <c r="G33" s="83">
         <v>42216</v>
       </c>
-      <c r="H33" s="37"/>
-      <c r="I33" s="35"/>
+      <c r="H33" s="69"/>
+      <c r="I33" s="67">
+        <v>42269</v>
+      </c>
     </row>
     <row r="34" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A34" s="48" t="s">
+      <c r="A34" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="33">
+      <c r="B34" s="65">
         <v>2</v>
       </c>
-      <c r="C34" s="34" t="s">
+      <c r="C34" s="66" t="s">
         <v>99</v>
       </c>
-      <c r="D34" s="34" t="s">
+      <c r="D34" s="66" t="s">
         <v>105</v>
       </c>
-      <c r="E34" s="33" t="s">
+      <c r="E34" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="F34" s="35">
+      <c r="F34" s="67">
         <v>41991</v>
       </c>
-      <c r="G34" s="79">
+      <c r="G34" s="83">
         <v>42216</v>
       </c>
-      <c r="H34" s="37"/>
-      <c r="I34" s="36"/>
+      <c r="H34" s="69"/>
+      <c r="I34" s="71">
+        <v>42269</v>
+      </c>
     </row>
     <row r="35" spans="1:9" s="19" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="48" t="s">
+      <c r="A35" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B35" s="33">
+      <c r="B35" s="65">
         <v>3</v>
       </c>
-      <c r="C35" s="34" t="s">
+      <c r="C35" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="D35" s="34" t="s">
+      <c r="D35" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="E35" s="33" t="s">
+      <c r="E35" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="F35" s="35">
+      <c r="F35" s="67">
         <v>41991</v>
       </c>
-      <c r="G35" s="45">
+      <c r="G35" s="68">
         <v>42076</v>
       </c>
-      <c r="H35" s="37">
+      <c r="H35" s="69">
         <v>42102</v>
       </c>
-      <c r="I35" s="36"/>
+      <c r="I35" s="71">
+        <v>42269</v>
+      </c>
     </row>
     <row r="36" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A36" s="48" t="s">
+      <c r="A36" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="33">
+      <c r="B36" s="65">
         <v>5</v>
       </c>
-      <c r="C36" s="34" t="s">
+      <c r="C36" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="D36" s="34" t="s">
+      <c r="D36" s="66" t="s">
         <v>106</v>
       </c>
-      <c r="E36" s="33" t="s">
+      <c r="E36" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="F36" s="35">
+      <c r="F36" s="67">
         <v>42120</v>
       </c>
-      <c r="G36" s="79">
+      <c r="G36" s="83">
         <v>42216</v>
       </c>
-      <c r="H36" s="37">
+      <c r="H36" s="69">
         <v>42195</v>
       </c>
-      <c r="I36" s="36"/>
+      <c r="I36" s="71">
+        <v>42269</v>
+      </c>
     </row>
     <row r="37" spans="1:9" s="19" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="74" t="s">
+      <c r="A37" s="70" t="s">
         <v>87</v>
       </c>
-      <c r="B37" s="33">
+      <c r="B37" s="65">
         <v>7</v>
       </c>
-      <c r="C37" s="34" t="s">
+      <c r="C37" s="66" t="s">
         <v>90</v>
       </c>
-      <c r="D37" s="34" t="s">
+      <c r="D37" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="E37" s="33"/>
-      <c r="F37" s="35">
+      <c r="E37" s="65"/>
+      <c r="F37" s="67">
         <v>42040</v>
       </c>
-      <c r="G37" s="35"/>
-      <c r="H37" s="37"/>
-      <c r="I37" s="36"/>
+      <c r="G37" s="67"/>
+      <c r="H37" s="69"/>
+      <c r="I37" s="71">
+        <v>42269</v>
+      </c>
     </row>
     <row r="38" spans="1:9" s="19" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="20" t="s">
+      <c r="A38" s="65" t="s">
         <v>87</v>
       </c>
-      <c r="B38" s="20">
+      <c r="B38" s="65">
         <v>8</v>
       </c>
-      <c r="C38" s="21" t="s">
+      <c r="C38" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="D38" s="21" t="s">
+      <c r="D38" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="E38" s="20"/>
-      <c r="F38" s="22">
+      <c r="E38" s="65"/>
+      <c r="F38" s="67">
         <v>41989</v>
       </c>
-      <c r="G38" s="22"/>
-      <c r="H38" s="24">
+      <c r="G38" s="67"/>
+      <c r="H38" s="69">
         <v>42121</v>
       </c>
-      <c r="I38" s="22"/>
+      <c r="I38" s="67">
+        <v>42269</v>
+      </c>
     </row>
     <row r="39" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A39" s="73" t="s">
+      <c r="A39" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B39" s="66">
+      <c r="B39" s="65">
         <v>4</v>
       </c>
-      <c r="C39" s="67" t="s">
+      <c r="C39" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="D39" s="67" t="s">
+      <c r="D39" s="66" t="s">
         <v>95</v>
       </c>
-      <c r="E39" s="66" t="s">
+      <c r="E39" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="F39" s="68">
+      <c r="F39" s="67">
         <v>42024</v>
       </c>
-      <c r="G39" s="69">
+      <c r="G39" s="68">
         <v>42097</v>
       </c>
-      <c r="H39" s="70">
+      <c r="H39" s="69">
         <v>42098</v>
       </c>
-      <c r="I39" s="72">
+      <c r="I39" s="71">
         <v>42121</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A40" s="71" t="s">
+      <c r="A40" s="70" t="s">
         <v>87</v>
       </c>
-      <c r="B40" s="66">
+      <c r="B40" s="65">
         <v>6</v>
       </c>
-      <c r="C40" s="67" t="s">
+      <c r="C40" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="D40" s="67" t="s">
+      <c r="D40" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="E40" s="66"/>
-      <c r="F40" s="68">
+      <c r="E40" s="65"/>
+      <c r="F40" s="67">
         <v>42024</v>
       </c>
-      <c r="G40" s="68"/>
-      <c r="H40" s="70">
+      <c r="G40" s="67"/>
+      <c r="H40" s="69">
         <v>42121</v>
       </c>
-      <c r="I40" s="72">
+      <c r="I40" s="71">
         <v>42195</v>
       </c>
     </row>
@@ -2355,7 +2391,7 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="5"/>
-      <c r="I1" s="55"/>
+      <c r="I1" s="54"/>
     </row>
     <row r="2" spans="1:9" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -2367,37 +2403,37 @@
       <c r="E2" s="8"/>
       <c r="G2" s="10"/>
       <c r="H2" s="11"/>
-      <c r="I2" s="56">
+      <c r="I2" s="55">
         <f ca="1">TODAY()</f>
-        <v>42261</v>
+        <v>42269</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="75" t="s">
+      <c r="C3" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="75" t="s">
+      <c r="D3" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="75" t="s">
+      <c r="E3" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="76" t="s">
+      <c r="F3" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="76" t="s">
+      <c r="G3" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="77" t="s">
+      <c r="H3" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="76" t="s">
+      <c r="I3" s="74" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2415,7 +2451,7 @@
       <c r="I4" s="18"/>
     </row>
     <row r="5" spans="1:9" s="19" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="60"/>
+      <c r="A5" s="59"/>
       <c r="B5" s="20">
         <v>1</v>
       </c>
@@ -2441,13 +2477,13 @@
     <row r="7" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="32"/>
       <c r="B7" s="20"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="64"/>
-      <c r="H7" s="65"/>
-      <c r="I7" s="63"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="62"/>
     </row>
     <row r="8" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13"/>
@@ -2544,10 +2580,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2565,7 +2601,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="53"/>
+      <c r="A1" s="52"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2586,37 +2622,37 @@
       <c r="E2" s="8"/>
       <c r="G2" s="10"/>
       <c r="H2" s="11"/>
-      <c r="I2" s="54">
+      <c r="I2" s="53">
         <f ca="1">TODAY()</f>
-        <v>42261</v>
+        <v>42269</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="49" t="s">
+      <c r="E3" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="50" t="s">
+      <c r="F3" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="50" t="s">
+      <c r="G3" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="51" t="s">
+      <c r="H3" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="50" t="s">
+      <c r="I3" s="49" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2634,9 +2670,7 @@
       <c r="I4" s="18"/>
     </row>
     <row r="5" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A5" s="52" t="s">
-        <v>12</v>
-      </c>
+      <c r="A5" s="51"/>
       <c r="B5" s="20">
         <v>1</v>
       </c>
@@ -2644,10 +2678,10 @@
         <v>26</v>
       </c>
       <c r="D5" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="E5" s="20" t="s">
         <v>152</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>153</v>
       </c>
       <c r="F5" s="22">
         <v>42177</v>
@@ -2661,9 +2695,7 @@
       <c r="I5" s="22"/>
     </row>
     <row r="6" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="52" t="s">
-        <v>12</v>
-      </c>
+      <c r="A6" s="51"/>
       <c r="B6" s="20">
         <v>2</v>
       </c>
@@ -2671,7 +2703,7 @@
         <v>132</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E6" s="20" t="s">
         <v>40</v>
@@ -2700,170 +2732,174 @@
       <c r="H7" s="30"/>
       <c r="I7" s="31"/>
     </row>
-    <row r="8" spans="1:9" s="19" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" s="19" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A8" s="46" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="33">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>134</v>
+        <v>30</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>156</v>
+        <v>40</v>
       </c>
       <c r="F8" s="35">
-        <v>42212</v>
-      </c>
-      <c r="G8" s="89">
-        <v>42279</v>
+        <v>42182</v>
+      </c>
+      <c r="G8" s="87">
+        <v>42307</v>
       </c>
       <c r="H8" s="22">
-        <v>42257</v>
+        <v>42261</v>
       </c>
       <c r="I8" s="36"/>
     </row>
-    <row r="9" spans="1:9" s="19" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" s="19" customFormat="1" ht="104.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="46" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="33">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D9" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="E9" s="33" t="s">
         <v>154</v>
       </c>
-      <c r="E9" s="33" t="s">
-        <v>40</v>
-      </c>
       <c r="F9" s="35">
-        <v>42216</v>
-      </c>
-      <c r="G9" s="89">
-        <v>42293</v>
+        <v>42212</v>
+      </c>
+      <c r="G9" s="87">
+        <v>42279</v>
       </c>
       <c r="H9" s="22">
-        <v>42258</v>
+        <v>42257</v>
       </c>
       <c r="I9" s="36"/>
     </row>
-    <row r="10" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" s="19" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A10" s="46" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="33">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>156</v>
+        <v>40</v>
       </c>
       <c r="F10" s="35">
-        <v>42219</v>
-      </c>
-      <c r="G10" s="89">
-        <v>42265</v>
+        <v>42216</v>
+      </c>
+      <c r="G10" s="87">
+        <v>42293</v>
       </c>
       <c r="H10" s="22">
         <v>42258</v>
       </c>
       <c r="I10" s="36"/>
     </row>
-    <row r="11" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A11" s="46" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="33">
+        <v>10</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="F11" s="35">
+        <v>42219</v>
+      </c>
+      <c r="G11" s="87">
+        <v>42307</v>
+      </c>
+      <c r="H11" s="22">
+        <v>42258</v>
+      </c>
+      <c r="I11" s="36"/>
+    </row>
+    <row r="12" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="34" t="s">
-        <v>160</v>
-      </c>
-      <c r="D11" s="34" t="s">
-        <v>161</v>
-      </c>
-      <c r="E11" s="33" t="s">
-        <v>156</v>
-      </c>
-      <c r="F11" s="35">
+      <c r="B12" s="33">
+        <v>12</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>164</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="F12" s="35">
         <v>42258</v>
       </c>
-      <c r="G11" s="89">
-        <v>42265</v>
-      </c>
-      <c r="H11" s="22"/>
-      <c r="I11" s="36"/>
-    </row>
-    <row r="12" spans="1:9" s="19" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="91" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="33">
-        <v>5</v>
-      </c>
-      <c r="C12" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="34" t="s">
-        <v>167</v>
-      </c>
-      <c r="E12" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="F12" s="35">
-        <v>42182</v>
-      </c>
-      <c r="G12" s="23"/>
+      <c r="G12" s="87">
+        <v>42281</v>
+      </c>
       <c r="H12" s="22">
-        <v>42261</v>
+        <v>42269</v>
       </c>
       <c r="I12" s="36"/>
     </row>
-    <row r="13" spans="1:9" s="19" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="91" t="s">
-        <v>44</v>
-      </c>
+    <row r="13" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A13" s="32"/>
       <c r="B13" s="33">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>158</v>
+        <v>24</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="E13" s="33" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="F13" s="35">
-        <v>42258</v>
-      </c>
-      <c r="G13" s="89"/>
-      <c r="H13" s="22"/>
+        <v>42178</v>
+      </c>
+      <c r="G13" s="23"/>
+      <c r="H13" s="22">
+        <v>42235</v>
+      </c>
       <c r="I13" s="36"/>
     </row>
-    <row r="14" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="46"/>
+    <row r="14" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="32"/>
       <c r="B14" s="33">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="E14" s="33" t="s">
         <v>23</v>
@@ -2873,139 +2909,109 @@
       </c>
       <c r="G14" s="23"/>
       <c r="H14" s="22">
-        <v>42249</v>
+        <v>42222</v>
       </c>
       <c r="I14" s="36"/>
     </row>
-    <row r="15" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A15" s="32"/>
+    <row r="15" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="89"/>
       <c r="B15" s="33">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>24</v>
+        <v>155</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
       <c r="E15" s="33" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F15" s="35">
-        <v>42178</v>
-      </c>
-      <c r="G15" s="23"/>
-      <c r="H15" s="22">
-        <v>42235</v>
-      </c>
+        <v>42258</v>
+      </c>
+      <c r="G15" s="87"/>
+      <c r="H15" s="22"/>
       <c r="I15" s="36"/>
     </row>
-    <row r="16" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="32"/>
-      <c r="B16" s="33">
-        <v>3</v>
-      </c>
-      <c r="C16" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="34" t="s">
-        <v>138</v>
-      </c>
-      <c r="E16" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="35">
-        <v>42178</v>
-      </c>
-      <c r="G16" s="23"/>
-      <c r="H16" s="22">
-        <v>42222</v>
-      </c>
-      <c r="I16" s="36"/>
-    </row>
-    <row r="17" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A17" s="71" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="66">
+    <row r="16" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="27"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="29"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="31"/>
+    </row>
+    <row r="17" spans="1:9" s="19" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A17" s="47"/>
+      <c r="B17" s="33">
+        <v>1</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>160</v>
+      </c>
+      <c r="E17" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="35">
+        <v>42177</v>
+      </c>
+      <c r="G17" s="45"/>
+      <c r="H17" s="37">
+        <v>42255</v>
+      </c>
+      <c r="I17" s="35"/>
+    </row>
+    <row r="18" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A18" s="47"/>
+      <c r="B18" s="33">
         <v>4</v>
       </c>
-      <c r="C17" s="67" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="67" t="s">
-        <v>146</v>
-      </c>
-      <c r="E17" s="66" t="s">
-        <v>40</v>
-      </c>
-      <c r="F17" s="68">
-        <v>42182</v>
-      </c>
-      <c r="G17" s="69"/>
-      <c r="H17" s="68">
-        <v>42249</v>
-      </c>
-      <c r="I17" s="72">
-        <v>42255</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" s="19" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="71"/>
-      <c r="B18" s="66">
-        <v>6</v>
-      </c>
-      <c r="C18" s="67" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="67" t="s">
-        <v>100</v>
-      </c>
-      <c r="E18" s="66" t="s">
-        <v>31</v>
-      </c>
-      <c r="F18" s="68">
-        <v>42182</v>
-      </c>
-      <c r="G18" s="69"/>
-      <c r="H18" s="68"/>
-      <c r="I18" s="72">
-        <v>42202</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="71" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="66">
-        <v>8</v>
-      </c>
-      <c r="C19" s="67" t="s">
-        <v>133</v>
-      </c>
-      <c r="D19" s="67" t="s">
-        <v>159</v>
-      </c>
-      <c r="E19" s="66" t="s">
+      <c r="C18" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="E18" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="68">
-        <v>42216</v>
-      </c>
-      <c r="G19" s="69"/>
-      <c r="H19" s="68">
-        <v>42255</v>
-      </c>
-      <c r="I19" s="72">
+      <c r="F18" s="35">
         <v>42258</v>
       </c>
+      <c r="G18" s="88">
+        <v>42263</v>
+      </c>
+      <c r="H18" s="37">
+        <v>42269</v>
+      </c>
+      <c r="I18" s="35"/>
+    </row>
+    <row r="19" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="44"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="36"/>
     </row>
     <row r="20" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A20" s="27"/>
       <c r="B20" s="14"/>
       <c r="C20" s="28"/>
       <c r="D20" s="28" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E20" s="29"/>
       <c r="F20" s="30"/>
@@ -3013,338 +3019,459 @@
       <c r="H20" s="30"/>
       <c r="I20" s="31"/>
     </row>
-    <row r="21" spans="1:9" s="19" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A21" s="47" t="s">
-        <v>12</v>
-      </c>
+    <row r="21" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="47"/>
       <c r="B21" s="33">
         <v>1</v>
       </c>
-      <c r="C21" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="34" t="s">
-        <v>165</v>
-      </c>
-      <c r="E21" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="F21" s="35">
-        <v>42177</v>
-      </c>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="35"/>
       <c r="G21" s="45"/>
-      <c r="H21" s="37">
-        <v>42255</v>
-      </c>
+      <c r="H21" s="37"/>
       <c r="I21" s="35"/>
     </row>
-    <row r="22" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A22" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="33">
+    <row r="22" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="27"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="29"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="31"/>
+    </row>
+    <row r="23" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="44"/>
+      <c r="B23" s="33">
+        <v>3</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="34" t="s">
+        <v>159</v>
+      </c>
+      <c r="E23" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="35">
+        <v>42179</v>
+      </c>
+      <c r="G23" s="35"/>
+      <c r="H23" s="37">
+        <v>42258</v>
+      </c>
+      <c r="I23" s="36"/>
+    </row>
+    <row r="24" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="44"/>
+      <c r="B24" s="33">
         <v>4</v>
       </c>
-      <c r="C22" s="34" t="s">
-        <v>162</v>
-      </c>
-      <c r="D22" s="34" t="s">
-        <v>163</v>
-      </c>
-      <c r="E22" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="F22" s="35">
+      <c r="C24" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="34" t="s">
+        <v>159</v>
+      </c>
+      <c r="E24" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="35">
+        <v>42179</v>
+      </c>
+      <c r="G24" s="35"/>
+      <c r="H24" s="37">
         <v>42258</v>
       </c>
-      <c r="G22" s="90">
+      <c r="I24" s="36"/>
+    </row>
+    <row r="25" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A25" s="44"/>
+      <c r="B25" s="33">
+        <v>5</v>
+      </c>
+      <c r="C25" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="34" t="s">
+        <v>161</v>
+      </c>
+      <c r="E25" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="35">
+        <v>42182</v>
+      </c>
+      <c r="G25" s="77">
         <v>42263</v>
       </c>
-      <c r="H22" s="37"/>
-      <c r="I22" s="35"/>
-    </row>
-    <row r="23" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="78" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" s="66">
-        <v>3</v>
-      </c>
-      <c r="C23" s="67" t="s">
-        <v>145</v>
-      </c>
-      <c r="D23" s="67" t="s">
-        <v>148</v>
-      </c>
-      <c r="E23" s="66" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" s="68">
-        <v>42249</v>
-      </c>
-      <c r="G23" s="69"/>
-      <c r="H23" s="70"/>
-      <c r="I23" s="68">
-        <v>42255</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" s="19" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="73" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" s="66">
-        <v>2</v>
-      </c>
-      <c r="C24" s="67" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" s="67" t="s">
-        <v>139</v>
-      </c>
-      <c r="E24" s="66" t="s">
-        <v>40</v>
-      </c>
-      <c r="F24" s="68">
-        <v>42160</v>
-      </c>
-      <c r="G24" s="69"/>
-      <c r="H24" s="70">
-        <v>42226</v>
-      </c>
-      <c r="I24" s="72">
-        <v>42228</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="44"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="35"/>
-      <c r="H25" s="37"/>
+      <c r="H25" s="37">
+        <v>42261</v>
+      </c>
       <c r="I25" s="36"/>
     </row>
-    <row r="26" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="27"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="E26" s="29"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="31"/>
+    <row r="26" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A26" s="44"/>
+      <c r="B26" s="33">
+        <v>6</v>
+      </c>
+      <c r="C26" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="E26" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="F26" s="35">
+        <v>42182</v>
+      </c>
+      <c r="G26" s="77">
+        <v>42223</v>
+      </c>
+      <c r="H26" s="37"/>
+      <c r="I26" s="36"/>
     </row>
     <row r="27" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="47"/>
-      <c r="B27" s="33">
-        <v>1</v>
-      </c>
+      <c r="A27" s="44"/>
+      <c r="B27" s="33"/>
       <c r="C27" s="34"/>
       <c r="D27" s="34"/>
       <c r="E27" s="33"/>
       <c r="F27" s="35"/>
-      <c r="G27" s="45"/>
+      <c r="G27" s="35"/>
       <c r="H27" s="37"/>
-      <c r="I27" s="35"/>
-    </row>
-    <row r="28" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="44"/>
-      <c r="B28" s="33"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="35"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="36"/>
-    </row>
-    <row r="29" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="27"/>
+      <c r="I27" s="36"/>
+    </row>
+    <row r="28" spans="1:9" s="12" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="91" t="s">
+        <v>169</v>
+      </c>
+      <c r="B28" s="92"/>
+      <c r="C28" s="92"/>
+      <c r="D28" s="92"/>
+      <c r="E28" s="92"/>
+      <c r="F28" s="92"/>
+      <c r="G28" s="92"/>
+      <c r="H28" s="92"/>
+      <c r="I28" s="93"/>
+    </row>
+    <row r="29" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="13"/>
       <c r="B29" s="14"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="E29" s="29"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="31"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="16"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="18"/>
     </row>
     <row r="30" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="44"/>
-      <c r="B30" s="33">
+      <c r="B30" s="33"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="35"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="36"/>
+    </row>
+    <row r="31" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="27"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="29"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="31"/>
+    </row>
+    <row r="32" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A32" s="72"/>
+      <c r="B32" s="65">
+        <v>1</v>
+      </c>
+      <c r="C32" s="66" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="66" t="s">
+        <v>162</v>
+      </c>
+      <c r="E32" s="65" t="s">
+        <v>23</v>
+      </c>
+      <c r="F32" s="67">
+        <v>42178</v>
+      </c>
+      <c r="G32" s="68"/>
+      <c r="H32" s="67">
+        <v>42249</v>
+      </c>
+      <c r="I32" s="71">
+        <v>42269</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A33" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="65">
+        <v>4</v>
+      </c>
+      <c r="C33" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="D33" s="66" t="s">
+        <v>145</v>
+      </c>
+      <c r="E33" s="65" t="s">
+        <v>40</v>
+      </c>
+      <c r="F33" s="67">
+        <v>42182</v>
+      </c>
+      <c r="G33" s="68"/>
+      <c r="H33" s="67">
+        <v>42249</v>
+      </c>
+      <c r="I33" s="71">
+        <v>42255</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="19" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="70"/>
+      <c r="B34" s="65">
+        <v>6</v>
+      </c>
+      <c r="C34" s="66" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" s="66" t="s">
+        <v>100</v>
+      </c>
+      <c r="E34" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="F34" s="67">
+        <v>42182</v>
+      </c>
+      <c r="G34" s="68"/>
+      <c r="H34" s="67"/>
+      <c r="I34" s="71">
+        <v>42202</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A35" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" s="65">
+        <v>8</v>
+      </c>
+      <c r="C35" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="D35" s="66" t="s">
+        <v>156</v>
+      </c>
+      <c r="E35" s="65" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" s="67">
+        <v>42216</v>
+      </c>
+      <c r="G35" s="68"/>
+      <c r="H35" s="67">
+        <v>42255</v>
+      </c>
+      <c r="I35" s="71">
+        <v>42258</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A36" s="27"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" s="29"/>
+      <c r="F36" s="30"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="30"/>
+      <c r="I36" s="31"/>
+    </row>
+    <row r="37" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A37" s="76" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="65">
         <v>3</v>
       </c>
-      <c r="C30" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="D30" s="34" t="s">
-        <v>164</v>
-      </c>
-      <c r="E30" s="33" t="s">
+      <c r="C37" s="66" t="s">
+        <v>144</v>
+      </c>
+      <c r="D37" s="66" t="s">
+        <v>147</v>
+      </c>
+      <c r="E37" s="65" t="s">
+        <v>15</v>
+      </c>
+      <c r="F37" s="67">
+        <v>42249</v>
+      </c>
+      <c r="G37" s="68"/>
+      <c r="H37" s="69"/>
+      <c r="I37" s="67">
+        <v>42255</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" s="19" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="72" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="65">
+        <v>2</v>
+      </c>
+      <c r="C38" s="66" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" s="66" t="s">
+        <v>139</v>
+      </c>
+      <c r="E38" s="65" t="s">
+        <v>40</v>
+      </c>
+      <c r="F38" s="67">
+        <v>42160</v>
+      </c>
+      <c r="G38" s="68"/>
+      <c r="H38" s="69">
+        <v>42226</v>
+      </c>
+      <c r="I38" s="71">
+        <v>42228</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A39" s="27"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39" s="29"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="30"/>
+      <c r="H39" s="30"/>
+      <c r="I39" s="31"/>
+    </row>
+    <row r="40" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="44"/>
+      <c r="B40" s="33"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="35"/>
+      <c r="H40" s="37"/>
+      <c r="I40" s="36"/>
+    </row>
+    <row r="41" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A41" s="27"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="E41" s="29"/>
+      <c r="F41" s="30"/>
+      <c r="G41" s="30"/>
+      <c r="H41" s="30"/>
+      <c r="I41" s="31"/>
+    </row>
+    <row r="42" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A42" s="76" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" s="65">
+        <v>1</v>
+      </c>
+      <c r="C42" s="66" t="s">
+        <v>19</v>
+      </c>
+      <c r="D42" s="66" t="s">
+        <v>101</v>
+      </c>
+      <c r="E42" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="F30" s="35">
-        <v>42179</v>
-      </c>
-      <c r="G30" s="35"/>
-      <c r="H30" s="37">
-        <v>42258</v>
-      </c>
-      <c r="I30" s="36"/>
-    </row>
-    <row r="31" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="44"/>
-      <c r="B31" s="33">
-        <v>4</v>
-      </c>
-      <c r="C31" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="D31" s="34" t="s">
-        <v>164</v>
-      </c>
-      <c r="E31" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="F31" s="35">
-        <v>42179</v>
-      </c>
-      <c r="G31" s="35"/>
-      <c r="H31" s="37">
-        <v>42258</v>
-      </c>
-      <c r="I31" s="36"/>
-    </row>
-    <row r="32" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A32" s="44"/>
-      <c r="B32" s="33">
-        <v>5</v>
-      </c>
-      <c r="C32" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D32" s="34" t="s">
-        <v>168</v>
-      </c>
-      <c r="E32" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="F32" s="35">
+      <c r="F42" s="67">
+        <v>42160</v>
+      </c>
+      <c r="G42" s="68"/>
+      <c r="H42" s="69">
         <v>42182</v>
       </c>
-      <c r="G32" s="79">
-        <v>42263</v>
-      </c>
-      <c r="H32" s="37">
-        <v>42261</v>
-      </c>
-      <c r="I32" s="36"/>
-    </row>
-    <row r="33" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A33" s="44"/>
-      <c r="B33" s="33">
-        <v>6</v>
-      </c>
-      <c r="C33" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="D33" s="34" t="s">
-        <v>102</v>
-      </c>
-      <c r="E33" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="F33" s="35">
+      <c r="I42" s="67">
+        <v>42202</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A43" s="82"/>
+      <c r="B43" s="65">
+        <v>2</v>
+      </c>
+      <c r="C43" s="66" t="s">
+        <v>21</v>
+      </c>
+      <c r="D43" s="66" t="s">
+        <v>137</v>
+      </c>
+      <c r="E43" s="65" t="s">
+        <v>40</v>
+      </c>
+      <c r="F43" s="67">
+        <v>42160</v>
+      </c>
+      <c r="G43" s="83">
+        <v>42216</v>
+      </c>
+      <c r="H43" s="69">
         <v>42182</v>
       </c>
-      <c r="G33" s="79">
+      <c r="I43" s="71">
         <v>42223</v>
       </c>
-      <c r="H33" s="37"/>
-      <c r="I33" s="36"/>
-    </row>
-    <row r="34" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A34" s="78" t="s">
-        <v>12</v>
-      </c>
-      <c r="B34" s="66">
-        <v>1</v>
-      </c>
-      <c r="C34" s="67" t="s">
-        <v>19</v>
-      </c>
-      <c r="D34" s="67" t="s">
-        <v>101</v>
-      </c>
-      <c r="E34" s="66" t="s">
-        <v>20</v>
-      </c>
-      <c r="F34" s="68">
-        <v>42160</v>
-      </c>
-      <c r="G34" s="69"/>
-      <c r="H34" s="70">
-        <v>42182</v>
-      </c>
-      <c r="I34" s="68">
-        <v>42202</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A35" s="84"/>
-      <c r="B35" s="66">
-        <v>2</v>
-      </c>
-      <c r="C35" s="67" t="s">
-        <v>21</v>
-      </c>
-      <c r="D35" s="67" t="s">
-        <v>137</v>
-      </c>
-      <c r="E35" s="66" t="s">
-        <v>40</v>
-      </c>
-      <c r="F35" s="68">
-        <v>42160</v>
-      </c>
-      <c r="G35" s="85">
-        <v>42216</v>
-      </c>
-      <c r="H35" s="70">
-        <v>42182</v>
-      </c>
-      <c r="I35" s="72">
-        <v>42223</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="44"/>
-      <c r="B36" s="33"/>
-      <c r="C36" s="34"/>
-      <c r="D36" s="34"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="35"/>
-      <c r="G36" s="35"/>
-      <c r="H36" s="37"/>
-      <c r="I36" s="36"/>
-    </row>
-    <row r="49" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D49" s="43"/>
+    </row>
+    <row r="56" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D56" s="43"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A28:I28"/>
+  </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.18" right="0.2" top="0.25" bottom="0.64" header="0.17" footer="0.19"/>
   <pageSetup scale="88" fitToHeight="0" orientation="landscape" verticalDpi="360" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
-  <rowBreaks count="1" manualBreakCount="1">
-    <brk id="18" max="8" man="1"/>
+  <rowBreaks count="2" manualBreakCount="2">
+    <brk id="15" max="16383" man="1"/>
+    <brk id="27" max="16383" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
@@ -3384,7 +3511,7 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="5"/>
-      <c r="I1" s="55"/>
+      <c r="I1" s="54"/>
     </row>
     <row r="2" spans="1:9" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -3396,37 +3523,37 @@
       <c r="E2" s="8"/>
       <c r="G2" s="10"/>
       <c r="H2" s="11"/>
-      <c r="I2" s="56">
+      <c r="I2" s="55">
         <f ca="1">TODAY()</f>
-        <v>42261</v>
+        <v>42269</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="86" t="s">
+      <c r="A3" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="86" t="s">
+      <c r="B3" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="86" t="s">
+      <c r="C3" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="86" t="s">
+      <c r="D3" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="86" t="s">
+      <c r="E3" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="87" t="s">
+      <c r="F3" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="87" t="s">
+      <c r="G3" s="85" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="88" t="s">
+      <c r="H3" s="86" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="87" t="s">
+      <c r="I3" s="85" t="s">
         <v>9</v>
       </c>
     </row>
@@ -3444,7 +3571,7 @@
       <c r="I4" s="18"/>
     </row>
     <row r="5" spans="1:9" s="19" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="60"/>
+      <c r="A5" s="59"/>
       <c r="B5" s="20">
         <v>1</v>
       </c>
@@ -3470,13 +3597,13 @@
     <row r="7" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="32"/>
       <c r="B7" s="20"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="64"/>
-      <c r="H7" s="65"/>
-      <c r="I7" s="63"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="62"/>
     </row>
     <row r="8" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13"/>
@@ -3492,7 +3619,7 @@
       <c r="I8" s="18"/>
     </row>
     <row r="9" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="60" t="s">
+      <c r="A9" s="59" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="20">
@@ -3563,10 +3690,10 @@
         <v>11</v>
       </c>
       <c r="C13" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="D13" s="34" t="s">
         <v>149</v>
-      </c>
-      <c r="D13" s="34" t="s">
-        <v>150</v>
       </c>
       <c r="E13" s="33" t="s">
         <v>40</v>
@@ -3574,7 +3701,7 @@
       <c r="F13" s="35">
         <v>42257</v>
       </c>
-      <c r="G13" s="89">
+      <c r="G13" s="87">
         <v>42293</v>
       </c>
       <c r="H13" s="22"/>
@@ -3652,7 +3779,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="53"/>
+      <c r="A1" s="52"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3673,37 +3800,37 @@
       <c r="E2" s="8"/>
       <c r="G2" s="10"/>
       <c r="H2" s="11"/>
-      <c r="I2" s="54">
+      <c r="I2" s="53">
         <f ca="1">TODAY()</f>
-        <v>42261</v>
+        <v>42269</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="49" t="s">
+      <c r="E3" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="50" t="s">
+      <c r="F3" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="50" t="s">
+      <c r="G3" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="51" t="s">
+      <c r="H3" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="50" t="s">
+      <c r="I3" s="49" t="s">
         <v>9</v>
       </c>
     </row>
@@ -3721,7 +3848,7 @@
       <c r="I4" s="18"/>
     </row>
     <row r="5" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="52"/>
+      <c r="A5" s="51"/>
       <c r="B5" s="20">
         <v>1</v>
       </c>
@@ -3736,7 +3863,7 @@
       <c r="I5" s="22"/>
     </row>
     <row r="6" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="52"/>
+      <c r="A6" s="51"/>
       <c r="B6" s="20">
         <v>2</v>
       </c>
@@ -3751,7 +3878,7 @@
       <c r="I6" s="22"/>
     </row>
     <row r="7" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="52"/>
+      <c r="A7" s="51"/>
       <c r="B7" s="20">
         <v>3</v>
       </c>
@@ -3766,7 +3893,7 @@
       <c r="I7" s="22"/>
     </row>
     <row r="8" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="52"/>
+      <c r="A8" s="51"/>
       <c r="B8" s="20">
         <v>4</v>
       </c>
@@ -3781,7 +3908,7 @@
       <c r="I8" s="22"/>
     </row>
     <row r="9" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="52"/>
+      <c r="A9" s="51"/>
       <c r="B9" s="20">
         <v>5</v>
       </c>
@@ -3796,7 +3923,7 @@
       <c r="I9" s="22"/>
     </row>
     <row r="10" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="52"/>
+      <c r="A10" s="51"/>
       <c r="B10" s="20">
         <v>6</v>
       </c>
@@ -3811,7 +3938,7 @@
       <c r="I10" s="22"/>
     </row>
     <row r="11" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="52"/>
+      <c r="A11" s="51"/>
       <c r="B11" s="20">
         <v>7</v>
       </c>
@@ -3826,7 +3953,7 @@
       <c r="I11" s="22"/>
     </row>
     <row r="12" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="52"/>
+      <c r="A12" s="51"/>
       <c r="B12" s="20">
         <v>8</v>
       </c>
@@ -3841,7 +3968,7 @@
       <c r="I12" s="22"/>
     </row>
     <row r="13" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="52"/>
+      <c r="A13" s="51"/>
       <c r="B13" s="20">
         <v>9</v>
       </c>
@@ -3856,7 +3983,7 @@
       <c r="I13" s="22"/>
     </row>
     <row r="14" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A14" s="52"/>
+      <c r="A14" s="51"/>
       <c r="B14" s="20">
         <v>10</v>
       </c>
@@ -3871,7 +3998,7 @@
       <c r="I14" s="22"/>
     </row>
     <row r="15" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A15" s="52"/>
+      <c r="A15" s="51"/>
       <c r="B15" s="20">
         <v>11</v>
       </c>
@@ -3886,7 +4013,7 @@
       <c r="I15" s="22"/>
     </row>
     <row r="16" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A16" s="52"/>
+      <c r="A16" s="51"/>
       <c r="B16" s="20">
         <v>12</v>
       </c>
@@ -3901,7 +4028,7 @@
       <c r="I16" s="22"/>
     </row>
     <row r="17" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A17" s="52"/>
+      <c r="A17" s="51"/>
       <c r="B17" s="20">
         <v>13</v>
       </c>
@@ -3916,7 +4043,7 @@
       <c r="I17" s="22"/>
     </row>
     <row r="18" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="52"/>
+      <c r="A18" s="51"/>
       <c r="B18" s="20">
         <v>14</v>
       </c>
@@ -3931,7 +4058,7 @@
       <c r="I18" s="22"/>
     </row>
     <row r="19" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="52"/>
+      <c r="A19" s="51"/>
       <c r="B19" s="20">
         <v>15</v>
       </c>
@@ -3946,7 +4073,7 @@
       <c r="I19" s="22"/>
     </row>
     <row r="20" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A20" s="52"/>
+      <c r="A20" s="51"/>
       <c r="B20" s="20">
         <v>16</v>
       </c>
@@ -3961,7 +4088,7 @@
       <c r="I20" s="22"/>
     </row>
     <row r="21" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A21" s="52"/>
+      <c r="A21" s="51"/>
       <c r="B21" s="20">
         <v>17</v>
       </c>
@@ -3976,7 +4103,7 @@
       <c r="I21" s="22"/>
     </row>
     <row r="22" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="52"/>
+      <c r="A22" s="51"/>
       <c r="B22" s="20">
         <v>18</v>
       </c>
@@ -3991,7 +4118,7 @@
       <c r="I22" s="22"/>
     </row>
     <row r="23" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="52"/>
+      <c r="A23" s="51"/>
       <c r="B23" s="20">
         <v>19</v>
       </c>
@@ -4006,7 +4133,7 @@
       <c r="I23" s="22"/>
     </row>
     <row r="24" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A24" s="52"/>
+      <c r="A24" s="51"/>
       <c r="B24" s="20">
         <v>20</v>
       </c>
@@ -4021,7 +4148,7 @@
       <c r="I24" s="22"/>
     </row>
     <row r="25" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="52"/>
+      <c r="A25" s="51"/>
       <c r="B25" s="20"/>
       <c r="C25" s="20"/>
       <c r="D25" s="21"/>
@@ -4032,7 +4159,7 @@
       <c r="I25" s="22"/>
     </row>
     <row r="26" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="52"/>
+      <c r="A26" s="51"/>
       <c r="B26" s="20"/>
       <c r="C26" s="20"/>
       <c r="D26" s="21"/>
@@ -4043,7 +4170,7 @@
       <c r="I26" s="22"/>
     </row>
     <row r="27" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="52"/>
+      <c r="A27" s="51"/>
       <c r="B27" s="20"/>
       <c r="C27" s="20"/>
       <c r="D27" s="21"/>
@@ -4054,7 +4181,7 @@
       <c r="I27" s="22"/>
     </row>
     <row r="28" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="52"/>
+      <c r="A28" s="51"/>
       <c r="B28" s="20"/>
       <c r="C28" s="20"/>
       <c r="D28" s="21"/>
@@ -4065,7 +4192,7 @@
       <c r="I28" s="22"/>
     </row>
     <row r="29" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="52"/>
+      <c r="A29" s="51"/>
       <c r="B29" s="20"/>
       <c r="C29" s="20"/>
       <c r="D29" s="21"/>
@@ -4076,7 +4203,7 @@
       <c r="I29" s="22"/>
     </row>
     <row r="30" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="52"/>
+      <c r="A30" s="51"/>
       <c r="B30" s="20"/>
       <c r="C30" s="20"/>
       <c r="D30" s="21"/>
@@ -4087,7 +4214,7 @@
       <c r="I30" s="22"/>
     </row>
     <row r="31" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="52"/>
+      <c r="A31" s="51"/>
       <c r="B31" s="20"/>
       <c r="C31" s="20"/>
       <c r="D31" s="21"/>
@@ -4098,7 +4225,7 @@
       <c r="I31" s="22"/>
     </row>
     <row r="32" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="52"/>
+      <c r="A32" s="51"/>
       <c r="B32" s="20"/>
       <c r="C32" s="20"/>
       <c r="D32" s="21"/>
@@ -4109,7 +4236,7 @@
       <c r="I32" s="22"/>
     </row>
     <row r="33" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="52"/>
+      <c r="A33" s="51"/>
       <c r="B33" s="20"/>
       <c r="C33" s="20"/>
       <c r="D33" s="21"/>
@@ -4143,7 +4270,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="53"/>
+      <c r="A1" s="52"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4164,37 +4291,37 @@
       <c r="E2" s="8"/>
       <c r="G2" s="10"/>
       <c r="H2" s="11"/>
-      <c r="I2" s="54">
+      <c r="I2" s="53">
         <f ca="1">TODAY()</f>
-        <v>42261</v>
+        <v>42269</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="49" t="s">
+      <c r="E3" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="50" t="s">
+      <c r="F3" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="50" t="s">
+      <c r="G3" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="51" t="s">
+      <c r="H3" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="50" t="s">
+      <c r="I3" s="49" t="s">
         <v>9</v>
       </c>
     </row>
@@ -4212,7 +4339,7 @@
       <c r="I4" s="18"/>
     </row>
     <row r="5" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="52"/>
+      <c r="A5" s="51"/>
       <c r="B5" s="20">
         <v>1</v>
       </c>
@@ -4227,7 +4354,7 @@
       <c r="I5" s="22"/>
     </row>
     <row r="6" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="52"/>
+      <c r="A6" s="51"/>
       <c r="B6" s="20">
         <v>2</v>
       </c>
@@ -4242,7 +4369,7 @@
       <c r="I6" s="22"/>
     </row>
     <row r="7" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="52"/>
+      <c r="A7" s="51"/>
       <c r="B7" s="20">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Updates to timing and issues
Updated task completion on a few items, closed two issues and updated
others.
</commit_message>
<xml_diff>
--- a/Project Tracking/SecuRemote Project Issues.xlsx
+++ b/Project Tracking/SecuRemote Project Issues.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="170">
   <si>
     <t>Open Issues List</t>
   </si>
@@ -335,9 +335,6 @@
     <t>Ashok sent email to Arek on 6/5/15. 6/27 - The fix is in the code, testing to be complete in 2-3 weeks. 7/17 - tested new code, appears to be working fine.</t>
   </si>
   <si>
-    <t>Needs to be reviewed. Doug to set up meeting with Jay and Craig.</t>
-  </si>
-  <si>
     <t>New fixture being shipped to Probuck. Need George/Navy to confim. 7/17- Conformed, tester delivered 7/16.</t>
   </si>
   <si>
@@ -479,18 +476,12 @@
     <t>Need to install one and test it.</t>
   </si>
   <si>
-    <t>Where to place the tags? Not on lock. Should go on Installation Guide, with a reference note in the Quick Start Guide. Need to mark up both and make changes.</t>
-  </si>
-  <si>
     <t>Who is responsible? Ashok last to update. 6/23 - Team reviewing new document. 7/31 - New version to have less screenshots. 9/11 - Heer sent new version, Doug &amp; Dave to review.</t>
   </si>
   <si>
     <t>Doug       Dave</t>
   </si>
   <si>
-    <t>Currently 32 LH and 11 RH assemblies in house. Need to order more of each and schedule assembly with Gene. 9/11 - Jim to check on status.</t>
-  </si>
-  <si>
     <t>Jim B</t>
   </si>
   <si>
@@ -507,6 +498,86 @@
   </si>
   <si>
     <t>On the roadmap, not being developed yet.</t>
+  </si>
+  <si>
+    <t>Threads were wrong for collar, date code not stamped in.  Waiting for resubmission from supplier. 8/6 - still waiting. 9/2 - threads still wrong for our rose nut sample.9/22 - Found matching nut, Fas approved.</t>
+  </si>
+  <si>
+    <t>Verify in displays. Order several samples. 8/13- samples received. When batteries installed, housing is too thick. Found a better solution on Alibaba. Ashley to order samples. Parts from Stride don't work. More coming from Tysonic. 9/10 - No useable sample from either vendors, yet. Need to revert back to previous battery pack and harnesses. 9/11 - Jim to look for rubber band and other solutions. 9/22 - One large band works well for the current housing. Design team is working on a prototype cover.</t>
+  </si>
+  <si>
+    <t>Apple takes at least 1 week, up to 2 weeks. 9/21 - Apps submitted. Android ready.</t>
+  </si>
+  <si>
+    <t>Closed Issues</t>
+  </si>
+  <si>
+    <t>Do we send rev C CPUs or wait for Rev D? Need to get timing from Intertek. They can start 1st week of September. 8/17 - parts ordered. 9/3 - parts sent. 9/11 - Testing to start week of 9/14. 9/22 - Testing complete. Failed Door Slam Test 9/25 - Appears to be mechanical issues. Go over results with Jay.</t>
+  </si>
+  <si>
+    <t>Currently 32 LH and 11 RH assemblies in house. Need to order more of each and schedule assembly with Gene. 9/11 - Jim to check on status. 9/25 - Ashok needs 3 LH and 1 RH eChassis.</t>
+  </si>
+  <si>
+    <t>Ashok, Bhikhu need more lock assemblies, with new CPU and harnesses. 9/18 - Two locks ordered, more available from Intertek week of 9/28. 9/25 - Two samples from Intertek to be sent.</t>
+  </si>
+  <si>
+    <t>Needs to be reviewed. Doug to set up meeting with Jay and Craig. 9/25 - Main page looks fine, other pages need work on verbiage and content.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Where to place the tags? Not on lock. Should go on Installation Guide, with a reference note in the Quick Start Guide. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Need to mark up both and make changes.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mike to take a look. Possibly </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>change main harness</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> length and add sleeving, so harness can be routed behind battery housing. ECO-1139. Verify parts when available. 7/27 - order parts 8/13 - Parts on order (PO 122419), 100pcs. 9/11 - parts received. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Sleeving is a bit stiff and snags on Mortise lock while installing. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Getting feedback from manufacturing. 9/14 - Jay doesn't like it. Tubing is too thick. We will remove tubing and use up this batch, but a better solution needs to be found.</t>
+    </r>
+  </si>
+  <si>
+    <t>Approx. 15 Ethernet bridges were built. Approx. 23 CDMA units were built. JV wants 150 Ethernet units. 10/2 - Doug has received 2 Ethernet Bridges and has tested them.</t>
   </si>
   <si>
     <r>
@@ -527,54 +598,20 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>8/7 - May implement a warning on the label for security. Goes with Issue #2 in Documentation section. 9/8 - Easier to put a warning inside the Installation Instructions.</t>
-    </r>
-  </si>
-  <si>
-    <t>Rules for notifications needs to be defined. 9/2 - Preliminary code in place. 9/14 - I tested it on Android, looks good, just some minor issues.</t>
-  </si>
-  <si>
-    <t>Threads were wrong for collar, date code not stamped in.  Waiting for resubmission from supplier. 8/6 - still waiting. 9/2 - threads still wrong for our rose nut sample.9/22 - Found matching nut, Fas approved.</t>
-  </si>
-  <si>
-    <t>Approx. 15 Ethernet bridges were built. Approx. 23 CDMA units were built. JV wants 150 Ethernet units.</t>
-  </si>
-  <si>
-    <t>Ashok, Bhikhu need more lock assemblies, with new CPU and harnesses. 9/18 - Two locks ordered, more available from Intertek week of 9/28.</t>
-  </si>
-  <si>
-    <t>Verify in displays. Order several samples. 8/13- samples received. When batteries installed, housing is too thick. Found a better solution on Alibaba. Ashley to order samples. Parts from Stride don't work. More coming from Tysonic. 9/10 - No useable sample from either vendors, yet. Need to revert back to previous battery pack and harnesses. 9/11 - Jim to look for rubber band and other solutions. 9/22 - One large band works well for the current housing. Design team is working on a prototype cover.</t>
-  </si>
-  <si>
-    <t>Do we send rev C CPUs or wait for Rev D? Need to get timing from Intertek. They can start 1st week of September. 8/17 - parts ordered. 9/3 - parts sent. 9/11 - Testing to start week of 9/14. 9/22 - Testing complete. Failed Door Slam Test (battery issue?). Locks to be returned this week.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Mike to take a look. Possibly </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>change main harness</t>
+      <t xml:space="preserve">8/7 - May implement a warning on the label for security. Goes with Issue #2 in Documentation section. 9/8 - Easier to </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> length and add sleeving, so harness can be routed behind battery housing. ECO-1139. Verify parts when available. 7/27 - order parts 8/13 - Parts on order (PO 122419), 100pcs. 9/11 - parts received. Sleeving is a bit stiff and snags on Mortise lock while installing. Getting feedback from manufacturing. 9/14 - Jay doesn't like it. Tubing is too thick. We will remove tubing and use up this batch, but a better solution needs to be found.</t>
+      <t>put a warning inside the Installation Instructions.</t>
     </r>
   </si>
   <si>
-    <t>Apple takes at least 1 week, up to 2 weeks. 9/21 - Apps submitted. Android ready.</t>
-  </si>
-  <si>
-    <t>Closed Issues</t>
+    <t>Rules for notifications needs to be defined. 9/2 - Preliminary code in place. 9/14 - I tested it on Android, looks good, just some minor issues. 9/25 - Doug to retest with latest app. 10/2 - Notification appear to be working fine.</t>
   </si>
 </sst>
 </file>
@@ -813,7 +850,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1041,9 +1078,6 @@
     <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1083,6 +1117,15 @@
     <xf numFmtId="164" fontId="12" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1091,6 +1134,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1443,7 +1489,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="55">
         <f ca="1">TODAY()</f>
-        <v>42269</v>
+        <v>42279</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -1576,20 +1622,20 @@
       <c r="B8" s="65">
         <v>4</v>
       </c>
-      <c r="C8" s="78" t="s">
+      <c r="C8" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="78" t="s">
+      <c r="D8" s="77" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="79" t="s">
+      <c r="E8" s="78" t="s">
         <v>49</v>
       </c>
       <c r="F8" s="71">
         <v>42048</v>
       </c>
-      <c r="G8" s="90"/>
-      <c r="H8" s="81"/>
+      <c r="G8" s="89"/>
+      <c r="H8" s="80"/>
       <c r="I8" s="71">
         <v>42269</v>
       </c>
@@ -1601,20 +1647,20 @@
       <c r="B9" s="65">
         <v>5</v>
       </c>
-      <c r="C9" s="78" t="s">
+      <c r="C9" s="77" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="78" t="s">
-        <v>103</v>
-      </c>
-      <c r="E9" s="79" t="s">
+      <c r="D9" s="77" t="s">
+        <v>102</v>
+      </c>
+      <c r="E9" s="78" t="s">
         <v>40</v>
       </c>
       <c r="F9" s="71">
         <v>42062</v>
       </c>
-      <c r="G9" s="80"/>
-      <c r="H9" s="81">
+      <c r="G9" s="79"/>
+      <c r="H9" s="80">
         <v>42195</v>
       </c>
       <c r="I9" s="71">
@@ -2131,7 +2177,7 @@
         <v>83</v>
       </c>
       <c r="D33" s="66" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E33" s="65" t="s">
         <v>40</v>
@@ -2139,7 +2185,7 @@
       <c r="F33" s="67">
         <v>41989</v>
       </c>
-      <c r="G33" s="83">
+      <c r="G33" s="82">
         <v>42216</v>
       </c>
       <c r="H33" s="69"/>
@@ -2158,7 +2204,7 @@
         <v>99</v>
       </c>
       <c r="D34" s="66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E34" s="65" t="s">
         <v>40</v>
@@ -2166,7 +2212,7 @@
       <c r="F34" s="67">
         <v>41991</v>
       </c>
-      <c r="G34" s="83">
+      <c r="G34" s="82">
         <v>42216</v>
       </c>
       <c r="H34" s="69"/>
@@ -2214,7 +2260,7 @@
         <v>86</v>
       </c>
       <c r="D36" s="66" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E36" s="65" t="s">
         <v>40</v>
@@ -2222,7 +2268,7 @@
       <c r="F36" s="67">
         <v>42120</v>
       </c>
-      <c r="G36" s="83">
+      <c r="G36" s="82">
         <v>42216</v>
       </c>
       <c r="H36" s="69">
@@ -2405,7 +2451,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="55">
         <f ca="1">TODAY()</f>
-        <v>42269</v>
+        <v>42279</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -2583,7 +2629,7 @@
   <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2624,7 +2670,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="53">
         <f ca="1">TODAY()</f>
-        <v>42269</v>
+        <v>42279</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -2669,349 +2715,325 @@
       <c r="H4" s="17"/>
       <c r="I4" s="18"/>
     </row>
-    <row r="5" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A5" s="51"/>
       <c r="B5" s="20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>26</v>
+        <v>131</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>152</v>
+        <v>40</v>
       </c>
       <c r="F5" s="22">
-        <v>42177</v>
+        <v>42212</v>
       </c>
       <c r="G5" s="26">
-        <v>42272</v>
+        <v>42286</v>
       </c>
       <c r="H5" s="24">
-        <v>42258</v>
+        <v>42255</v>
       </c>
       <c r="I5" s="22"/>
     </row>
-    <row r="6" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="51"/>
-      <c r="B6" s="20">
-        <v>2</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="E6" s="20" t="s">
+    <row r="6" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="27"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="29"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="31"/>
+    </row>
+    <row r="7" spans="1:9" s="19" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A7" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="33">
+        <v>5</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="34" t="s">
+        <v>166</v>
+      </c>
+      <c r="E7" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="22">
-        <v>42212</v>
-      </c>
-      <c r="G6" s="26">
-        <v>42272</v>
-      </c>
-      <c r="H6" s="24">
-        <v>42255</v>
-      </c>
-      <c r="I6" s="22"/>
-    </row>
-    <row r="7" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="27"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="29"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="31"/>
-    </row>
-    <row r="8" spans="1:9" s="19" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="F7" s="35">
+        <v>42182</v>
+      </c>
+      <c r="G7" s="86">
+        <v>42307</v>
+      </c>
+      <c r="H7" s="22">
+        <v>42261</v>
+      </c>
+      <c r="I7" s="36"/>
+    </row>
+    <row r="8" spans="1:9" s="19" customFormat="1" ht="104.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="46" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="33">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>30</v>
+        <v>133</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>40</v>
+        <v>151</v>
       </c>
       <c r="F8" s="35">
-        <v>42182</v>
-      </c>
-      <c r="G8" s="87">
-        <v>42307</v>
+        <v>42212</v>
+      </c>
+      <c r="G8" s="86">
+        <v>42293</v>
       </c>
       <c r="H8" s="22">
-        <v>42261</v>
+        <v>42257</v>
       </c>
       <c r="I8" s="36"/>
     </row>
-    <row r="9" spans="1:9" s="19" customFormat="1" ht="104.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" s="19" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="46" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="33">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D9" s="34" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E9" s="33" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F9" s="35">
-        <v>42212</v>
-      </c>
-      <c r="G9" s="87">
-        <v>42279</v>
+        <v>42219</v>
+      </c>
+      <c r="G9" s="86">
+        <v>42293</v>
       </c>
       <c r="H9" s="22">
-        <v>42257</v>
+        <v>42258</v>
       </c>
       <c r="I9" s="36"/>
     </row>
-    <row r="10" spans="1:9" s="19" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="46" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="33">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E10" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="F10" s="35">
+        <v>42258</v>
+      </c>
+      <c r="G10" s="86">
+        <v>42279</v>
+      </c>
+      <c r="H10" s="22">
+        <v>42269</v>
+      </c>
+      <c r="I10" s="36"/>
+    </row>
+    <row r="11" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A11" s="32"/>
+      <c r="B11" s="33">
+        <v>2</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="35">
+        <v>42178</v>
+      </c>
+      <c r="G11" s="23"/>
+      <c r="H11" s="22">
+        <v>42235</v>
+      </c>
+      <c r="I11" s="36"/>
+    </row>
+    <row r="12" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A12" s="32"/>
+      <c r="B12" s="33">
+        <v>3</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="35">
+        <v>42178</v>
+      </c>
+      <c r="G12" s="23"/>
+      <c r="H12" s="22">
+        <v>42222</v>
+      </c>
+      <c r="I12" s="36"/>
+    </row>
+    <row r="13" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A13" s="88"/>
+      <c r="B13" s="33">
+        <v>13</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>167</v>
+      </c>
+      <c r="E13" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="35">
+        <v>42258</v>
+      </c>
+      <c r="G13" s="86"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="36"/>
+    </row>
+    <row r="14" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="27"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="29"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="31"/>
+    </row>
+    <row r="15" spans="1:9" s="19" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A15" s="47"/>
+      <c r="B15" s="33">
+        <v>1</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="E15" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="35">
-        <v>42216</v>
-      </c>
-      <c r="G10" s="87">
-        <v>42293</v>
-      </c>
-      <c r="H10" s="22">
+      <c r="F15" s="35">
+        <v>42177</v>
+      </c>
+      <c r="G15" s="87">
+        <v>42286</v>
+      </c>
+      <c r="H15" s="37">
+        <v>42255</v>
+      </c>
+      <c r="I15" s="35"/>
+    </row>
+    <row r="16" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="47"/>
+      <c r="B16" s="33">
+        <v>4</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>159</v>
+      </c>
+      <c r="E16" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="35">
         <v>42258</v>
       </c>
-      <c r="I10" s="36"/>
-    </row>
-    <row r="11" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="46" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="33">
-        <v>10</v>
-      </c>
-      <c r="C11" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="D11" s="34" t="s">
-        <v>153</v>
-      </c>
-      <c r="E11" s="33" t="s">
-        <v>154</v>
-      </c>
-      <c r="F11" s="35">
-        <v>42219</v>
-      </c>
-      <c r="G11" s="87">
-        <v>42307</v>
-      </c>
-      <c r="H11" s="22">
-        <v>42258</v>
-      </c>
-      <c r="I11" s="36"/>
-    </row>
-    <row r="12" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="46" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="33">
-        <v>12</v>
-      </c>
-      <c r="C12" s="34" t="s">
-        <v>157</v>
-      </c>
-      <c r="D12" s="34" t="s">
-        <v>164</v>
-      </c>
-      <c r="E12" s="33" t="s">
-        <v>154</v>
-      </c>
-      <c r="F12" s="35">
-        <v>42258</v>
-      </c>
-      <c r="G12" s="87">
-        <v>42281</v>
-      </c>
-      <c r="H12" s="22">
+      <c r="G16" s="87">
+        <v>42279</v>
+      </c>
+      <c r="H16" s="37">
         <v>42269</v>
       </c>
-      <c r="I12" s="36"/>
-    </row>
-    <row r="13" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="32"/>
-      <c r="B13" s="33">
-        <v>2</v>
-      </c>
-      <c r="C13" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="34" t="s">
-        <v>146</v>
-      </c>
-      <c r="E13" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="35">
-        <v>42178</v>
-      </c>
-      <c r="G13" s="23"/>
-      <c r="H13" s="22">
-        <v>42235</v>
-      </c>
-      <c r="I13" s="36"/>
-    </row>
-    <row r="14" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A14" s="32"/>
-      <c r="B14" s="33">
-        <v>3</v>
-      </c>
-      <c r="C14" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="34" t="s">
-        <v>138</v>
-      </c>
-      <c r="E14" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" s="35">
-        <v>42178</v>
-      </c>
-      <c r="G14" s="23"/>
-      <c r="H14" s="22">
-        <v>42222</v>
-      </c>
-      <c r="I14" s="36"/>
-    </row>
-    <row r="15" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="89"/>
-      <c r="B15" s="33">
-        <v>13</v>
-      </c>
-      <c r="C15" s="34" t="s">
-        <v>155</v>
-      </c>
-      <c r="D15" s="34" t="s">
-        <v>163</v>
-      </c>
-      <c r="E15" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="35">
-        <v>42258</v>
-      </c>
-      <c r="G15" s="87"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="36"/>
-    </row>
-    <row r="16" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="27"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="31"/>
-    </row>
-    <row r="17" spans="1:9" s="19" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="47"/>
-      <c r="B17" s="33">
+      <c r="I16" s="35"/>
+    </row>
+    <row r="17" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="44"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="36"/>
+    </row>
+    <row r="18" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="27"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="29"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="31"/>
+    </row>
+    <row r="19" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="47"/>
+      <c r="B19" s="33">
         <v>1</v>
       </c>
-      <c r="C17" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="34" t="s">
-        <v>160</v>
-      </c>
-      <c r="E17" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="F17" s="35">
-        <v>42177</v>
-      </c>
-      <c r="G17" s="45"/>
-      <c r="H17" s="37">
-        <v>42255</v>
-      </c>
-      <c r="I17" s="35"/>
-    </row>
-    <row r="18" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="47"/>
-      <c r="B18" s="33">
-        <v>4</v>
-      </c>
-      <c r="C18" s="34" t="s">
-        <v>158</v>
-      </c>
-      <c r="D18" s="34" t="s">
-        <v>168</v>
-      </c>
-      <c r="E18" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" s="35">
-        <v>42258</v>
-      </c>
-      <c r="G18" s="88">
-        <v>42263</v>
-      </c>
-      <c r="H18" s="37">
-        <v>42269</v>
-      </c>
-      <c r="I18" s="35"/>
-    </row>
-    <row r="19" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="44"/>
-      <c r="B19" s="33"/>
       <c r="C19" s="34"/>
       <c r="D19" s="34"/>
       <c r="E19" s="33"/>
       <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
+      <c r="G19" s="45"/>
       <c r="H19" s="37"/>
-      <c r="I19" s="36"/>
+      <c r="I19" s="35"/>
     </row>
     <row r="20" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A20" s="27"/>
       <c r="B20" s="14"/>
       <c r="C20" s="28"/>
       <c r="D20" s="28" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E20" s="29"/>
       <c r="F20" s="30"/>
@@ -3019,42 +3041,64 @@
       <c r="H20" s="30"/>
       <c r="I20" s="31"/>
     </row>
-    <row r="21" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="47"/>
+    <row r="21" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A21" s="92" t="s">
+        <v>12</v>
+      </c>
       <c r="B21" s="33">
-        <v>1</v>
-      </c>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="45"/>
+        <v>6</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="34" t="s">
+        <v>164</v>
+      </c>
+      <c r="E21" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21" s="35">
+        <v>42182</v>
+      </c>
+      <c r="G21" s="87">
+        <v>42286</v>
+      </c>
       <c r="H21" s="37"/>
-      <c r="I21" s="35"/>
-    </row>
-    <row r="22" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="27"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" s="29"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="31"/>
+      <c r="I21" s="36"/>
+    </row>
+    <row r="22" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="44"/>
+      <c r="B22" s="33">
+        <v>3</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="E22" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="35">
+        <v>42179</v>
+      </c>
+      <c r="G22" s="35"/>
+      <c r="H22" s="37">
+        <v>42258</v>
+      </c>
+      <c r="I22" s="36"/>
     </row>
     <row r="23" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="44"/>
       <c r="B23" s="33">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C23" s="34" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D23" s="34" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E23" s="33" t="s">
         <v>20</v>
@@ -3070,392 +3114,406 @@
     </row>
     <row r="24" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="44"/>
-      <c r="B24" s="33">
+      <c r="B24" s="33"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="36"/>
+    </row>
+    <row r="25" spans="1:9" s="12" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="93" t="s">
+        <v>160</v>
+      </c>
+      <c r="B25" s="94"/>
+      <c r="C25" s="94"/>
+      <c r="D25" s="94"/>
+      <c r="E25" s="94"/>
+      <c r="F25" s="94"/>
+      <c r="G25" s="94"/>
+      <c r="H25" s="94"/>
+      <c r="I25" s="95"/>
+    </row>
+    <row r="26" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="13"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="16"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="18"/>
+    </row>
+    <row r="27" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A27" s="90"/>
+      <c r="B27" s="65">
+        <v>1</v>
+      </c>
+      <c r="C27" s="66" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="66" t="s">
+        <v>149</v>
+      </c>
+      <c r="E27" s="65" t="s">
+        <v>150</v>
+      </c>
+      <c r="F27" s="67">
+        <v>42177</v>
+      </c>
+      <c r="G27" s="91">
+        <v>42272</v>
+      </c>
+      <c r="H27" s="69">
+        <v>42258</v>
+      </c>
+      <c r="I27" s="67">
+        <v>42272</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="44"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="36"/>
+    </row>
+    <row r="29" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="27"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="29"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="31"/>
+    </row>
+    <row r="30" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A30" s="72"/>
+      <c r="B30" s="65">
+        <v>1</v>
+      </c>
+      <c r="C30" s="66" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="66" t="s">
+        <v>157</v>
+      </c>
+      <c r="E30" s="65" t="s">
+        <v>23</v>
+      </c>
+      <c r="F30" s="67">
+        <v>42178</v>
+      </c>
+      <c r="G30" s="68"/>
+      <c r="H30" s="67">
+        <v>42249</v>
+      </c>
+      <c r="I30" s="71">
+        <v>42269</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A31" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="65">
         <v>4</v>
       </c>
-      <c r="C24" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="34" t="s">
-        <v>159</v>
-      </c>
-      <c r="E24" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="F24" s="35">
-        <v>42179</v>
-      </c>
-      <c r="G24" s="35"/>
-      <c r="H24" s="37">
-        <v>42258</v>
-      </c>
-      <c r="I24" s="36"/>
-    </row>
-    <row r="25" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A25" s="44"/>
-      <c r="B25" s="33">
-        <v>5</v>
-      </c>
-      <c r="C25" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="34" t="s">
-        <v>161</v>
-      </c>
-      <c r="E25" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="F25" s="35">
+      <c r="C31" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="66" t="s">
+        <v>144</v>
+      </c>
+      <c r="E31" s="65" t="s">
+        <v>40</v>
+      </c>
+      <c r="F31" s="67">
         <v>42182</v>
       </c>
-      <c r="G25" s="77">
-        <v>42263</v>
-      </c>
-      <c r="H25" s="37">
-        <v>42261</v>
-      </c>
-      <c r="I25" s="36"/>
-    </row>
-    <row r="26" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A26" s="44"/>
-      <c r="B26" s="33">
+      <c r="G31" s="68"/>
+      <c r="H31" s="67">
+        <v>42249</v>
+      </c>
+      <c r="I31" s="71">
+        <v>42255</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="19" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="70"/>
+      <c r="B32" s="65">
         <v>6</v>
       </c>
-      <c r="C26" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="D26" s="34" t="s">
-        <v>102</v>
-      </c>
-      <c r="E26" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="F26" s="35">
+      <c r="C32" s="66" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" s="66" t="s">
+        <v>100</v>
+      </c>
+      <c r="E32" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="F32" s="67">
         <v>42182</v>
       </c>
-      <c r="G26" s="77">
-        <v>42223</v>
-      </c>
-      <c r="H26" s="37"/>
-      <c r="I26" s="36"/>
-    </row>
-    <row r="27" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="44"/>
-      <c r="B27" s="33"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="36"/>
-    </row>
-    <row r="28" spans="1:9" s="12" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="91" t="s">
-        <v>169</v>
-      </c>
-      <c r="B28" s="92"/>
-      <c r="C28" s="92"/>
-      <c r="D28" s="92"/>
-      <c r="E28" s="92"/>
-      <c r="F28" s="92"/>
-      <c r="G28" s="92"/>
-      <c r="H28" s="92"/>
-      <c r="I28" s="93"/>
-    </row>
-    <row r="29" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="13"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" s="16"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="18"/>
-    </row>
-    <row r="30" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="44"/>
-      <c r="B30" s="33"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="35"/>
-      <c r="H30" s="37"/>
-      <c r="I30" s="36"/>
-    </row>
-    <row r="31" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="27"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31" s="29"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="30"/>
-      <c r="H31" s="30"/>
-      <c r="I31" s="31"/>
-    </row>
-    <row r="32" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A32" s="72"/>
-      <c r="B32" s="65">
-        <v>1</v>
-      </c>
-      <c r="C32" s="66" t="s">
-        <v>22</v>
-      </c>
-      <c r="D32" s="66" t="s">
-        <v>162</v>
-      </c>
-      <c r="E32" s="65" t="s">
-        <v>23</v>
-      </c>
-      <c r="F32" s="67">
-        <v>42178</v>
-      </c>
       <c r="G32" s="68"/>
-      <c r="H32" s="67">
-        <v>42249</v>
-      </c>
+      <c r="H32" s="67"/>
       <c r="I32" s="71">
-        <v>42269</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+        <v>42202</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A33" s="70" t="s">
         <v>44</v>
       </c>
       <c r="B33" s="65">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C33" s="66" t="s">
-        <v>29</v>
+        <v>132</v>
       </c>
       <c r="D33" s="66" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E33" s="65" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="F33" s="67">
-        <v>42182</v>
+        <v>42216</v>
       </c>
       <c r="G33" s="68"/>
       <c r="H33" s="67">
+        <v>42255</v>
+      </c>
+      <c r="I33" s="71">
+        <v>42258</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="19" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="72" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="65">
+        <v>9</v>
+      </c>
+      <c r="C34" s="66" t="s">
+        <v>134</v>
+      </c>
+      <c r="D34" s="66" t="s">
+        <v>161</v>
+      </c>
+      <c r="E34" s="65" t="s">
+        <v>40</v>
+      </c>
+      <c r="F34" s="67">
+        <v>42216</v>
+      </c>
+      <c r="G34" s="96">
+        <v>42293</v>
+      </c>
+      <c r="H34" s="67">
+        <v>42258</v>
+      </c>
+      <c r="I34" s="71">
+        <v>42278</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="27"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" s="29"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="30"/>
+      <c r="I35" s="31"/>
+    </row>
+    <row r="36" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A36" s="76" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="65">
+        <v>3</v>
+      </c>
+      <c r="C36" s="66" t="s">
+        <v>143</v>
+      </c>
+      <c r="D36" s="66" t="s">
+        <v>146</v>
+      </c>
+      <c r="E36" s="65" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36" s="67">
         <v>42249</v>
       </c>
-      <c r="I33" s="71">
+      <c r="G36" s="68"/>
+      <c r="H36" s="69"/>
+      <c r="I36" s="67">
         <v>42255</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="19" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="70"/>
-      <c r="B34" s="65">
-        <v>6</v>
-      </c>
-      <c r="C34" s="66" t="s">
-        <v>32</v>
-      </c>
-      <c r="D34" s="66" t="s">
-        <v>100</v>
-      </c>
-      <c r="E34" s="65" t="s">
-        <v>31</v>
-      </c>
-      <c r="F34" s="67">
+    <row r="37" spans="1:9" s="19" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="72" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="65">
+        <v>2</v>
+      </c>
+      <c r="C37" s="66" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" s="66" t="s">
+        <v>138</v>
+      </c>
+      <c r="E37" s="65" t="s">
+        <v>40</v>
+      </c>
+      <c r="F37" s="67">
+        <v>42160</v>
+      </c>
+      <c r="G37" s="68"/>
+      <c r="H37" s="69">
+        <v>42226</v>
+      </c>
+      <c r="I37" s="71">
+        <v>42228</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A38" s="27"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="28"/>
+      <c r="D38" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" s="29"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="30"/>
+      <c r="H38" s="30"/>
+      <c r="I38" s="31"/>
+    </row>
+    <row r="39" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="44"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="33"/>
+      <c r="F39" s="35"/>
+      <c r="G39" s="35"/>
+      <c r="H39" s="37"/>
+      <c r="I39" s="36"/>
+    </row>
+    <row r="40" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A40" s="27"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" s="29"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="30"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="31"/>
+    </row>
+    <row r="41" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A41" s="76" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" s="65">
+        <v>1</v>
+      </c>
+      <c r="C41" s="66" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="66" t="s">
+        <v>101</v>
+      </c>
+      <c r="E41" s="65" t="s">
+        <v>20</v>
+      </c>
+      <c r="F41" s="67">
+        <v>42160</v>
+      </c>
+      <c r="G41" s="68"/>
+      <c r="H41" s="69">
         <v>42182</v>
       </c>
-      <c r="G34" s="68"/>
-      <c r="H34" s="67"/>
-      <c r="I34" s="71">
+      <c r="I41" s="67">
         <v>42202</v>
       </c>
     </row>
-    <row r="35" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A35" s="70" t="s">
-        <v>44</v>
-      </c>
-      <c r="B35" s="65">
-        <v>8</v>
-      </c>
-      <c r="C35" s="66" t="s">
-        <v>133</v>
-      </c>
-      <c r="D35" s="66" t="s">
-        <v>156</v>
-      </c>
-      <c r="E35" s="65" t="s">
-        <v>15</v>
-      </c>
-      <c r="F35" s="67">
-        <v>42216</v>
-      </c>
-      <c r="G35" s="68"/>
-      <c r="H35" s="67">
-        <v>42255</v>
-      </c>
-      <c r="I35" s="71">
-        <v>42258</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="27"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="28"/>
-      <c r="D36" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="E36" s="29"/>
-      <c r="F36" s="30"/>
-      <c r="G36" s="30"/>
-      <c r="H36" s="30"/>
-      <c r="I36" s="31"/>
-    </row>
-    <row r="37" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A37" s="76" t="s">
-        <v>12</v>
-      </c>
-      <c r="B37" s="65">
-        <v>3</v>
-      </c>
-      <c r="C37" s="66" t="s">
-        <v>144</v>
-      </c>
-      <c r="D37" s="66" t="s">
-        <v>147</v>
-      </c>
-      <c r="E37" s="65" t="s">
-        <v>15</v>
-      </c>
-      <c r="F37" s="67">
-        <v>42249</v>
-      </c>
-      <c r="G37" s="68"/>
-      <c r="H37" s="69"/>
-      <c r="I37" s="67">
-        <v>42255</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" s="19" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="72" t="s">
-        <v>12</v>
-      </c>
-      <c r="B38" s="65">
+    <row r="42" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A42" s="81"/>
+      <c r="B42" s="65">
         <v>2</v>
       </c>
-      <c r="C38" s="66" t="s">
-        <v>16</v>
-      </c>
-      <c r="D38" s="66" t="s">
-        <v>139</v>
-      </c>
-      <c r="E38" s="65" t="s">
+      <c r="C42" s="66" t="s">
+        <v>21</v>
+      </c>
+      <c r="D42" s="66" t="s">
+        <v>136</v>
+      </c>
+      <c r="E42" s="65" t="s">
         <v>40</v>
-      </c>
-      <c r="F38" s="67">
-        <v>42160</v>
-      </c>
-      <c r="G38" s="68"/>
-      <c r="H38" s="69">
-        <v>42226</v>
-      </c>
-      <c r="I38" s="71">
-        <v>42228</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A39" s="27"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="E39" s="29"/>
-      <c r="F39" s="30"/>
-      <c r="G39" s="30"/>
-      <c r="H39" s="30"/>
-      <c r="I39" s="31"/>
-    </row>
-    <row r="40" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="44"/>
-      <c r="B40" s="33"/>
-      <c r="C40" s="34"/>
-      <c r="D40" s="34"/>
-      <c r="E40" s="33"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="35"/>
-      <c r="H40" s="37"/>
-      <c r="I40" s="36"/>
-    </row>
-    <row r="41" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="27"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="28"/>
-      <c r="D41" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="E41" s="29"/>
-      <c r="F41" s="30"/>
-      <c r="G41" s="30"/>
-      <c r="H41" s="30"/>
-      <c r="I41" s="31"/>
-    </row>
-    <row r="42" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A42" s="76" t="s">
-        <v>12</v>
-      </c>
-      <c r="B42" s="65">
-        <v>1</v>
-      </c>
-      <c r="C42" s="66" t="s">
-        <v>19</v>
-      </c>
-      <c r="D42" s="66" t="s">
-        <v>101</v>
-      </c>
-      <c r="E42" s="65" t="s">
-        <v>20</v>
       </c>
       <c r="F42" s="67">
         <v>42160</v>
       </c>
-      <c r="G42" s="68"/>
+      <c r="G42" s="82">
+        <v>42216</v>
+      </c>
       <c r="H42" s="69">
         <v>42182</v>
       </c>
-      <c r="I42" s="67">
-        <v>42202</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A43" s="82"/>
+      <c r="I42" s="71">
+        <v>42223</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A43" s="72" t="s">
+        <v>12</v>
+      </c>
       <c r="B43" s="65">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C43" s="66" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="D43" s="66" t="s">
-        <v>137</v>
+        <v>169</v>
       </c>
       <c r="E43" s="65" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F43" s="67">
-        <v>42160</v>
-      </c>
-      <c r="G43" s="83">
-        <v>42216</v>
+        <v>42182</v>
+      </c>
+      <c r="G43" s="96">
+        <v>42279</v>
       </c>
       <c r="H43" s="69">
-        <v>42182</v>
+        <v>42261</v>
       </c>
       <c r="I43" s="71">
-        <v>42223</v>
+        <v>42279</v>
       </c>
     </row>
     <row r="56" spans="4:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -3463,15 +3521,15 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A28:I28"/>
+    <mergeCell ref="A25:I25"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.18" right="0.2" top="0.25" bottom="0.64" header="0.17" footer="0.19"/>
   <pageSetup scale="88" fitToHeight="0" orientation="landscape" verticalDpi="360" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <rowBreaks count="2" manualBreakCount="2">
-    <brk id="15" max="16383" man="1"/>
-    <brk id="27" max="16383" man="1"/>
+    <brk id="13" max="16383" man="1"/>
+    <brk id="24" max="16383" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
@@ -3515,7 +3573,7 @@
     </row>
     <row r="2" spans="1:9" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B2"/>
       <c r="C2" s="7"/>
@@ -3525,35 +3583,35 @@
       <c r="H2" s="11"/>
       <c r="I2" s="55">
         <f ca="1">TODAY()</f>
-        <v>42269</v>
+        <v>42279</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="84" t="s">
+      <c r="C3" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="84" t="s">
+      <c r="D3" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="84" t="s">
+      <c r="E3" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="85" t="s">
+      <c r="F3" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="85" t="s">
+      <c r="G3" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="86" t="s">
+      <c r="H3" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="85" t="s">
+      <c r="I3" s="84" t="s">
         <v>9</v>
       </c>
     </row>
@@ -3626,7 +3684,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="20"/>
@@ -3669,10 +3727,10 @@
         <v>1</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E12" s="33"/>
       <c r="F12" s="35">
@@ -3690,10 +3748,10 @@
         <v>11</v>
       </c>
       <c r="C13" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="D13" s="34" t="s">
         <v>148</v>
-      </c>
-      <c r="D13" s="34" t="s">
-        <v>149</v>
       </c>
       <c r="E13" s="33" t="s">
         <v>40</v>
@@ -3701,7 +3759,7 @@
       <c r="F13" s="35">
         <v>42257</v>
       </c>
-      <c r="G13" s="87">
+      <c r="G13" s="86">
         <v>42293</v>
       </c>
       <c r="H13" s="22"/>
@@ -3792,7 +3850,7 @@
     </row>
     <row r="2" spans="1:9" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2"/>
       <c r="C2" s="7"/>
@@ -3802,7 +3860,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="53">
         <f ca="1">TODAY()</f>
-        <v>42269</v>
+        <v>42279</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -3853,7 +3911,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D5" s="21"/>
       <c r="E5" s="20"/>
@@ -3868,7 +3926,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="20"/>
@@ -3883,7 +3941,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D7" s="21"/>
       <c r="E7" s="20"/>
@@ -3898,7 +3956,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="20"/>
@@ -3913,7 +3971,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D9" s="21"/>
       <c r="E9" s="20"/>
@@ -3928,7 +3986,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="20"/>
@@ -3943,7 +4001,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D11" s="21"/>
       <c r="E11" s="20"/>
@@ -3958,7 +4016,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="20"/>
@@ -3973,7 +4031,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="20"/>
@@ -3988,7 +4046,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="20"/>
@@ -4003,7 +4061,7 @@
         <v>11</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="20"/>
@@ -4018,7 +4076,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="20"/>
@@ -4033,7 +4091,7 @@
         <v>13</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D17" s="21"/>
       <c r="E17" s="20"/>
@@ -4048,7 +4106,7 @@
         <v>14</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D18" s="21"/>
       <c r="E18" s="20"/>
@@ -4063,7 +4121,7 @@
         <v>15</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D19" s="21"/>
       <c r="E19" s="20"/>
@@ -4078,7 +4136,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="20"/>
@@ -4093,7 +4151,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D21" s="21"/>
       <c r="E21" s="20"/>
@@ -4108,7 +4166,7 @@
         <v>18</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="20"/>
@@ -4123,7 +4181,7 @@
         <v>19</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D23" s="21"/>
       <c r="E23" s="20"/>
@@ -4138,7 +4196,7 @@
         <v>20</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D24" s="21"/>
       <c r="E24" s="20"/>
@@ -4283,7 +4341,7 @@
     </row>
     <row r="2" spans="1:9" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B2"/>
       <c r="C2" s="7"/>
@@ -4293,7 +4351,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="53">
         <f ca="1">TODAY()</f>
-        <v>42269</v>
+        <v>42279</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -4344,7 +4402,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D5" s="21"/>
       <c r="E5" s="20"/>
@@ -4359,7 +4417,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="20"/>
@@ -4374,7 +4432,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D7" s="21"/>
       <c r="E7" s="20"/>

</xml_diff>

<commit_message>
Updated Issues lists and added an item to QS Guide
Closed some issues, updated others, added instructions for QR tag and
Serial Number storage in the Quick Start Guide for Keeler.
</commit_message>
<xml_diff>
--- a/Project Tracking/SecuRemote Project Issues.xlsx
+++ b/Project Tracking/SecuRemote Project Issues.xlsx
@@ -4,17 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24105" windowHeight="9870" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24105" windowHeight="9870" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Smart Deadbolt Gen1" sheetId="2" r:id="rId1"/>
     <sheet name="Smart Deadbolt Gen2" sheetId="3" r:id="rId2"/>
     <sheet name="Keeler Lock" sheetId="1" r:id="rId3"/>
     <sheet name="GDOpener" sheetId="6" r:id="rId4"/>
-    <sheet name="UDI" sheetId="4" r:id="rId5"/>
-    <sheet name="PDI" sheetId="5" r:id="rId6"/>
+    <sheet name="Bridge" sheetId="7" r:id="rId5"/>
+    <sheet name="UDI" sheetId="4" r:id="rId6"/>
+    <sheet name="PDI" sheetId="5" r:id="rId7"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Titles" localSheetId="4">Bridge!$1:$3</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="3">GDOpener!$1:$3</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'Keeler Lock'!$1:$3</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Smart Deadbolt Gen1'!$1:$3</definedName>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="173">
   <si>
     <t>Open Issues List</t>
   </si>
@@ -503,9 +505,6 @@
     <t>Threads were wrong for collar, date code not stamped in.  Waiting for resubmission from supplier. 8/6 - still waiting. 9/2 - threads still wrong for our rose nut sample.9/22 - Found matching nut, Fas approved.</t>
   </si>
   <si>
-    <t>Verify in displays. Order several samples. 8/13- samples received. When batteries installed, housing is too thick. Found a better solution on Alibaba. Ashley to order samples. Parts from Stride don't work. More coming from Tysonic. 9/10 - No useable sample from either vendors, yet. Need to revert back to previous battery pack and harnesses. 9/11 - Jim to look for rubber band and other solutions. 9/22 - One large band works well for the current housing. Design team is working on a prototype cover.</t>
-  </si>
-  <si>
     <t>Apple takes at least 1 week, up to 2 weeks. 9/21 - Apps submitted. Android ready.</t>
   </si>
   <si>
@@ -513,9 +512,6 @@
   </si>
   <si>
     <t>Do we send rev C CPUs or wait for Rev D? Need to get timing from Intertek. They can start 1st week of September. 8/17 - parts ordered. 9/3 - parts sent. 9/11 - Testing to start week of 9/14. 9/22 - Testing complete. Failed Door Slam Test 9/25 - Appears to be mechanical issues. Go over results with Jay.</t>
-  </si>
-  <si>
-    <t>Currently 32 LH and 11 RH assemblies in house. Need to order more of each and schedule assembly with Gene. 9/11 - Jim to check on status. 9/25 - Ashok needs 3 LH and 1 RH eChassis.</t>
   </si>
   <si>
     <t>Ashok, Bhikhu need more lock assemblies, with new CPU and harnesses. 9/18 - Two locks ordered, more available from Intertek week of 9/28. 9/25 - Two samples from Intertek to be sent.</t>
@@ -536,6 +532,43 @@
       </rPr>
       <t>Need to mark up both and make changes.</t>
     </r>
+  </si>
+  <si>
+    <t>Approx. 15 Ethernet bridges were built. Approx. 23 CDMA units were built. JV wants 150 Ethernet units. 10/2 - Doug has received 2 Ethernet Bridges and has tested them.</t>
+  </si>
+  <si>
+    <r>
+      <t>Should the software not allow this to happen? Maybe the CPU firmware can lock this out until a factory reset is performed 6/22/15 - This is how it is designed. We need to discuss with Arek if need to change this.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">8/7 - May implement a warning on the label for security. Goes with Issue #2 in Documentation section. 9/8 - Easier to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>put a warning inside the Installation Instructions.</t>
+    </r>
+  </si>
+  <si>
+    <t>Rules for notifications needs to be defined. 9/2 - Preliminary code in place. 9/14 - I tested it on Android, looks good, just some minor issues. 9/25 - Doug to retest with latest app. 10/2 - Notification appear to be working fine.</t>
   </si>
   <si>
     <r>
@@ -573,15 +606,15 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Getting feedback from manufacturing. 9/14 - Jay doesn't like it. Tubing is too thick. We will remove tubing and use up this batch, but a better solution needs to be found.</t>
+      <t>Getting feedback from manufacturing. 9/14 - Jay doesn't like it. Tubing is too thick. We will remove tubing and use up this batch, but a better solution needs to be found. 10/2 - Mike/Eugene looking at other materials.</t>
     </r>
   </si>
   <si>
-    <t>Approx. 15 Ethernet bridges were built. Approx. 23 CDMA units were built. JV wants 150 Ethernet units. 10/2 - Doug has received 2 Ethernet Bridges and has tested them.</t>
+    <t>Mike C</t>
   </si>
   <si>
     <r>
-      <t>Should the software not allow this to happen? Maybe the CPU firmware can lock this out until a factory reset is performed 6/22/15 - This is how it is designed. We need to discuss with Arek if need to change this.</t>
+      <t xml:space="preserve">Verify in displays. Order several samples. 8/13- samples received. When batteries installed, housing is too thick. Found a better solution on Alibaba. Ashley to order samples. Parts from Stride don't work. More coming from Tysonic. 9/10 - No useable sample from either vendors, yet. Need to revert back to previous battery pack and harnesses. 9/11 - Jim to look for rubber band and other solutions. 9/22 - One large band works well for the current housing. Design team is working on a prototype cover. 10/2 - </t>
     </r>
     <r>
       <rPr>
@@ -590,15 +623,12 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> </t>
+      <t>Getting samples of yet another battery pack.</t>
     </r>
+  </si>
+  <si>
     <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">8/7 - May implement a warning on the label for security. Goes with Issue #2 in Documentation section. 9/8 - Easier to </t>
+      <t xml:space="preserve">Currently 32 LH and 11 RH assemblies in house. Need to order more of each and schedule assembly with Gene. 9/11 - Jim to check on status. 9/25 - Ashok needs 3 LH and 1 RH eChassis. 10/2 - </t>
     </r>
     <r>
       <rPr>
@@ -607,11 +637,14 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>put a warning inside the Installation Instructions.</t>
+      <t>Ashok to test them.</t>
     </r>
   </si>
   <si>
-    <t>Rules for notifications needs to be defined. 9/2 - Preliminary code in place. 9/14 - I tested it on Android, looks good, just some minor issues. 9/25 - Doug to retest with latest app. 10/2 - Notification appear to be working fine.</t>
+    <t>Ethernet Bridge</t>
+  </si>
+  <si>
+    <t>Initial operation was a bit flaky, took several tries to get it to work routinely.</t>
   </si>
 </sst>
 </file>
@@ -1126,6 +1159,9 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="16" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1134,9 +1170,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2628,8 +2661,8 @@
   </sheetPr>
   <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2724,7 +2757,7 @@
         <v>131</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E5" s="20" t="s">
         <v>40</v>
@@ -2753,7 +2786,7 @@
       <c r="H6" s="30"/>
       <c r="I6" s="31"/>
     </row>
-    <row r="7" spans="1:9" s="19" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" s="19" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A7" s="46" t="s">
         <v>12</v>
       </c>
@@ -2764,10 +2797,10 @@
         <v>30</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>40</v>
+        <v>168</v>
       </c>
       <c r="F7" s="35">
         <v>42182</v>
@@ -2780,7 +2813,7 @@
       </c>
       <c r="I7" s="36"/>
     </row>
-    <row r="8" spans="1:9" s="19" customFormat="1" ht="104.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" s="19" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="46" t="s">
         <v>12</v>
       </c>
@@ -2791,10 +2824,10 @@
         <v>133</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>151</v>
+        <v>40</v>
       </c>
       <c r="F8" s="35">
         <v>42212</v>
@@ -2807,7 +2840,7 @@
       </c>
       <c r="I8" s="36"/>
     </row>
-    <row r="9" spans="1:9" s="19" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="46" t="s">
         <v>12</v>
       </c>
@@ -2818,10 +2851,10 @@
         <v>135</v>
       </c>
       <c r="D9" s="34" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="E9" s="33" t="s">
-        <v>151</v>
+        <v>15</v>
       </c>
       <c r="F9" s="35">
         <v>42219</v>
@@ -2834,43 +2867,39 @@
       </c>
       <c r="I9" s="36"/>
     </row>
-    <row r="10" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="46" t="s">
-        <v>12</v>
-      </c>
+    <row r="10" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A10" s="32"/>
       <c r="B10" s="33">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>154</v>
+        <v>24</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>151</v>
+        <v>23</v>
       </c>
       <c r="F10" s="35">
-        <v>42258</v>
-      </c>
-      <c r="G10" s="86">
-        <v>42279</v>
-      </c>
+        <v>42178</v>
+      </c>
+      <c r="G10" s="23"/>
       <c r="H10" s="22">
-        <v>42269</v>
+        <v>42235</v>
       </c>
       <c r="I10" s="36"/>
     </row>
-    <row r="11" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" s="32"/>
       <c r="B11" s="33">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D11" s="34" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="E11" s="33" t="s">
         <v>23</v>
@@ -2880,199 +2909,199 @@
       </c>
       <c r="G11" s="23"/>
       <c r="H11" s="22">
-        <v>42235</v>
+        <v>42222</v>
       </c>
       <c r="I11" s="36"/>
     </row>
-    <row r="12" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="32"/>
+    <row r="12" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="88"/>
       <c r="B12" s="33">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>25</v>
+        <v>152</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>137</v>
+        <v>164</v>
       </c>
       <c r="E12" s="33" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F12" s="35">
-        <v>42178</v>
-      </c>
-      <c r="G12" s="23"/>
-      <c r="H12" s="22">
-        <v>42222</v>
-      </c>
+        <v>42258</v>
+      </c>
+      <c r="G12" s="86"/>
+      <c r="H12" s="22"/>
       <c r="I12" s="36"/>
     </row>
-    <row r="13" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="88"/>
-      <c r="B13" s="33">
+    <row r="13" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="27"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="34" t="s">
-        <v>152</v>
-      </c>
-      <c r="D13" s="34" t="s">
-        <v>167</v>
-      </c>
-      <c r="E13" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" s="35">
-        <v>42258</v>
-      </c>
-      <c r="G13" s="86"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="36"/>
-    </row>
-    <row r="14" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="27"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="29"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="31"/>
-    </row>
-    <row r="15" spans="1:9" s="19" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="E13" s="29"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="31"/>
+    </row>
+    <row r="14" spans="1:9" s="19" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="47"/>
+      <c r="B14" s="33">
+        <v>1</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="E14" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="35">
+        <v>42177</v>
+      </c>
+      <c r="G14" s="87">
+        <v>42286</v>
+      </c>
+      <c r="H14" s="37">
+        <v>42255</v>
+      </c>
+      <c r="I14" s="35"/>
+    </row>
+    <row r="15" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="47"/>
       <c r="B15" s="33">
+        <v>4</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="E15" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="35">
+        <v>42258</v>
+      </c>
+      <c r="G15" s="87">
+        <v>42279</v>
+      </c>
+      <c r="H15" s="37">
+        <v>42269</v>
+      </c>
+      <c r="I15" s="35"/>
+    </row>
+    <row r="16" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="44"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="36"/>
+    </row>
+    <row r="17" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="27"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="29"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="31"/>
+    </row>
+    <row r="18" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="47"/>
+      <c r="B18" s="33">
         <v>1</v>
       </c>
-      <c r="C15" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="34" t="s">
-        <v>168</v>
-      </c>
-      <c r="E15" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" s="35">
-        <v>42177</v>
-      </c>
-      <c r="G15" s="87">
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="35"/>
+    </row>
+    <row r="19" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="27"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="29"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="31"/>
+    </row>
+    <row r="20" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A20" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="33">
+        <v>6</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" s="35">
+        <v>42182</v>
+      </c>
+      <c r="G20" s="87">
         <v>42286</v>
       </c>
-      <c r="H15" s="37">
-        <v>42255</v>
-      </c>
-      <c r="I15" s="35"/>
-    </row>
-    <row r="16" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="47"/>
-      <c r="B16" s="33">
-        <v>4</v>
-      </c>
-      <c r="C16" s="34" t="s">
-        <v>155</v>
-      </c>
-      <c r="D16" s="34" t="s">
-        <v>159</v>
-      </c>
-      <c r="E16" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" s="35">
+      <c r="H20" s="37"/>
+      <c r="I20" s="36"/>
+    </row>
+    <row r="21" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="44"/>
+      <c r="B21" s="33">
+        <v>3</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="E21" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="35">
+        <v>42179</v>
+      </c>
+      <c r="G21" s="35"/>
+      <c r="H21" s="37">
         <v>42258</v>
       </c>
-      <c r="G16" s="87">
-        <v>42279</v>
-      </c>
-      <c r="H16" s="37">
-        <v>42269</v>
-      </c>
-      <c r="I16" s="35"/>
-    </row>
-    <row r="17" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="44"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="36"/>
-    </row>
-    <row r="18" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="27"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="29"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="31"/>
-    </row>
-    <row r="19" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="47"/>
-      <c r="B19" s="33">
-        <v>1</v>
-      </c>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="35"/>
-    </row>
-    <row r="20" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="27"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20" s="29"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="30"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="31"/>
-    </row>
-    <row r="21" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A21" s="92" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="33">
-        <v>6</v>
-      </c>
-      <c r="C21" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" s="34" t="s">
-        <v>164</v>
-      </c>
-      <c r="E21" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="F21" s="35">
-        <v>42182</v>
-      </c>
-      <c r="G21" s="87">
-        <v>42286</v>
-      </c>
-      <c r="H21" s="37"/>
       <c r="I21" s="36"/>
     </row>
     <row r="22" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="44"/>
       <c r="B22" s="33">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C22" s="34" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D22" s="34" t="s">
         <v>156</v>
@@ -3091,244 +3120,250 @@
     </row>
     <row r="23" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="44"/>
-      <c r="B23" s="33">
+      <c r="B23" s="33"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="36"/>
+    </row>
+    <row r="24" spans="1:9" s="12" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="94" t="s">
+        <v>159</v>
+      </c>
+      <c r="B24" s="95"/>
+      <c r="C24" s="95"/>
+      <c r="D24" s="95"/>
+      <c r="E24" s="95"/>
+      <c r="F24" s="95"/>
+      <c r="G24" s="95"/>
+      <c r="H24" s="95"/>
+      <c r="I24" s="96"/>
+    </row>
+    <row r="25" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="13"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="16"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="18"/>
+    </row>
+    <row r="26" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A26" s="90"/>
+      <c r="B26" s="65">
+        <v>1</v>
+      </c>
+      <c r="C26" s="66" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="66" t="s">
+        <v>149</v>
+      </c>
+      <c r="E26" s="65" t="s">
+        <v>150</v>
+      </c>
+      <c r="F26" s="67">
+        <v>42177</v>
+      </c>
+      <c r="G26" s="91">
+        <v>42272</v>
+      </c>
+      <c r="H26" s="69">
+        <v>42258</v>
+      </c>
+      <c r="I26" s="67">
+        <v>42272</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="44"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="35"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="36"/>
+    </row>
+    <row r="28" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="27"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="29"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="31"/>
+    </row>
+    <row r="29" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A29" s="72"/>
+      <c r="B29" s="65">
+        <v>1</v>
+      </c>
+      <c r="C29" s="66" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="66" t="s">
+        <v>157</v>
+      </c>
+      <c r="E29" s="65" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" s="67">
+        <v>42178</v>
+      </c>
+      <c r="G29" s="68"/>
+      <c r="H29" s="67">
+        <v>42249</v>
+      </c>
+      <c r="I29" s="71">
+        <v>42269</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A30" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="65">
         <v>4</v>
       </c>
-      <c r="C23" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23" s="34" t="s">
-        <v>156</v>
-      </c>
-      <c r="E23" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="F23" s="35">
-        <v>42179</v>
-      </c>
-      <c r="G23" s="35"/>
-      <c r="H23" s="37">
-        <v>42258</v>
-      </c>
-      <c r="I23" s="36"/>
-    </row>
-    <row r="24" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="44"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="37"/>
-      <c r="I24" s="36"/>
-    </row>
-    <row r="25" spans="1:9" s="12" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="93" t="s">
-        <v>160</v>
-      </c>
-      <c r="B25" s="94"/>
-      <c r="C25" s="94"/>
-      <c r="D25" s="94"/>
-      <c r="E25" s="94"/>
-      <c r="F25" s="94"/>
-      <c r="G25" s="94"/>
-      <c r="H25" s="94"/>
-      <c r="I25" s="95"/>
-    </row>
-    <row r="26" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="13"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" s="16"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="18"/>
-    </row>
-    <row r="27" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A27" s="90"/>
-      <c r="B27" s="65">
-        <v>1</v>
-      </c>
-      <c r="C27" s="66" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" s="66" t="s">
-        <v>149</v>
-      </c>
-      <c r="E27" s="65" t="s">
-        <v>150</v>
-      </c>
-      <c r="F27" s="67">
-        <v>42177</v>
-      </c>
-      <c r="G27" s="91">
-        <v>42272</v>
-      </c>
-      <c r="H27" s="69">
-        <v>42258</v>
-      </c>
-      <c r="I27" s="67">
-        <v>42272</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="44"/>
-      <c r="B28" s="33"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="35"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="36"/>
-    </row>
-    <row r="29" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="27"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29" s="29"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="31"/>
-    </row>
-    <row r="30" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A30" s="72"/>
-      <c r="B30" s="65">
-        <v>1</v>
-      </c>
       <c r="C30" s="66" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D30" s="66" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="E30" s="65" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="F30" s="67">
-        <v>42178</v>
+        <v>42182</v>
       </c>
       <c r="G30" s="68"/>
       <c r="H30" s="67">
         <v>42249</v>
       </c>
       <c r="I30" s="71">
-        <v>42269</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A31" s="70" t="s">
-        <v>44</v>
-      </c>
+        <v>42255</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="19" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="70"/>
       <c r="B31" s="65">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C31" s="66" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D31" s="66" t="s">
-        <v>144</v>
+        <v>100</v>
       </c>
       <c r="E31" s="65" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="F31" s="67">
         <v>42182</v>
       </c>
       <c r="G31" s="68"/>
-      <c r="H31" s="67">
-        <v>42249</v>
-      </c>
+      <c r="H31" s="67"/>
       <c r="I31" s="71">
+        <v>42202</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A32" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="65">
+        <v>8</v>
+      </c>
+      <c r="C32" s="66" t="s">
+        <v>132</v>
+      </c>
+      <c r="D32" s="66" t="s">
+        <v>153</v>
+      </c>
+      <c r="E32" s="65" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" s="67">
+        <v>42216</v>
+      </c>
+      <c r="G32" s="68"/>
+      <c r="H32" s="67">
         <v>42255</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" s="19" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="70"/>
-      <c r="B32" s="65">
-        <v>6</v>
-      </c>
-      <c r="C32" s="66" t="s">
-        <v>32</v>
-      </c>
-      <c r="D32" s="66" t="s">
-        <v>100</v>
-      </c>
-      <c r="E32" s="65" t="s">
-        <v>31</v>
-      </c>
-      <c r="F32" s="67">
-        <v>42182</v>
-      </c>
-      <c r="G32" s="68"/>
-      <c r="H32" s="67"/>
       <c r="I32" s="71">
-        <v>42202</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A33" s="70" t="s">
-        <v>44</v>
+        <v>42258</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" s="19" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="72" t="s">
+        <v>12</v>
       </c>
       <c r="B33" s="65">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C33" s="66" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D33" s="66" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="E33" s="65" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="F33" s="67">
         <v>42216</v>
       </c>
-      <c r="G33" s="68"/>
+      <c r="G33" s="93">
+        <v>42293</v>
+      </c>
       <c r="H33" s="67">
-        <v>42255</v>
+        <v>42258</v>
       </c>
       <c r="I33" s="71">
-        <v>42258</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" s="19" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+        <v>42278</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" s="72" t="s">
         <v>12</v>
       </c>
       <c r="B34" s="65">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C34" s="66" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
       <c r="D34" s="66" t="s">
         <v>161</v>
       </c>
       <c r="E34" s="65" t="s">
-        <v>40</v>
+        <v>151</v>
       </c>
       <c r="F34" s="67">
-        <v>42216</v>
-      </c>
-      <c r="G34" s="96">
-        <v>42293</v>
+        <v>42258</v>
+      </c>
+      <c r="G34" s="93">
+        <v>42279</v>
       </c>
       <c r="H34" s="67">
-        <v>42258</v>
+        <v>42269</v>
       </c>
       <c r="I34" s="71">
-        <v>42278</v>
+        <v>42279</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
@@ -3498,7 +3533,7 @@
         <v>33</v>
       </c>
       <c r="D43" s="66" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E43" s="65" t="s">
         <v>20</v>
@@ -3506,7 +3541,7 @@
       <c r="F43" s="67">
         <v>42182</v>
       </c>
-      <c r="G43" s="96">
+      <c r="G43" s="93">
         <v>42279</v>
       </c>
       <c r="H43" s="69">
@@ -3521,15 +3556,15 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A25:I25"/>
+    <mergeCell ref="A24:I24"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.18" right="0.2" top="0.25" bottom="0.64" header="0.17" footer="0.19"/>
   <pageSetup scale="88" fitToHeight="0" orientation="landscape" verticalDpi="360" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <rowBreaks count="2" manualBreakCount="2">
-    <brk id="13" max="16383" man="1"/>
-    <brk id="24" max="16383" man="1"/>
+    <brk id="12" max="16383" man="1"/>
+    <brk id="23" max="16383" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
@@ -3820,6 +3855,261 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I35"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6" style="38" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.42578125" style="39" customWidth="1"/>
+    <col min="3" max="3" width="42.42578125" style="38" customWidth="1"/>
+    <col min="4" max="4" width="54.140625" style="38" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="40" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" style="41" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" style="41" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="42" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" style="41" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="38"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="54"/>
+    </row>
+    <row r="2" spans="1:9" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="55">
+        <f ca="1">TODAY()</f>
+        <v>42279</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="83" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="83" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="83" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="83" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="83" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="84" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="85" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="84" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="13"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="16"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="18"/>
+    </row>
+    <row r="5" spans="1:9" s="19" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="59"/>
+      <c r="B5" s="20">
+        <v>1</v>
+      </c>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="22"/>
+    </row>
+    <row r="6" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="22"/>
+    </row>
+    <row r="7" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="32"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="62"/>
+    </row>
+    <row r="8" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="13"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="16"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="18"/>
+    </row>
+    <row r="9" spans="1:9" s="19" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="59"/>
+      <c r="B9" s="20">
+        <v>1</v>
+      </c>
+      <c r="C9" s="21"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="22"/>
+    </row>
+    <row r="10" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="21"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="22"/>
+    </row>
+    <row r="11" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="27"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="29"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="31"/>
+    </row>
+    <row r="12" spans="1:9" s="19" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="46"/>
+      <c r="B12" s="33">
+        <v>1</v>
+      </c>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="36"/>
+    </row>
+    <row r="13" spans="1:9" s="19" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="46"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="86"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="36"/>
+    </row>
+    <row r="14" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="27"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14" s="29"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="31"/>
+    </row>
+    <row r="15" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="33">
+        <v>1</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="D15" s="34"/>
+      <c r="E15" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="35">
+        <v>42279</v>
+      </c>
+      <c r="G15" s="35"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="36"/>
+    </row>
+    <row r="35" spans="1:9" s="40" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="38"/>
+      <c r="B35" s="39"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="43"/>
+      <c r="F35" s="41"/>
+      <c r="G35" s="41"/>
+      <c r="H35" s="42"/>
+      <c r="I35" s="41"/>
+    </row>
+  </sheetData>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.18" right="0.2" top="0.25" bottom="0.64" header="0.17" footer="0.19"/>
+  <pageSetup scale="89" fitToHeight="2" orientation="landscape" verticalDpi="360" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4309,7 +4599,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updated Issues list and Keeler QS Guide
Updated Keeler Issues list based on meeting from 10/2/15.  Updated
Keeler Quickstart Guide: Cleaned up language throughout document, added
a paragraph for what to do with Barcode and Serial number.
</commit_message>
<xml_diff>
--- a/Project Tracking/SecuRemote Project Issues.xlsx
+++ b/Project Tracking/SecuRemote Project Issues.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24105" windowHeight="9870" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24105" windowHeight="9870" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Smart Deadbolt Gen1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="176">
   <si>
     <t>Open Issues List</t>
   </si>
@@ -518,20 +518,6 @@
   </si>
   <si>
     <t>Needs to be reviewed. Doug to set up meeting with Jay and Craig. 9/25 - Main page looks fine, other pages need work on verbiage and content.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Where to place the tags? Not on lock. Should go on Installation Guide, with a reference note in the Quick Start Guide. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Need to mark up both and make changes.</t>
-    </r>
   </si>
   <si>
     <t>Approx. 15 Ethernet bridges were built. Approx. 23 CDMA units were built. JV wants 150 Ethernet units. 10/2 - Doug has received 2 Ethernet Bridges and has tested them.</t>
@@ -645,6 +631,18 @@
   </si>
   <si>
     <t>Initial operation was a bit flaky, took several tries to get it to work routinely.</t>
+  </si>
+  <si>
+    <t>FMEA Training</t>
+  </si>
+  <si>
+    <t>Both PFMEA and DFMEA</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>Where to place the tags? Not on lock. Should go on Installation Guide, with a reference note in the Quick Start Guide. Need to mark up both and make changes.</t>
   </si>
 </sst>
 </file>
@@ -769,7 +767,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -815,6 +813,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -883,7 +887,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1162,6 +1166,15 @@
     <xf numFmtId="164" fontId="16" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1170,6 +1183,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1481,7 +1497,7 @@
   <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1522,7 +1538,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="55">
         <f ca="1">TODAY()</f>
-        <v>42279</v>
+        <v>42283</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -2484,7 +2500,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="55">
         <f ca="1">TODAY()</f>
-        <v>42279</v>
+        <v>42283</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -2661,8 +2677,8 @@
   </sheetPr>
   <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2703,7 +2719,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="53">
         <f ca="1">TODAY()</f>
-        <v>42279</v>
+        <v>42283</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -2740,7 +2756,7 @@
       <c r="B4" s="14"/>
       <c r="C4" s="15"/>
       <c r="D4" s="15" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="E4" s="16"/>
       <c r="F4" s="17"/>
@@ -2748,712 +2764,724 @@
       <c r="H4" s="17"/>
       <c r="I4" s="18"/>
     </row>
-    <row r="5" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" s="19" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="51"/>
       <c r="B5" s="20">
+        <v>1</v>
+      </c>
+      <c r="C5" s="100" t="s">
+        <v>172</v>
+      </c>
+      <c r="D5" s="100" t="s">
+        <v>173</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="22">
+        <v>42282</v>
+      </c>
+      <c r="G5" s="26"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="22"/>
+    </row>
+    <row r="6" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="13"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="16"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="18"/>
+    </row>
+    <row r="7" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A7" s="51"/>
+      <c r="B7" s="20">
         <v>2</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C7" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="D5" s="21" t="s">
-        <v>163</v>
-      </c>
-      <c r="E5" s="20" t="s">
+      <c r="D7" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="E7" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="22">
+      <c r="F7" s="22">
         <v>42212</v>
       </c>
-      <c r="G5" s="26">
+      <c r="G7" s="26">
         <v>42286</v>
       </c>
-      <c r="H5" s="24">
+      <c r="H7" s="24">
         <v>42255</v>
       </c>
-      <c r="I5" s="22"/>
-    </row>
-    <row r="6" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="27"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28" t="s">
+      <c r="I7" s="22"/>
+    </row>
+    <row r="8" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="27"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="29"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="31"/>
-    </row>
-    <row r="7" spans="1:9" s="19" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="46" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="33">
-        <v>5</v>
-      </c>
-      <c r="C7" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="34" t="s">
-        <v>167</v>
-      </c>
-      <c r="E7" s="33" t="s">
-        <v>168</v>
-      </c>
-      <c r="F7" s="35">
-        <v>42182</v>
-      </c>
-      <c r="G7" s="86">
-        <v>42307</v>
-      </c>
-      <c r="H7" s="22">
-        <v>42261</v>
-      </c>
-      <c r="I7" s="36"/>
-    </row>
-    <row r="8" spans="1:9" s="19" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="46" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="33">
-        <v>7</v>
-      </c>
-      <c r="C8" s="34" t="s">
-        <v>133</v>
-      </c>
-      <c r="D8" s="34" t="s">
-        <v>169</v>
-      </c>
-      <c r="E8" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="35">
-        <v>42212</v>
-      </c>
-      <c r="G8" s="86">
-        <v>42293</v>
-      </c>
-      <c r="H8" s="22">
-        <v>42257</v>
-      </c>
-      <c r="I8" s="36"/>
-    </row>
-    <row r="9" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="E8" s="29"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="31"/>
+    </row>
+    <row r="9" spans="1:9" s="19" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A9" s="46" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="33">
+        <v>5</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="34" t="s">
+        <v>166</v>
+      </c>
+      <c r="E9" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="F9" s="35">
+        <v>42182</v>
+      </c>
+      <c r="G9" s="86">
+        <v>42307</v>
+      </c>
+      <c r="H9" s="22">
+        <v>42261</v>
+      </c>
+      <c r="I9" s="36"/>
+    </row>
+    <row r="10" spans="1:9" s="19" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="33">
+        <v>7</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="D10" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="35">
+        <v>42212</v>
+      </c>
+      <c r="G10" s="86">
+        <v>42293</v>
+      </c>
+      <c r="H10" s="22">
+        <v>42257</v>
+      </c>
+      <c r="I10" s="36"/>
+    </row>
+    <row r="11" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="33">
         <v>10</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C11" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="D9" s="34" t="s">
-        <v>170</v>
-      </c>
-      <c r="E9" s="33" t="s">
+      <c r="D11" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="E11" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="35">
+      <c r="F11" s="35">
         <v>42219</v>
       </c>
-      <c r="G9" s="86">
+      <c r="G11" s="86">
         <v>42293</v>
       </c>
-      <c r="H9" s="22">
+      <c r="H11" s="22">
         <v>42258</v>
       </c>
-      <c r="I9" s="36"/>
-    </row>
-    <row r="10" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="32"/>
-      <c r="B10" s="33">
+      <c r="I11" s="36"/>
+    </row>
+    <row r="12" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="32"/>
+      <c r="B12" s="33">
         <v>2</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C12" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="D12" s="34" t="s">
         <v>145</v>
       </c>
-      <c r="E10" s="33" t="s">
+      <c r="E12" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="35">
+      <c r="F12" s="35">
         <v>42178</v>
       </c>
-      <c r="G10" s="23"/>
-      <c r="H10" s="22">
+      <c r="G12" s="23"/>
+      <c r="H12" s="22">
         <v>42235</v>
       </c>
-      <c r="I10" s="36"/>
-    </row>
-    <row r="11" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="32"/>
-      <c r="B11" s="33">
+      <c r="I12" s="36"/>
+    </row>
+    <row r="13" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="32"/>
+      <c r="B13" s="33">
         <v>3</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C13" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="34" t="s">
+      <c r="D13" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="E11" s="33" t="s">
+      <c r="E13" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="35">
+      <c r="F13" s="35">
         <v>42178</v>
       </c>
-      <c r="G11" s="23"/>
-      <c r="H11" s="22">
+      <c r="G13" s="23"/>
+      <c r="H13" s="22">
         <v>42222</v>
       </c>
-      <c r="I11" s="36"/>
-    </row>
-    <row r="12" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="88"/>
-      <c r="B12" s="33">
+      <c r="I13" s="36"/>
+    </row>
+    <row r="14" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="88"/>
+      <c r="B14" s="33">
         <v>13</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C14" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="D14" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="E14" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="35">
+        <v>42258</v>
+      </c>
+      <c r="G14" s="86"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="36"/>
+    </row>
+    <row r="15" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="27"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="29"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="31"/>
+    </row>
+    <row r="16" spans="1:9" s="19" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A16" s="47"/>
+      <c r="B16" s="33">
+        <v>1</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="34" t="s">
         <v>164</v>
       </c>
-      <c r="E12" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="35">
-        <v>42258</v>
-      </c>
-      <c r="G12" s="86"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="36"/>
-    </row>
-    <row r="13" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="27"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="29"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="31"/>
-    </row>
-    <row r="14" spans="1:9" s="19" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="47"/>
-      <c r="B14" s="33">
+      <c r="E16" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="35">
+        <v>42177</v>
+      </c>
+      <c r="G16" s="87">
+        <v>42286</v>
+      </c>
+      <c r="H16" s="37">
+        <v>42255</v>
+      </c>
+      <c r="I16" s="35"/>
+    </row>
+    <row r="17" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="44"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="36"/>
+    </row>
+    <row r="18" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="27"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="29"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="31"/>
+    </row>
+    <row r="19" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="47"/>
+      <c r="B19" s="33">
         <v>1</v>
       </c>
-      <c r="C14" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="34" t="s">
-        <v>165</v>
-      </c>
-      <c r="E14" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" s="35">
-        <v>42177</v>
-      </c>
-      <c r="G14" s="87">
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="35"/>
+    </row>
+    <row r="20" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="47"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="35"/>
+    </row>
+    <row r="21" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="27"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="29"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="31"/>
+    </row>
+    <row r="22" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A22" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="33">
+        <v>6</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="E22" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" s="35">
+        <v>42182</v>
+      </c>
+      <c r="G22" s="87">
         <v>42286</v>
       </c>
-      <c r="H14" s="37">
-        <v>42255</v>
-      </c>
-      <c r="I14" s="35"/>
-    </row>
-    <row r="15" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="47"/>
-      <c r="B15" s="33">
-        <v>4</v>
-      </c>
-      <c r="C15" s="34" t="s">
-        <v>155</v>
-      </c>
-      <c r="D15" s="34" t="s">
-        <v>158</v>
-      </c>
-      <c r="E15" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="35">
-        <v>42258</v>
-      </c>
-      <c r="G15" s="87">
-        <v>42279</v>
-      </c>
-      <c r="H15" s="37">
-        <v>42269</v>
-      </c>
-      <c r="I15" s="35"/>
-    </row>
-    <row r="16" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="44"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="36"/>
-    </row>
-    <row r="17" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="27"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="29"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="31"/>
-    </row>
-    <row r="18" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="47"/>
-      <c r="B18" s="33">
-        <v>1</v>
-      </c>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="35"/>
-    </row>
-    <row r="19" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="27"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="29"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="31"/>
-    </row>
-    <row r="20" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="92" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="33">
-        <v>6</v>
-      </c>
-      <c r="C20" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" s="34" t="s">
-        <v>162</v>
-      </c>
-      <c r="E20" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="F20" s="35">
-        <v>42182</v>
-      </c>
-      <c r="G20" s="87">
-        <v>42286</v>
-      </c>
-      <c r="H20" s="37"/>
-      <c r="I20" s="36"/>
-    </row>
-    <row r="21" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="44"/>
-      <c r="B21" s="33">
-        <v>3</v>
-      </c>
-      <c r="C21" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" s="34" t="s">
-        <v>156</v>
-      </c>
-      <c r="E21" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="35">
-        <v>42179</v>
-      </c>
-      <c r="G21" s="35"/>
-      <c r="H21" s="37">
-        <v>42258</v>
-      </c>
-      <c r="I21" s="36"/>
-    </row>
-    <row r="22" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="44"/>
-      <c r="B22" s="33">
-        <v>4</v>
-      </c>
-      <c r="C22" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="34" t="s">
-        <v>156</v>
-      </c>
-      <c r="E22" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="F22" s="35">
-        <v>42179</v>
-      </c>
-      <c r="G22" s="35"/>
-      <c r="H22" s="37">
-        <v>42258</v>
-      </c>
+      <c r="H22" s="37"/>
       <c r="I22" s="36"/>
     </row>
     <row r="23" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="44"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="35"/>
+      <c r="B23" s="33">
+        <v>3</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="E23" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="35">
+        <v>42179</v>
+      </c>
       <c r="G23" s="35"/>
-      <c r="H23" s="37"/>
+      <c r="H23" s="37">
+        <v>42258</v>
+      </c>
       <c r="I23" s="36"/>
     </row>
-    <row r="24" spans="1:9" s="12" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="94" t="s">
+    <row r="24" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="44"/>
+      <c r="B24" s="33">
+        <v>4</v>
+      </c>
+      <c r="C24" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="E24" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="35">
+        <v>42179</v>
+      </c>
+      <c r="G24" s="35"/>
+      <c r="H24" s="37">
+        <v>42258</v>
+      </c>
+      <c r="I24" s="36"/>
+    </row>
+    <row r="25" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="44"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="35"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="36"/>
+    </row>
+    <row r="26" spans="1:9" s="12" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="97" t="s">
         <v>159</v>
       </c>
-      <c r="B24" s="95"/>
-      <c r="C24" s="95"/>
-      <c r="D24" s="95"/>
-      <c r="E24" s="95"/>
-      <c r="F24" s="95"/>
-      <c r="G24" s="95"/>
-      <c r="H24" s="95"/>
-      <c r="I24" s="96"/>
-    </row>
-    <row r="25" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="13"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15" t="s">
+      <c r="B26" s="98"/>
+      <c r="C26" s="98"/>
+      <c r="D26" s="98"/>
+      <c r="E26" s="98"/>
+      <c r="F26" s="98"/>
+      <c r="G26" s="98"/>
+      <c r="H26" s="98"/>
+      <c r="I26" s="99"/>
+    </row>
+    <row r="27" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="13"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="16"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="18"/>
-    </row>
-    <row r="26" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A26" s="90"/>
-      <c r="B26" s="65">
+      <c r="E27" s="16"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="18"/>
+    </row>
+    <row r="28" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A28" s="90"/>
+      <c r="B28" s="65">
         <v>1</v>
       </c>
-      <c r="C26" s="66" t="s">
+      <c r="C28" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="D26" s="66" t="s">
+      <c r="D28" s="66" t="s">
         <v>149</v>
       </c>
-      <c r="E26" s="65" t="s">
+      <c r="E28" s="65" t="s">
         <v>150</v>
       </c>
-      <c r="F26" s="67">
+      <c r="F28" s="67">
         <v>42177</v>
       </c>
-      <c r="G26" s="91">
+      <c r="G28" s="91">
         <v>42272</v>
       </c>
-      <c r="H26" s="69">
+      <c r="H28" s="69">
         <v>42258</v>
       </c>
-      <c r="I26" s="67">
+      <c r="I28" s="67">
         <v>42272</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="44"/>
-      <c r="B27" s="33"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="36"/>
-    </row>
-    <row r="28" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="27"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28" t="s">
+    <row r="29" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="27"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="E28" s="29"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="30"/>
-      <c r="I28" s="31"/>
-    </row>
-    <row r="29" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A29" s="72"/>
-      <c r="B29" s="65">
+      <c r="E29" s="29"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="31"/>
+    </row>
+    <row r="30" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A30" s="72"/>
+      <c r="B30" s="65">
         <v>1</v>
       </c>
-      <c r="C29" s="66" t="s">
+      <c r="C30" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="D29" s="66" t="s">
+      <c r="D30" s="66" t="s">
         <v>157</v>
       </c>
-      <c r="E29" s="65" t="s">
+      <c r="E30" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="F29" s="67">
+      <c r="F30" s="67">
         <v>42178</v>
-      </c>
-      <c r="G29" s="68"/>
-      <c r="H29" s="67">
-        <v>42249</v>
-      </c>
-      <c r="I29" s="71">
-        <v>42269</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A30" s="70" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" s="65">
-        <v>4</v>
-      </c>
-      <c r="C30" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="D30" s="66" t="s">
-        <v>144</v>
-      </c>
-      <c r="E30" s="65" t="s">
-        <v>40</v>
-      </c>
-      <c r="F30" s="67">
-        <v>42182</v>
       </c>
       <c r="G30" s="68"/>
       <c r="H30" s="67">
         <v>42249</v>
       </c>
       <c r="I30" s="71">
-        <v>42255</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" s="19" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="70"/>
+        <v>42269</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A31" s="70" t="s">
+        <v>44</v>
+      </c>
       <c r="B31" s="65">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C31" s="66" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D31" s="66" t="s">
-        <v>100</v>
+        <v>144</v>
       </c>
       <c r="E31" s="65" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="F31" s="67">
         <v>42182</v>
       </c>
       <c r="G31" s="68"/>
-      <c r="H31" s="67"/>
+      <c r="H31" s="67">
+        <v>42249</v>
+      </c>
       <c r="I31" s="71">
+        <v>42255</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="19" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="70"/>
+      <c r="B32" s="65">
+        <v>6</v>
+      </c>
+      <c r="C32" s="66" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" s="66" t="s">
+        <v>100</v>
+      </c>
+      <c r="E32" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="F32" s="67">
+        <v>42182</v>
+      </c>
+      <c r="G32" s="68"/>
+      <c r="H32" s="67"/>
+      <c r="I32" s="71">
         <v>42202</v>
       </c>
     </row>
-    <row r="32" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A32" s="70" t="s">
+    <row r="33" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A33" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="B32" s="65">
+      <c r="B33" s="65">
         <v>8</v>
       </c>
-      <c r="C32" s="66" t="s">
+      <c r="C33" s="66" t="s">
         <v>132</v>
       </c>
-      <c r="D32" s="66" t="s">
+      <c r="D33" s="66" t="s">
         <v>153</v>
       </c>
-      <c r="E32" s="65" t="s">
+      <c r="E33" s="65" t="s">
         <v>15</v>
-      </c>
-      <c r="F32" s="67">
-        <v>42216</v>
-      </c>
-      <c r="G32" s="68"/>
-      <c r="H32" s="67">
-        <v>42255</v>
-      </c>
-      <c r="I32" s="71">
-        <v>42258</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" s="19" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A33" s="72" t="s">
-        <v>12</v>
-      </c>
-      <c r="B33" s="65">
-        <v>9</v>
-      </c>
-      <c r="C33" s="66" t="s">
-        <v>134</v>
-      </c>
-      <c r="D33" s="66" t="s">
-        <v>160</v>
-      </c>
-      <c r="E33" s="65" t="s">
-        <v>40</v>
       </c>
       <c r="F33" s="67">
         <v>42216</v>
       </c>
-      <c r="G33" s="93">
-        <v>42293</v>
-      </c>
+      <c r="G33" s="68"/>
       <c r="H33" s="67">
+        <v>42255</v>
+      </c>
+      <c r="I33" s="71">
         <v>42258</v>
       </c>
-      <c r="I33" s="71">
-        <v>42278</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:9" s="19" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A34" s="72" t="s">
         <v>12</v>
       </c>
       <c r="B34" s="65">
+        <v>9</v>
+      </c>
+      <c r="C34" s="66" t="s">
+        <v>134</v>
+      </c>
+      <c r="D34" s="66" t="s">
+        <v>160</v>
+      </c>
+      <c r="E34" s="65" t="s">
+        <v>40</v>
+      </c>
+      <c r="F34" s="67">
+        <v>42216</v>
+      </c>
+      <c r="G34" s="93">
+        <v>42293</v>
+      </c>
+      <c r="H34" s="67">
+        <v>42258</v>
+      </c>
+      <c r="I34" s="71">
+        <v>42278</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A35" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="66" t="s">
+      <c r="B35" s="65">
+        <v>12</v>
+      </c>
+      <c r="C35" s="66" t="s">
         <v>154</v>
       </c>
-      <c r="D34" s="66" t="s">
+      <c r="D35" s="66" t="s">
         <v>161</v>
       </c>
-      <c r="E34" s="65" t="s">
+      <c r="E35" s="65" t="s">
         <v>151</v>
       </c>
-      <c r="F34" s="67">
+      <c r="F35" s="67">
         <v>42258</v>
       </c>
-      <c r="G34" s="93">
+      <c r="G35" s="93">
         <v>42279</v>
       </c>
-      <c r="H34" s="67">
+      <c r="H35" s="67">
         <v>42269</v>
       </c>
-      <c r="I34" s="71">
+      <c r="I35" s="71">
         <v>42279</v>
       </c>
     </row>
-    <row r="35" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="27"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="28"/>
-      <c r="D35" s="28" t="s">
+    <row r="36" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A36" s="27"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="E35" s="29"/>
-      <c r="F35" s="30"/>
-      <c r="G35" s="30"/>
-      <c r="H35" s="30"/>
-      <c r="I35" s="31"/>
-    </row>
-    <row r="36" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A36" s="76" t="s">
+      <c r="E36" s="29"/>
+      <c r="F36" s="30"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="30"/>
+      <c r="I36" s="31"/>
+    </row>
+    <row r="37" spans="1:9" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A37" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="65">
+      <c r="B37" s="65">
         <v>3</v>
       </c>
-      <c r="C36" s="66" t="s">
+      <c r="C37" s="66" t="s">
         <v>143</v>
       </c>
-      <c r="D36" s="66" t="s">
+      <c r="D37" s="66" t="s">
         <v>146</v>
       </c>
-      <c r="E36" s="65" t="s">
+      <c r="E37" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="F36" s="67">
+      <c r="F37" s="67">
         <v>42249</v>
       </c>
-      <c r="G36" s="68"/>
-      <c r="H36" s="69"/>
-      <c r="I36" s="67">
+      <c r="G37" s="68"/>
+      <c r="H37" s="69"/>
+      <c r="I37" s="67">
         <v>42255</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="19" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="72" t="s">
+    <row r="38" spans="1:9" s="19" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B37" s="65">
+      <c r="B38" s="65">
         <v>2</v>
       </c>
-      <c r="C37" s="66" t="s">
+      <c r="C38" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="D37" s="66" t="s">
+      <c r="D38" s="66" t="s">
         <v>138</v>
       </c>
-      <c r="E37" s="65" t="s">
+      <c r="E38" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="F37" s="67">
+      <c r="F38" s="67">
         <v>42160</v>
       </c>
-      <c r="G37" s="68"/>
-      <c r="H37" s="69">
+      <c r="G38" s="68"/>
+      <c r="H38" s="69">
         <v>42226</v>
       </c>
-      <c r="I37" s="71">
+      <c r="I38" s="71">
         <v>42228</v>
       </c>
     </row>
-    <row r="38" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="27"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="28"/>
-      <c r="D38" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="E38" s="29"/>
-      <c r="F38" s="30"/>
-      <c r="G38" s="30"/>
-      <c r="H38" s="30"/>
-      <c r="I38" s="31"/>
-    </row>
-    <row r="39" spans="1:9" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="44"/>
-      <c r="B39" s="33"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="33"/>
-      <c r="F39" s="35"/>
-      <c r="G39" s="35"/>
-      <c r="H39" s="37"/>
-      <c r="I39" s="36"/>
+    <row r="39" spans="1:9" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A39" s="76"/>
+      <c r="B39" s="65">
+        <v>4</v>
+      </c>
+      <c r="C39" s="66" t="s">
+        <v>155</v>
+      </c>
+      <c r="D39" s="66" t="s">
+        <v>158</v>
+      </c>
+      <c r="E39" s="65" t="s">
+        <v>15</v>
+      </c>
+      <c r="F39" s="67">
+        <v>42258</v>
+      </c>
+      <c r="G39" s="93">
+        <v>42279</v>
+      </c>
+      <c r="H39" s="69">
+        <v>42269</v>
+      </c>
+      <c r="I39" s="67">
+        <v>42282</v>
+      </c>
     </row>
     <row r="40" spans="1:9" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A40" s="27"/>
@@ -3533,7 +3561,7 @@
         <v>33</v>
       </c>
       <c r="D43" s="66" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E43" s="65" t="s">
         <v>20</v>
@@ -3556,15 +3584,15 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A24:I24"/>
+    <mergeCell ref="A26:I26"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.18" right="0.2" top="0.25" bottom="0.64" header="0.17" footer="0.19"/>
   <pageSetup scale="88" fitToHeight="0" orientation="landscape" verticalDpi="360" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <rowBreaks count="2" manualBreakCount="2">
-    <brk id="12" max="16383" man="1"/>
-    <brk id="23" max="16383" man="1"/>
+    <brk id="14" max="16383" man="1"/>
+    <brk id="25" max="16383" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
@@ -3577,7 +3605,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -3618,35 +3646,35 @@
       <c r="H2" s="11"/>
       <c r="I2" s="55">
         <f ca="1">TODAY()</f>
-        <v>42279</v>
+        <v>42283</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="83" t="s">
+      <c r="C3" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="83" t="s">
+      <c r="D3" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="83" t="s">
+      <c r="E3" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="84" t="s">
+      <c r="F3" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="84" t="s">
+      <c r="G3" s="95" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="85" t="s">
+      <c r="H3" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="84" t="s">
+      <c r="I3" s="95" t="s">
         <v>9</v>
       </c>
     </row>
@@ -3860,8 +3888,8 @@
   </sheetPr>
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -3892,7 +3920,7 @@
     </row>
     <row r="2" spans="1:9" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B2"/>
       <c r="C2" s="7"/>
@@ -3902,7 +3930,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="55">
         <f ca="1">TODAY()</f>
-        <v>42279</v>
+        <v>42283</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -4077,7 +4105,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D15" s="34"/>
       <c r="E15" s="33" t="s">
@@ -4150,7 +4178,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="53">
         <f ca="1">TODAY()</f>
-        <v>42279</v>
+        <v>42283</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -4641,7 +4669,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="53">
         <f ca="1">TODAY()</f>
-        <v>42279</v>
+        <v>42283</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">

</xml_diff>